<commit_message>
Version 1.0c (backoffice complet)
</commit_message>
<xml_diff>
--- a/ALM/Planning.xlsx
+++ b/ALM/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="69">
   <si>
     <t>Menu</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Mise en place de la sécurité</t>
+  </si>
+  <si>
+    <t>Livraison/Mise à disposition pour recette</t>
   </si>
 </sst>
 </file>
@@ -314,11 +317,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray0625">
-        <bgColor theme="2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="gray0625">
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
@@ -355,8 +353,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -585,22 +589,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -618,33 +613,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -656,17 +627,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -678,11 +638,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -715,95 +708,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,114 +1088,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BV59"/>
+  <dimension ref="A1:BV60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BO8" sqref="BO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="2" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39.1796875" customWidth="1"/>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
+    <col min="2" max="2" width="37.08984375" customWidth="1"/>
     <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.36328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="59" width="3.36328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="60" max="66" width="3.36328125" style="71" bestFit="1" customWidth="1"/>
+    <col min="5" max="60" width="3.36328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="61" max="66" width="3.36328125" style="51" bestFit="1" customWidth="1"/>
     <col min="67" max="74" width="3.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="57" t="s">
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57" t="s">
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
-      <c r="U1" s="57"/>
-      <c r="V1" s="57"/>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57" t="s">
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="57"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="57"/>
-      <c r="AC1" s="57"/>
-      <c r="AD1" s="57"/>
-      <c r="AE1" s="57"/>
-      <c r="AF1" s="57" t="s">
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="63"/>
+      <c r="AD1" s="63"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="57"/>
-      <c r="AH1" s="57"/>
-      <c r="AI1" s="57"/>
-      <c r="AJ1" s="57"/>
-      <c r="AK1" s="57"/>
-      <c r="AL1" s="57"/>
-      <c r="AM1" s="58" t="s">
+      <c r="AG1" s="63"/>
+      <c r="AH1" s="63"/>
+      <c r="AI1" s="63"/>
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="63"/>
+      <c r="AL1" s="63"/>
+      <c r="AM1" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="59"/>
-      <c r="AO1" s="59"/>
-      <c r="AP1" s="59"/>
-      <c r="AQ1" s="59"/>
-      <c r="AR1" s="59"/>
-      <c r="AS1" s="60"/>
-      <c r="AT1" s="57" t="s">
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="67"/>
+      <c r="AP1" s="67"/>
+      <c r="AQ1" s="67"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="68"/>
+      <c r="AT1" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="AU1" s="57"/>
-      <c r="AV1" s="57"/>
-      <c r="AW1" s="57"/>
-      <c r="AX1" s="57"/>
-      <c r="AY1" s="57"/>
-      <c r="AZ1" s="57"/>
-      <c r="BA1" s="58" t="s">
+      <c r="AU1" s="63"/>
+      <c r="AV1" s="63"/>
+      <c r="AW1" s="63"/>
+      <c r="AX1" s="63"/>
+      <c r="AY1" s="63"/>
+      <c r="AZ1" s="63"/>
+      <c r="BA1" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="BB1" s="59"/>
-      <c r="BC1" s="59"/>
-      <c r="BD1" s="59"/>
-      <c r="BE1" s="59"/>
-      <c r="BF1" s="59"/>
-      <c r="BG1" s="60"/>
-      <c r="BH1" s="57" t="s">
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="68"/>
+      <c r="BH1" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="BI1" s="57"/>
-      <c r="BJ1" s="57"/>
-      <c r="BK1" s="57"/>
-      <c r="BL1" s="57"/>
-      <c r="BM1" s="57"/>
-      <c r="BN1" s="57"/>
-      <c r="BO1" s="55" t="s">
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="67"/>
+      <c r="BN1" s="68"/>
+      <c r="BO1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="BP1" s="55"/>
-      <c r="BQ1" s="55"/>
-      <c r="BR1" s="55"/>
-      <c r="BS1" s="55"/>
-      <c r="BT1" s="55"/>
-      <c r="BU1" s="55"/>
+      <c r="BP1" s="64"/>
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="64"/>
+      <c r="BT1" s="64"/>
+      <c r="BU1" s="64"/>
     </row>
     <row r="2" spans="1:74" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="11">
@@ -1362,129 +1366,129 @@
       <c r="BG2" s="11">
         <v>43450</v>
       </c>
-      <c r="BH2" s="70">
+      <c r="BH2" s="11">
         <v>43451</v>
       </c>
-      <c r="BI2" s="70">
+      <c r="BI2" s="50">
         <v>43452</v>
       </c>
-      <c r="BJ2" s="70">
+      <c r="BJ2" s="50">
         <v>43453</v>
       </c>
-      <c r="BK2" s="70">
+      <c r="BK2" s="50">
         <v>43454</v>
       </c>
-      <c r="BL2" s="54">
+      <c r="BL2" s="41">
         <v>43455</v>
       </c>
-      <c r="BM2" s="54">
+      <c r="BM2" s="41">
         <v>43456</v>
       </c>
-      <c r="BN2" s="54">
+      <c r="BN2" s="41">
         <v>43457</v>
       </c>
-      <c r="BO2" s="54">
+      <c r="BO2" s="41">
         <v>43458</v>
       </c>
-      <c r="BP2" s="54">
+      <c r="BP2" s="41">
         <v>43459</v>
       </c>
-      <c r="BQ2" s="54">
+      <c r="BQ2" s="41">
         <v>43460</v>
       </c>
-      <c r="BR2" s="54">
+      <c r="BR2" s="41">
         <v>43461</v>
       </c>
-      <c r="BS2" s="54">
+      <c r="BS2" s="41">
         <v>43462</v>
       </c>
-      <c r="BT2" s="54">
+      <c r="BT2" s="41">
         <v>43463</v>
       </c>
-      <c r="BU2" s="54">
+      <c r="BU2" s="41">
         <v>43464</v>
       </c>
-      <c r="BV2" s="54">
+      <c r="BV2" s="41">
         <v>43465</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="32" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:74" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="34"/>
-      <c r="Z3" s="34"/>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="34"/>
-      <c r="AD3" s="34"/>
-      <c r="AE3" s="34"/>
-      <c r="AF3" s="34"/>
-      <c r="AG3" s="34"/>
-      <c r="AH3" s="34"/>
-      <c r="AI3" s="34"/>
-      <c r="AJ3" s="34"/>
-      <c r="AK3" s="34"/>
-      <c r="AL3" s="34"/>
-      <c r="AM3" s="34"/>
-      <c r="AN3" s="34"/>
-      <c r="AO3" s="34"/>
-      <c r="AP3" s="34"/>
-      <c r="AQ3" s="38"/>
-      <c r="AR3" s="38"/>
-      <c r="AS3" s="38"/>
-      <c r="AT3" s="38"/>
-      <c r="AU3" s="38"/>
-      <c r="AV3" s="38"/>
-      <c r="AW3" s="38"/>
-      <c r="AX3" s="38"/>
-      <c r="AY3" s="38"/>
-      <c r="AZ3" s="38"/>
-      <c r="BA3" s="38"/>
-      <c r="BB3" s="38"/>
-      <c r="BC3" s="38"/>
-      <c r="BD3" s="38"/>
-      <c r="BE3" s="38"/>
-      <c r="BF3" s="38"/>
-      <c r="BG3" s="38"/>
-      <c r="BH3" s="34"/>
-      <c r="BI3" s="34"/>
-      <c r="BJ3" s="34"/>
-      <c r="BK3" s="34"/>
-      <c r="BL3" s="34"/>
-      <c r="BM3" s="34"/>
-      <c r="BN3" s="34"/>
-      <c r="BO3" s="34"/>
-      <c r="BP3" s="34"/>
-      <c r="BQ3" s="34"/>
-      <c r="BR3" s="34"/>
-      <c r="BS3" s="34"/>
-      <c r="BT3" s="34"/>
-      <c r="BU3" s="34"/>
-      <c r="BV3" s="34"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="70"/>
+      <c r="T3" s="70"/>
+      <c r="U3" s="70"/>
+      <c r="V3" s="70"/>
+      <c r="W3" s="70"/>
+      <c r="X3" s="70"/>
+      <c r="Y3" s="70"/>
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="70"/>
+      <c r="AB3" s="70"/>
+      <c r="AC3" s="70"/>
+      <c r="AD3" s="70"/>
+      <c r="AE3" s="70"/>
+      <c r="AF3" s="70"/>
+      <c r="AG3" s="70"/>
+      <c r="AH3" s="70"/>
+      <c r="AI3" s="70"/>
+      <c r="AJ3" s="70"/>
+      <c r="AK3" s="70"/>
+      <c r="AL3" s="70"/>
+      <c r="AM3" s="70"/>
+      <c r="AN3" s="70"/>
+      <c r="AO3" s="70"/>
+      <c r="AP3" s="70"/>
+      <c r="AQ3" s="70"/>
+      <c r="AR3" s="70"/>
+      <c r="AS3" s="70"/>
+      <c r="AT3" s="70"/>
+      <c r="AU3" s="70"/>
+      <c r="AV3" s="70"/>
+      <c r="AW3" s="70"/>
+      <c r="AX3" s="70"/>
+      <c r="AY3" s="70"/>
+      <c r="AZ3" s="70"/>
+      <c r="BA3" s="70"/>
+      <c r="BB3" s="70"/>
+      <c r="BC3" s="70"/>
+      <c r="BD3" s="70"/>
+      <c r="BE3" s="70"/>
+      <c r="BF3" s="70"/>
+      <c r="BG3" s="70"/>
+      <c r="BH3" s="70"/>
+      <c r="BI3" s="70"/>
+      <c r="BJ3" s="70"/>
+      <c r="BK3" s="70"/>
+      <c r="BL3" s="70"/>
+      <c r="BM3" s="70"/>
+      <c r="BN3" s="70"/>
+      <c r="BO3" s="70"/>
+      <c r="BP3" s="70"/>
+      <c r="BQ3" s="70"/>
+      <c r="BR3" s="70"/>
+      <c r="BS3" s="70"/>
+      <c r="BT3" s="70"/>
+      <c r="BU3" s="70"/>
+      <c r="BV3" s="70"/>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -1550,13 +1554,13 @@
       <c r="BE4" s="14"/>
       <c r="BF4" s="14"/>
       <c r="BG4" s="14"/>
-      <c r="BH4" s="69"/>
-      <c r="BI4" s="69"/>
-      <c r="BJ4" s="69"/>
-      <c r="BK4" s="69"/>
-      <c r="BL4" s="69"/>
-      <c r="BM4" s="69"/>
-      <c r="BN4" s="69"/>
+      <c r="BH4" s="14"/>
+      <c r="BI4" s="49"/>
+      <c r="BJ4" s="49"/>
+      <c r="BK4" s="49"/>
+      <c r="BL4" s="49"/>
+      <c r="BM4" s="49"/>
+      <c r="BN4" s="49"/>
       <c r="BO4" s="1"/>
       <c r="BP4" s="1"/>
       <c r="BQ4" s="1"/>
@@ -1630,13 +1634,13 @@
       <c r="BE5" s="14"/>
       <c r="BF5" s="14"/>
       <c r="BG5" s="14"/>
-      <c r="BH5" s="69"/>
-      <c r="BI5" s="69"/>
-      <c r="BJ5" s="69"/>
-      <c r="BK5" s="69"/>
-      <c r="BL5" s="69"/>
-      <c r="BM5" s="69"/>
-      <c r="BN5" s="69"/>
+      <c r="BH5" s="14"/>
+      <c r="BI5" s="49"/>
+      <c r="BJ5" s="49"/>
+      <c r="BK5" s="49"/>
+      <c r="BL5" s="49"/>
+      <c r="BM5" s="49"/>
+      <c r="BN5" s="49"/>
       <c r="BO5" s="1"/>
       <c r="BP5" s="1"/>
       <c r="BQ5" s="1"/>
@@ -1710,13 +1714,13 @@
       <c r="BE6" s="14"/>
       <c r="BF6" s="14"/>
       <c r="BG6" s="14"/>
-      <c r="BH6" s="69"/>
-      <c r="BI6" s="69"/>
-      <c r="BJ6" s="69"/>
-      <c r="BK6" s="69"/>
-      <c r="BL6" s="69"/>
-      <c r="BM6" s="69"/>
-      <c r="BN6" s="69"/>
+      <c r="BH6" s="14"/>
+      <c r="BI6" s="49"/>
+      <c r="BJ6" s="49"/>
+      <c r="BK6" s="49"/>
+      <c r="BL6" s="49"/>
+      <c r="BM6" s="49"/>
+      <c r="BN6" s="49"/>
       <c r="BO6" s="1"/>
       <c r="BP6" s="1"/>
       <c r="BQ6" s="1"/>
@@ -1790,13 +1794,13 @@
       <c r="BE7" s="13"/>
       <c r="BF7" s="13"/>
       <c r="BG7" s="13"/>
-      <c r="BH7" s="69"/>
-      <c r="BI7" s="69"/>
-      <c r="BJ7" s="69"/>
-      <c r="BK7" s="69"/>
-      <c r="BL7" s="69"/>
-      <c r="BM7" s="69"/>
-      <c r="BN7" s="69"/>
+      <c r="BH7" s="13"/>
+      <c r="BI7" s="49"/>
+      <c r="BJ7" s="49"/>
+      <c r="BK7" s="49"/>
+      <c r="BL7" s="49"/>
+      <c r="BM7" s="49"/>
+      <c r="BN7" s="49"/>
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
       <c r="BQ7" s="1"/>
@@ -1870,13 +1874,13 @@
       <c r="BE8" s="13"/>
       <c r="BF8" s="13"/>
       <c r="BG8" s="13"/>
-      <c r="BH8" s="69"/>
-      <c r="BI8" s="69"/>
-      <c r="BJ8" s="69"/>
-      <c r="BK8" s="69"/>
-      <c r="BL8" s="69"/>
-      <c r="BM8" s="69"/>
-      <c r="BN8" s="69"/>
+      <c r="BH8" s="13"/>
+      <c r="BI8" s="49"/>
+      <c r="BJ8" s="49"/>
+      <c r="BK8" s="49"/>
+      <c r="BL8" s="49"/>
+      <c r="BM8" s="49"/>
+      <c r="BN8" s="49"/>
       <c r="BO8" s="1"/>
       <c r="BP8" s="1"/>
       <c r="BQ8" s="1"/>
@@ -1950,13 +1954,13 @@
       <c r="BE9" s="14"/>
       <c r="BF9" s="14"/>
       <c r="BG9" s="14"/>
-      <c r="BH9" s="69"/>
-      <c r="BI9" s="69"/>
-      <c r="BJ9" s="69"/>
-      <c r="BK9" s="69"/>
-      <c r="BL9" s="69"/>
-      <c r="BM9" s="69"/>
-      <c r="BN9" s="69"/>
+      <c r="BH9" s="14"/>
+      <c r="BI9" s="49"/>
+      <c r="BJ9" s="49"/>
+      <c r="BK9" s="49"/>
+      <c r="BL9" s="49"/>
+      <c r="BM9" s="49"/>
+      <c r="BN9" s="49"/>
       <c r="BO9" s="1"/>
       <c r="BP9" s="1"/>
       <c r="BQ9" s="1"/>
@@ -2030,13 +2034,13 @@
       <c r="BE10" s="14"/>
       <c r="BF10" s="14"/>
       <c r="BG10" s="14"/>
-      <c r="BH10" s="69"/>
-      <c r="BI10" s="69"/>
-      <c r="BJ10" s="69"/>
-      <c r="BK10" s="69"/>
-      <c r="BL10" s="69"/>
-      <c r="BM10" s="69"/>
-      <c r="BN10" s="69"/>
+      <c r="BH10" s="14"/>
+      <c r="BI10" s="49"/>
+      <c r="BJ10" s="49"/>
+      <c r="BK10" s="49"/>
+      <c r="BL10" s="49"/>
+      <c r="BM10" s="49"/>
+      <c r="BN10" s="49"/>
       <c r="BO10" s="1"/>
       <c r="BP10" s="1"/>
       <c r="BQ10" s="1"/>
@@ -2110,13 +2114,13 @@
       <c r="BE11" s="14"/>
       <c r="BF11" s="14"/>
       <c r="BG11" s="14"/>
-      <c r="BH11" s="69"/>
-      <c r="BI11" s="69"/>
-      <c r="BJ11" s="69"/>
-      <c r="BK11" s="69"/>
-      <c r="BL11" s="69"/>
-      <c r="BM11" s="69"/>
-      <c r="BN11" s="69"/>
+      <c r="BH11" s="14"/>
+      <c r="BI11" s="49"/>
+      <c r="BJ11" s="49"/>
+      <c r="BK11" s="49"/>
+      <c r="BL11" s="49"/>
+      <c r="BM11" s="49"/>
+      <c r="BN11" s="49"/>
       <c r="BO11" s="1"/>
       <c r="BP11" s="1"/>
       <c r="BQ11" s="1"/>
@@ -2190,13 +2194,13 @@
       <c r="BE12" s="14"/>
       <c r="BF12" s="14"/>
       <c r="BG12" s="14"/>
-      <c r="BH12" s="69"/>
-      <c r="BI12" s="69"/>
-      <c r="BJ12" s="69"/>
-      <c r="BK12" s="69"/>
-      <c r="BL12" s="69"/>
-      <c r="BM12" s="69"/>
-      <c r="BN12" s="69"/>
+      <c r="BH12" s="14"/>
+      <c r="BI12" s="49"/>
+      <c r="BJ12" s="49"/>
+      <c r="BK12" s="49"/>
+      <c r="BL12" s="49"/>
+      <c r="BM12" s="49"/>
+      <c r="BN12" s="49"/>
       <c r="BO12" s="1"/>
       <c r="BP12" s="1"/>
       <c r="BQ12" s="1"/>
@@ -2270,13 +2274,13 @@
       <c r="BE13" s="14"/>
       <c r="BF13" s="14"/>
       <c r="BG13" s="14"/>
-      <c r="BH13" s="69"/>
-      <c r="BI13" s="69"/>
-      <c r="BJ13" s="69"/>
-      <c r="BK13" s="69"/>
-      <c r="BL13" s="69"/>
-      <c r="BM13" s="69"/>
-      <c r="BN13" s="69"/>
+      <c r="BH13" s="14"/>
+      <c r="BI13" s="49"/>
+      <c r="BJ13" s="49"/>
+      <c r="BK13" s="49"/>
+      <c r="BL13" s="49"/>
+      <c r="BM13" s="49"/>
+      <c r="BN13" s="49"/>
       <c r="BO13" s="1"/>
       <c r="BP13" s="1"/>
       <c r="BQ13" s="1"/>
@@ -2348,13 +2352,13 @@
       <c r="BE14" s="14"/>
       <c r="BF14" s="14"/>
       <c r="BG14" s="14"/>
-      <c r="BH14" s="69"/>
-      <c r="BI14" s="69"/>
-      <c r="BJ14" s="69"/>
-      <c r="BK14" s="69"/>
-      <c r="BL14" s="69"/>
-      <c r="BM14" s="69"/>
-      <c r="BN14" s="69"/>
+      <c r="BH14" s="14"/>
+      <c r="BI14" s="49"/>
+      <c r="BJ14" s="49"/>
+      <c r="BK14" s="49"/>
+      <c r="BL14" s="49"/>
+      <c r="BM14" s="49"/>
+      <c r="BN14" s="49"/>
       <c r="BO14" s="1"/>
       <c r="BP14" s="1"/>
       <c r="BQ14" s="1"/>
@@ -2428,13 +2432,13 @@
       <c r="BE15" s="14"/>
       <c r="BF15" s="14"/>
       <c r="BG15" s="14"/>
-      <c r="BH15" s="69"/>
-      <c r="BI15" s="69"/>
-      <c r="BJ15" s="69"/>
-      <c r="BK15" s="69"/>
-      <c r="BL15" s="69"/>
-      <c r="BM15" s="69"/>
-      <c r="BN15" s="69"/>
+      <c r="BH15" s="14"/>
+      <c r="BI15" s="49"/>
+      <c r="BJ15" s="49"/>
+      <c r="BK15" s="49"/>
+      <c r="BL15" s="49"/>
+      <c r="BM15" s="49"/>
+      <c r="BN15" s="49"/>
       <c r="BO15" s="1"/>
       <c r="BP15" s="1"/>
       <c r="BQ15" s="1"/>
@@ -2508,13 +2512,13 @@
       <c r="BE16" s="14"/>
       <c r="BF16" s="14"/>
       <c r="BG16" s="14"/>
-      <c r="BH16" s="69"/>
-      <c r="BI16" s="69"/>
-      <c r="BJ16" s="69"/>
-      <c r="BK16" s="69"/>
-      <c r="BL16" s="69"/>
-      <c r="BM16" s="69"/>
-      <c r="BN16" s="69"/>
+      <c r="BH16" s="14"/>
+      <c r="BI16" s="49"/>
+      <c r="BJ16" s="49"/>
+      <c r="BK16" s="49"/>
+      <c r="BL16" s="49"/>
+      <c r="BM16" s="49"/>
+      <c r="BN16" s="49"/>
       <c r="BO16" s="1"/>
       <c r="BP16" s="1"/>
       <c r="BQ16" s="1"/>
@@ -2588,13 +2592,13 @@
       <c r="BE17" s="14"/>
       <c r="BF17" s="14"/>
       <c r="BG17" s="14"/>
-      <c r="BH17" s="69"/>
-      <c r="BI17" s="69"/>
-      <c r="BJ17" s="69"/>
-      <c r="BK17" s="69"/>
-      <c r="BL17" s="69"/>
-      <c r="BM17" s="69"/>
-      <c r="BN17" s="69"/>
+      <c r="BH17" s="14"/>
+      <c r="BI17" s="49"/>
+      <c r="BJ17" s="49"/>
+      <c r="BK17" s="49"/>
+      <c r="BL17" s="49"/>
+      <c r="BM17" s="49"/>
+      <c r="BN17" s="49"/>
       <c r="BO17" s="1"/>
       <c r="BP17" s="1"/>
       <c r="BQ17" s="1"/>
@@ -2604,246 +2608,245 @@
       <c r="BU17" s="1"/>
       <c r="BV17" s="1"/>
     </row>
-    <row r="18" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="33" t="s">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A18" s="83"/>
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
+      <c r="AM18" s="14"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="14"/>
+      <c r="AP18" s="14"/>
+      <c r="AQ18" s="14"/>
+      <c r="AR18" s="14"/>
+      <c r="AS18" s="14"/>
+      <c r="AT18" s="14"/>
+      <c r="AU18" s="14"/>
+      <c r="AV18" s="14"/>
+      <c r="AW18" s="14"/>
+      <c r="AX18" s="14"/>
+      <c r="AY18" s="14"/>
+      <c r="AZ18" s="14"/>
+      <c r="BA18" s="14"/>
+      <c r="BB18" s="14"/>
+      <c r="BC18" s="14"/>
+      <c r="BD18" s="14"/>
+      <c r="BE18" s="14"/>
+      <c r="BF18" s="14"/>
+      <c r="BG18" s="14"/>
+      <c r="BH18" s="14"/>
+      <c r="BI18" s="85"/>
+      <c r="BJ18" s="49"/>
+      <c r="BK18" s="49"/>
+      <c r="BL18" s="49"/>
+      <c r="BM18" s="49"/>
+      <c r="BN18" s="49"/>
+      <c r="BO18" s="1"/>
+      <c r="BP18" s="1"/>
+      <c r="BQ18" s="1"/>
+      <c r="BR18" s="1"/>
+      <c r="BS18" s="1"/>
+      <c r="BT18" s="1"/>
+      <c r="BU18" s="1"/>
+      <c r="BV18" s="1"/>
+    </row>
+    <row r="19" spans="1:74" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="34"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="34"/>
-      <c r="Z18" s="34"/>
-      <c r="AA18" s="34"/>
-      <c r="AB18" s="34"/>
-      <c r="AC18" s="34"/>
-      <c r="AD18" s="34"/>
-      <c r="AE18" s="34"/>
-      <c r="AF18" s="34"/>
-      <c r="AG18" s="34"/>
-      <c r="AH18" s="34"/>
-      <c r="AI18" s="34"/>
-      <c r="AJ18" s="34"/>
-      <c r="AK18" s="34"/>
-      <c r="AL18" s="34"/>
-      <c r="AM18" s="34"/>
-      <c r="AN18" s="34"/>
-      <c r="AO18" s="34"/>
-      <c r="AP18" s="34"/>
-      <c r="AQ18" s="38"/>
-      <c r="AR18" s="38"/>
-      <c r="AS18" s="38"/>
-      <c r="AT18" s="38"/>
-      <c r="AU18" s="38"/>
-      <c r="AV18" s="38"/>
-      <c r="AW18" s="38"/>
-      <c r="AX18" s="38"/>
-      <c r="AY18" s="38"/>
-      <c r="AZ18" s="38"/>
-      <c r="BA18" s="51"/>
-      <c r="BB18" s="51"/>
-      <c r="BC18" s="51"/>
-      <c r="BD18" s="51"/>
-      <c r="BE18" s="51"/>
-      <c r="BF18" s="38"/>
-      <c r="BG18" s="38"/>
-      <c r="BH18" s="34"/>
-      <c r="BI18" s="34"/>
-      <c r="BJ18" s="34"/>
-      <c r="BK18" s="34"/>
-      <c r="BL18" s="34"/>
-      <c r="BM18" s="34"/>
-      <c r="BN18" s="34"/>
-      <c r="BO18" s="34"/>
-      <c r="BP18" s="34"/>
-      <c r="BQ18" s="34"/>
-      <c r="BR18" s="34"/>
-      <c r="BS18" s="34"/>
-      <c r="BT18" s="34"/>
-      <c r="BU18" s="34"/>
-      <c r="BV18" s="35"/>
-    </row>
-    <row r="19" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="70"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70"/>
+      <c r="S19" s="70"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="70"/>
+      <c r="V19" s="70"/>
+      <c r="W19" s="70"/>
+      <c r="X19" s="70"/>
+      <c r="Y19" s="70"/>
+      <c r="Z19" s="70"/>
+      <c r="AA19" s="70"/>
+      <c r="AB19" s="70"/>
+      <c r="AC19" s="70"/>
+      <c r="AD19" s="70"/>
+      <c r="AE19" s="70"/>
+      <c r="AF19" s="70"/>
+      <c r="AG19" s="70"/>
+      <c r="AH19" s="70"/>
+      <c r="AI19" s="70"/>
+      <c r="AJ19" s="70"/>
+      <c r="AK19" s="70"/>
+      <c r="AL19" s="70"/>
+      <c r="AM19" s="70"/>
+      <c r="AN19" s="70"/>
+      <c r="AO19" s="70"/>
+      <c r="AP19" s="70"/>
+      <c r="AQ19" s="70"/>
+      <c r="AR19" s="70"/>
+      <c r="AS19" s="70"/>
+      <c r="AT19" s="70"/>
+      <c r="AU19" s="70"/>
+      <c r="AV19" s="70"/>
+      <c r="AW19" s="70"/>
+      <c r="AX19" s="70"/>
+      <c r="AY19" s="70"/>
+      <c r="AZ19" s="70"/>
+      <c r="BA19" s="70"/>
+      <c r="BB19" s="70"/>
+      <c r="BC19" s="70"/>
+      <c r="BD19" s="70"/>
+      <c r="BE19" s="70"/>
+      <c r="BF19" s="70"/>
+      <c r="BG19" s="70"/>
+      <c r="BH19" s="70"/>
+      <c r="BI19" s="70"/>
+      <c r="BJ19" s="70"/>
+      <c r="BK19" s="70"/>
+      <c r="BL19" s="70"/>
+      <c r="BM19" s="70"/>
+      <c r="BN19" s="70"/>
+      <c r="BO19" s="70"/>
+      <c r="BP19" s="70"/>
+      <c r="BQ19" s="70"/>
+      <c r="BR19" s="70"/>
+      <c r="BS19" s="70"/>
+      <c r="BT19" s="70"/>
+      <c r="BU19" s="70"/>
+      <c r="BV19" s="70"/>
+    </row>
+    <row r="20" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C20" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="16"/>
-      <c r="X19" s="16"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="14"/>
-      <c r="AE19" s="14"/>
-      <c r="AF19" s="14"/>
-      <c r="AG19" s="14"/>
-      <c r="AH19" s="14"/>
-      <c r="AI19" s="14"/>
-      <c r="AJ19" s="14"/>
-      <c r="AK19" s="14"/>
-      <c r="AL19" s="14"/>
-      <c r="AM19" s="14"/>
-      <c r="AN19" s="14"/>
-      <c r="AO19" s="14"/>
-      <c r="AP19" s="14"/>
-      <c r="AQ19" s="14"/>
-      <c r="AR19" s="14"/>
-      <c r="AS19" s="14"/>
-      <c r="AT19" s="14"/>
-      <c r="AU19" s="14"/>
-      <c r="AV19" s="14"/>
-      <c r="AW19" s="14"/>
-      <c r="AX19" s="14"/>
-      <c r="AY19" s="14"/>
-      <c r="AZ19" s="14"/>
-      <c r="BA19" s="52"/>
-      <c r="BB19" s="14"/>
-      <c r="BC19" s="14"/>
-      <c r="BD19" s="14"/>
-      <c r="BE19" s="14"/>
-      <c r="BF19" s="52"/>
-      <c r="BG19" s="61"/>
-      <c r="BI19" s="69"/>
-      <c r="BJ19" s="69"/>
-      <c r="BK19" s="69"/>
-      <c r="BM19" s="8"/>
-      <c r="BN19" s="69"/>
-      <c r="BO19" s="1"/>
-      <c r="BP19" s="1"/>
-      <c r="BQ19" s="1"/>
-      <c r="BR19" s="1"/>
-      <c r="BS19" s="1"/>
-      <c r="BT19" s="1"/>
-      <c r="BU19" s="1"/>
-      <c r="BV19" s="1"/>
-    </row>
-    <row r="20" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="14"/>
-      <c r="AB20" s="14"/>
-      <c r="AC20" s="14"/>
-      <c r="AD20" s="14"/>
-      <c r="AE20" s="14"/>
-      <c r="AF20" s="14"/>
-      <c r="AG20" s="14"/>
-      <c r="AH20" s="14"/>
-      <c r="AI20" s="14"/>
-      <c r="AJ20" s="14"/>
-      <c r="AK20" s="14"/>
-      <c r="AL20" s="14"/>
-      <c r="AM20" s="14"/>
-      <c r="AN20" s="14"/>
-      <c r="AO20" s="14"/>
-      <c r="AP20" s="14"/>
-      <c r="AQ20" s="14"/>
-      <c r="AR20" s="14"/>
-      <c r="AS20" s="14"/>
-      <c r="AT20" s="14"/>
-      <c r="AU20" s="14"/>
-      <c r="AV20" s="14"/>
-      <c r="AW20" s="14"/>
-      <c r="AX20" s="14"/>
-      <c r="AY20" s="14"/>
-      <c r="AZ20" s="14"/>
-      <c r="BA20" s="52"/>
-      <c r="BB20" s="14"/>
-      <c r="BC20" s="14"/>
-      <c r="BD20" s="14"/>
-      <c r="BE20" s="14"/>
-      <c r="BF20" s="52"/>
-      <c r="BG20" s="63"/>
-      <c r="BH20" s="69"/>
-      <c r="BI20" s="69"/>
-      <c r="BJ20" s="69"/>
-      <c r="BK20" s="69"/>
-      <c r="BL20" s="69"/>
-      <c r="BM20" s="69"/>
-      <c r="BN20" s="69"/>
-      <c r="BO20" s="1"/>
-      <c r="BP20" s="1"/>
-      <c r="BQ20" s="1"/>
-      <c r="BR20" s="1"/>
-      <c r="BS20" s="1"/>
-      <c r="BT20" s="1"/>
-      <c r="BU20" s="1"/>
-      <c r="BV20" s="1"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="73"/>
+      <c r="T20" s="73"/>
+      <c r="U20" s="73"/>
+      <c r="V20" s="73"/>
+      <c r="W20" s="73"/>
+      <c r="X20" s="73"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="48"/>
+      <c r="AE20" s="48"/>
+      <c r="AF20" s="48"/>
+      <c r="AG20" s="48"/>
+      <c r="AH20" s="48"/>
+      <c r="AI20" s="48"/>
+      <c r="AJ20" s="48"/>
+      <c r="AK20" s="48"/>
+      <c r="AL20" s="48"/>
+      <c r="AM20" s="48"/>
+      <c r="AN20" s="48"/>
+      <c r="AO20" s="48"/>
+      <c r="AP20" s="48"/>
+      <c r="AQ20" s="48"/>
+      <c r="AR20" s="48"/>
+      <c r="AS20" s="48"/>
+      <c r="AT20" s="48"/>
+      <c r="AU20" s="48"/>
+      <c r="AV20" s="48"/>
+      <c r="AW20" s="48"/>
+      <c r="AX20" s="48"/>
+      <c r="AY20" s="48"/>
+      <c r="AZ20" s="48"/>
+      <c r="BA20" s="74"/>
+      <c r="BB20" s="48"/>
+      <c r="BC20" s="48"/>
+      <c r="BD20" s="48"/>
+      <c r="BE20" s="48"/>
+      <c r="BF20" s="74"/>
+      <c r="BG20" s="75"/>
+      <c r="BI20" s="53"/>
+      <c r="BJ20" s="53"/>
+      <c r="BK20" s="53"/>
+      <c r="BM20" s="30"/>
+      <c r="BO20" s="22"/>
+      <c r="BP20" s="22"/>
+      <c r="BQ20" s="22"/>
+      <c r="BR20" s="22"/>
+      <c r="BS20" s="22"/>
+      <c r="BT20" s="22"/>
+      <c r="BU20" s="22"/>
+      <c r="BV20" s="22"/>
     </row>
     <row r="21" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>48</v>
@@ -2863,10 +2866,10 @@
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
       <c r="R21" s="14"/>
-      <c r="S21" s="16"/>
+      <c r="S21" s="14"/>
       <c r="T21" s="14"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
+      <c r="V21" s="16"/>
       <c r="W21" s="14"/>
       <c r="X21" s="14"/>
       <c r="Y21" s="14"/>
@@ -2897,20 +2900,20 @@
       <c r="AX21" s="14"/>
       <c r="AY21" s="14"/>
       <c r="AZ21" s="14"/>
-      <c r="BA21" s="52"/>
+      <c r="BA21" s="39"/>
       <c r="BB21" s="14"/>
       <c r="BC21" s="14"/>
       <c r="BD21" s="14"/>
       <c r="BE21" s="14"/>
-      <c r="BF21" s="52"/>
-      <c r="BG21" s="63"/>
-      <c r="BH21" s="69"/>
-      <c r="BI21" s="69"/>
-      <c r="BJ21" s="69"/>
-      <c r="BK21" s="69"/>
-      <c r="BL21" s="69"/>
-      <c r="BM21" s="69"/>
-      <c r="BN21" s="69"/>
+      <c r="BF21" s="39"/>
+      <c r="BG21" s="43"/>
+      <c r="BH21" s="14"/>
+      <c r="BI21" s="49"/>
+      <c r="BJ21" s="49"/>
+      <c r="BK21" s="49"/>
+      <c r="BL21" s="49"/>
+      <c r="BM21" s="49"/>
+      <c r="BN21" s="49"/>
       <c r="BO21" s="1"/>
       <c r="BP21" s="1"/>
       <c r="BQ21" s="1"/>
@@ -2923,7 +2926,7 @@
     <row r="22" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="19" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>48</v>
@@ -2977,20 +2980,20 @@
       <c r="AX22" s="14"/>
       <c r="AY22" s="14"/>
       <c r="AZ22" s="14"/>
-      <c r="BA22" s="52"/>
+      <c r="BA22" s="39"/>
       <c r="BB22" s="14"/>
       <c r="BC22" s="14"/>
       <c r="BD22" s="14"/>
       <c r="BE22" s="14"/>
-      <c r="BF22" s="52"/>
-      <c r="BG22" s="64"/>
-      <c r="BH22" s="69"/>
-      <c r="BI22" s="69"/>
-      <c r="BJ22" s="69"/>
-      <c r="BK22" s="69"/>
-      <c r="BL22" s="69"/>
-      <c r="BM22" s="69"/>
-      <c r="BN22" s="69"/>
+      <c r="BF22" s="39"/>
+      <c r="BG22" s="43"/>
+      <c r="BH22" s="14"/>
+      <c r="BI22" s="49"/>
+      <c r="BJ22" s="49"/>
+      <c r="BK22" s="49"/>
+      <c r="BL22" s="49"/>
+      <c r="BM22" s="49"/>
+      <c r="BN22" s="49"/>
       <c r="BO22" s="1"/>
       <c r="BP22" s="1"/>
       <c r="BQ22" s="1"/>
@@ -3003,7 +3006,7 @@
     <row r="23" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="19" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>48</v>
@@ -3023,8 +3026,8 @@
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="14"/>
       <c r="U23" s="14"/>
       <c r="V23" s="14"/>
       <c r="W23" s="14"/>
@@ -3057,20 +3060,20 @@
       <c r="AX23" s="14"/>
       <c r="AY23" s="14"/>
       <c r="AZ23" s="14"/>
-      <c r="BA23" s="52"/>
+      <c r="BA23" s="39"/>
       <c r="BB23" s="14"/>
       <c r="BC23" s="14"/>
       <c r="BD23" s="14"/>
       <c r="BE23" s="14"/>
-      <c r="BF23" s="52"/>
-      <c r="BG23" s="64"/>
-      <c r="BH23" s="69"/>
-      <c r="BI23" s="69"/>
-      <c r="BJ23" s="69"/>
-      <c r="BK23" s="69"/>
-      <c r="BL23" s="69"/>
-      <c r="BM23" s="69"/>
-      <c r="BN23" s="69"/>
+      <c r="BF23" s="39"/>
+      <c r="BG23" s="44"/>
+      <c r="BH23" s="14"/>
+      <c r="BI23" s="49"/>
+      <c r="BJ23" s="49"/>
+      <c r="BK23" s="49"/>
+      <c r="BL23" s="49"/>
+      <c r="BM23" s="49"/>
+      <c r="BN23" s="49"/>
       <c r="BO23" s="1"/>
       <c r="BP23" s="1"/>
       <c r="BQ23" s="1"/>
@@ -3083,7 +3086,7 @@
     <row r="24" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>48</v>
@@ -3104,8 +3107,8 @@
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
       <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="14"/>
       <c r="V24" s="14"/>
       <c r="W24" s="14"/>
       <c r="X24" s="14"/>
@@ -3137,33 +3140,33 @@
       <c r="AX24" s="14"/>
       <c r="AY24" s="14"/>
       <c r="AZ24" s="14"/>
-      <c r="BA24" s="52"/>
+      <c r="BA24" s="39"/>
       <c r="BB24" s="14"/>
       <c r="BC24" s="14"/>
       <c r="BD24" s="14"/>
       <c r="BE24" s="14"/>
-      <c r="BF24" s="52"/>
-      <c r="BG24" s="63"/>
-      <c r="BH24" s="69"/>
-      <c r="BI24" s="69"/>
-      <c r="BJ24" s="69"/>
-      <c r="BK24" s="69"/>
-      <c r="BL24" s="69"/>
-      <c r="BM24" s="69"/>
-      <c r="BN24" s="69"/>
-      <c r="BO24" s="69"/>
-      <c r="BP24" s="69"/>
-      <c r="BQ24" s="69"/>
-      <c r="BR24" s="69"/>
-      <c r="BS24" s="69"/>
+      <c r="BF24" s="39"/>
+      <c r="BG24" s="44"/>
+      <c r="BH24" s="14"/>
+      <c r="BI24" s="49"/>
+      <c r="BJ24" s="49"/>
+      <c r="BK24" s="49"/>
+      <c r="BL24" s="49"/>
+      <c r="BM24" s="49"/>
+      <c r="BN24" s="49"/>
+      <c r="BO24" s="1"/>
+      <c r="BP24" s="1"/>
+      <c r="BQ24" s="1"/>
+      <c r="BR24" s="1"/>
+      <c r="BS24" s="1"/>
       <c r="BT24" s="1"/>
       <c r="BU24" s="1"/>
       <c r="BV24" s="1"/>
     </row>
-    <row r="25" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="19" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>48</v>
@@ -3185,10 +3188,10 @@
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
       <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
+      <c r="U25" s="16"/>
       <c r="V25" s="14"/>
       <c r="W25" s="14"/>
-      <c r="X25" s="16"/>
+      <c r="X25" s="14"/>
       <c r="Y25" s="14"/>
       <c r="Z25" s="14"/>
       <c r="AA25" s="14"/>
@@ -3217,33 +3220,33 @@
       <c r="AX25" s="14"/>
       <c r="AY25" s="14"/>
       <c r="AZ25" s="14"/>
-      <c r="BA25" s="52"/>
+      <c r="BA25" s="39"/>
       <c r="BB25" s="14"/>
       <c r="BC25" s="14"/>
       <c r="BD25" s="14"/>
       <c r="BE25" s="14"/>
-      <c r="BF25" s="52"/>
-      <c r="BG25" s="65"/>
-      <c r="BH25" s="69"/>
-      <c r="BI25" s="69"/>
-      <c r="BJ25" s="69"/>
-      <c r="BK25" s="69"/>
-      <c r="BL25" s="69"/>
-      <c r="BM25" s="69"/>
-      <c r="BN25" s="69"/>
-      <c r="BO25" s="69"/>
-      <c r="BP25" s="69"/>
-      <c r="BQ25" s="69"/>
-      <c r="BR25" s="69"/>
-      <c r="BS25" s="69"/>
+      <c r="BF25" s="39"/>
+      <c r="BG25" s="43"/>
+      <c r="BH25" s="14"/>
+      <c r="BI25" s="49"/>
+      <c r="BJ25" s="49"/>
+      <c r="BK25" s="49"/>
+      <c r="BL25" s="49"/>
+      <c r="BM25" s="49"/>
+      <c r="BN25" s="49"/>
+      <c r="BO25" s="49"/>
+      <c r="BP25" s="49"/>
+      <c r="BQ25" s="49"/>
+      <c r="BR25" s="49"/>
+      <c r="BS25" s="49"/>
       <c r="BT25" s="1"/>
       <c r="BU25" s="1"/>
       <c r="BV25" s="1"/>
     </row>
-    <row r="26" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>12</v>
+      <c r="B26" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>48</v>
@@ -3268,15 +3271,15 @@
       <c r="U26" s="14"/>
       <c r="V26" s="14"/>
       <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="20"/>
-      <c r="Z26" s="20"/>
-      <c r="AA26" s="20"/>
-      <c r="AB26" s="20"/>
-      <c r="AC26" s="20"/>
-      <c r="AD26" s="20"/>
-      <c r="AE26" s="20"/>
-      <c r="AF26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="14"/>
+      <c r="Z26" s="14"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="14"/>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="14"/>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="14"/>
       <c r="AG26" s="14"/>
       <c r="AH26" s="14"/>
       <c r="AI26" s="14"/>
@@ -3297,25 +3300,25 @@
       <c r="AX26" s="14"/>
       <c r="AY26" s="14"/>
       <c r="AZ26" s="14"/>
-      <c r="BA26" s="52"/>
+      <c r="BA26" s="39"/>
       <c r="BB26" s="14"/>
       <c r="BC26" s="14"/>
       <c r="BD26" s="14"/>
-      <c r="BE26" s="68"/>
-      <c r="BF26" s="66"/>
-      <c r="BG26" s="14"/>
-      <c r="BH26" s="69"/>
-      <c r="BI26" s="69"/>
-      <c r="BJ26" s="69"/>
-      <c r="BK26" s="69"/>
-      <c r="BL26" s="69"/>
-      <c r="BM26" s="69"/>
-      <c r="BN26" s="41"/>
-      <c r="BO26" s="1"/>
-      <c r="BP26" s="69"/>
-      <c r="BQ26" s="69"/>
-      <c r="BR26" s="69"/>
-      <c r="BS26" s="69"/>
+      <c r="BE26" s="14"/>
+      <c r="BF26" s="39"/>
+      <c r="BG26" s="45"/>
+      <c r="BH26" s="14"/>
+      <c r="BI26" s="49"/>
+      <c r="BJ26" s="49"/>
+      <c r="BK26" s="49"/>
+      <c r="BL26" s="49"/>
+      <c r="BM26" s="49"/>
+      <c r="BN26" s="49"/>
+      <c r="BO26" s="49"/>
+      <c r="BP26" s="49"/>
+      <c r="BQ26" s="49"/>
+      <c r="BR26" s="49"/>
+      <c r="BS26" s="49"/>
       <c r="BT26" s="1"/>
       <c r="BU26" s="1"/>
       <c r="BV26" s="1"/>
@@ -3323,7 +3326,7 @@
     <row r="27" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>48</v>
@@ -3349,13 +3352,14 @@
       <c r="V27" s="14"/>
       <c r="W27" s="14"/>
       <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="14"/>
-      <c r="AB27" s="14"/>
-      <c r="AC27" s="14"/>
-      <c r="AD27" s="16"/>
-      <c r="AF27" s="14"/>
+      <c r="Y27" s="20"/>
+      <c r="Z27" s="20"/>
+      <c r="AA27" s="20"/>
+      <c r="AB27" s="20"/>
+      <c r="AC27" s="20"/>
+      <c r="AD27" s="20"/>
+      <c r="AE27" s="20"/>
+      <c r="AF27" s="16"/>
       <c r="AG27" s="14"/>
       <c r="AH27" s="14"/>
       <c r="AI27" s="14"/>
@@ -3376,25 +3380,25 @@
       <c r="AX27" s="14"/>
       <c r="AY27" s="14"/>
       <c r="AZ27" s="14"/>
-      <c r="BA27" s="52"/>
+      <c r="BA27" s="39"/>
       <c r="BB27" s="14"/>
       <c r="BC27" s="14"/>
       <c r="BD27" s="14"/>
-      <c r="BE27" s="14"/>
-      <c r="BF27" s="62"/>
+      <c r="BE27" s="48"/>
+      <c r="BF27" s="46"/>
       <c r="BG27" s="14"/>
-      <c r="BH27" s="69"/>
-      <c r="BI27" s="69"/>
-      <c r="BJ27" s="69"/>
-      <c r="BK27" s="69"/>
-      <c r="BL27" s="69"/>
-      <c r="BM27" s="69"/>
-      <c r="BN27" s="41"/>
-      <c r="BO27" s="1"/>
-      <c r="BP27" s="69"/>
-      <c r="BQ27" s="69"/>
-      <c r="BR27" s="69"/>
-      <c r="BS27" s="69"/>
+      <c r="BH27" s="26"/>
+      <c r="BI27" s="49"/>
+      <c r="BJ27" s="49"/>
+      <c r="BK27" s="49"/>
+      <c r="BL27" s="49"/>
+      <c r="BM27" s="49"/>
+      <c r="BN27" s="49"/>
+      <c r="BO27" s="8"/>
+      <c r="BP27" s="49"/>
+      <c r="BQ27" s="49"/>
+      <c r="BR27" s="49"/>
+      <c r="BS27" s="49"/>
       <c r="BT27" s="1"/>
       <c r="BU27" s="1"/>
       <c r="BV27" s="1"/>
@@ -3402,7 +3406,7 @@
     <row r="28" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>48</v>
@@ -3427,14 +3431,14 @@
       <c r="U28" s="14"/>
       <c r="V28" s="14"/>
       <c r="W28" s="14"/>
-      <c r="Y28" s="20"/>
-      <c r="Z28" s="20"/>
-      <c r="AA28" s="20"/>
-      <c r="AB28" s="20"/>
-      <c r="AC28" s="20"/>
-      <c r="AD28" s="20"/>
-      <c r="AE28" s="20"/>
-      <c r="AF28" s="16"/>
+      <c r="X28" s="14"/>
+      <c r="Y28" s="14"/>
+      <c r="Z28" s="14"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="14"/>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="16"/>
+      <c r="AF28" s="14"/>
       <c r="AG28" s="14"/>
       <c r="AH28" s="14"/>
       <c r="AI28" s="14"/>
@@ -3455,25 +3459,25 @@
       <c r="AX28" s="14"/>
       <c r="AY28" s="14"/>
       <c r="AZ28" s="14"/>
-      <c r="BA28" s="52"/>
+      <c r="BA28" s="39"/>
       <c r="BB28" s="14"/>
       <c r="BC28" s="14"/>
       <c r="BD28" s="14"/>
       <c r="BE28" s="14"/>
-      <c r="BF28" s="62"/>
+      <c r="BF28" s="42"/>
       <c r="BG28" s="14"/>
-      <c r="BH28" s="7"/>
-      <c r="BI28" s="69"/>
-      <c r="BJ28" s="69"/>
-      <c r="BK28" s="69"/>
-      <c r="BL28" s="69"/>
-      <c r="BM28" s="69"/>
-      <c r="BN28" s="41"/>
-      <c r="BO28" s="1"/>
-      <c r="BP28" s="69"/>
-      <c r="BQ28" s="69"/>
-      <c r="BR28" s="69"/>
-      <c r="BS28" s="69"/>
+      <c r="BH28" s="26"/>
+      <c r="BI28" s="49"/>
+      <c r="BJ28" s="49"/>
+      <c r="BK28" s="49"/>
+      <c r="BL28" s="49"/>
+      <c r="BM28" s="58"/>
+      <c r="BN28" s="49"/>
+      <c r="BO28" s="8"/>
+      <c r="BP28" s="49"/>
+      <c r="BQ28" s="49"/>
+      <c r="BR28" s="49"/>
+      <c r="BS28" s="49"/>
       <c r="BT28" s="1"/>
       <c r="BU28" s="1"/>
       <c r="BV28" s="1"/>
@@ -3481,7 +3485,7 @@
     <row r="29" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>48</v>
@@ -3505,16 +3509,15 @@
       <c r="T29" s="14"/>
       <c r="U29" s="14"/>
       <c r="V29" s="14"/>
-      <c r="W29" s="16"/>
-      <c r="X29" s="14"/>
-      <c r="Y29" s="14"/>
-      <c r="Z29" s="14"/>
-      <c r="AA29" s="14"/>
-      <c r="AB29" s="14"/>
-      <c r="AC29" s="14"/>
-      <c r="AD29" s="14"/>
-      <c r="AE29" s="14"/>
-      <c r="AF29" s="14"/>
+      <c r="W29" s="14"/>
+      <c r="Y29" s="20"/>
+      <c r="Z29" s="20"/>
+      <c r="AA29" s="20"/>
+      <c r="AB29" s="20"/>
+      <c r="AC29" s="20"/>
+      <c r="AD29" s="20"/>
+      <c r="AE29" s="20"/>
+      <c r="AF29" s="16"/>
       <c r="AG29" s="14"/>
       <c r="AH29" s="14"/>
       <c r="AI29" s="14"/>
@@ -3535,33 +3538,33 @@
       <c r="AX29" s="14"/>
       <c r="AY29" s="14"/>
       <c r="AZ29" s="14"/>
-      <c r="BA29" s="52"/>
+      <c r="BA29" s="39"/>
       <c r="BB29" s="14"/>
       <c r="BC29" s="14"/>
       <c r="BD29" s="14"/>
       <c r="BE29" s="14"/>
-      <c r="BF29" s="62"/>
+      <c r="BF29" s="42"/>
       <c r="BG29" s="14"/>
-      <c r="BH29" s="7"/>
-      <c r="BI29" s="69"/>
-      <c r="BJ29" s="69"/>
-      <c r="BK29" s="69"/>
-      <c r="BL29" s="69"/>
-      <c r="BM29" s="69"/>
-      <c r="BN29" s="69"/>
-      <c r="BO29" s="69"/>
-      <c r="BP29" s="27"/>
-      <c r="BQ29" s="69"/>
-      <c r="BR29" s="69"/>
-      <c r="BS29" s="69"/>
+      <c r="BH29" s="26"/>
+      <c r="BI29" s="49"/>
+      <c r="BJ29" s="49"/>
+      <c r="BK29" s="49"/>
+      <c r="BL29" s="49"/>
+      <c r="BM29" s="58"/>
+      <c r="BN29" s="49"/>
+      <c r="BO29" s="8"/>
+      <c r="BP29" s="49"/>
+      <c r="BQ29" s="49"/>
+      <c r="BR29" s="49"/>
+      <c r="BS29" s="49"/>
       <c r="BT29" s="1"/>
       <c r="BU29" s="1"/>
       <c r="BV29" s="1"/>
     </row>
-    <row r="30" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>48</v>
@@ -3585,8 +3588,8 @@
       <c r="T30" s="14"/>
       <c r="U30" s="14"/>
       <c r="V30" s="14"/>
-      <c r="W30" s="14"/>
-      <c r="X30" s="16"/>
+      <c r="W30" s="16"/>
+      <c r="X30" s="14"/>
       <c r="Y30" s="14"/>
       <c r="Z30" s="14"/>
       <c r="AA30" s="14"/>
@@ -3615,33 +3618,33 @@
       <c r="AX30" s="14"/>
       <c r="AY30" s="14"/>
       <c r="AZ30" s="14"/>
-      <c r="BA30" s="52"/>
+      <c r="BA30" s="39"/>
       <c r="BB30" s="14"/>
       <c r="BC30" s="14"/>
       <c r="BD30" s="14"/>
       <c r="BE30" s="14"/>
-      <c r="BF30" s="62"/>
+      <c r="BF30" s="42"/>
       <c r="BG30" s="14"/>
-      <c r="BH30" s="7"/>
-      <c r="BI30" s="69"/>
-      <c r="BJ30" s="69"/>
-      <c r="BK30" s="69"/>
-      <c r="BL30" s="72"/>
-      <c r="BM30" s="72"/>
-      <c r="BN30" s="72"/>
-      <c r="BO30" s="69"/>
-      <c r="BP30" s="27"/>
-      <c r="BQ30" s="69"/>
-      <c r="BR30" s="69"/>
-      <c r="BS30" s="69"/>
+      <c r="BH30" s="26"/>
+      <c r="BI30" s="49"/>
+      <c r="BJ30" s="49"/>
+      <c r="BK30" s="49"/>
+      <c r="BL30" s="49"/>
+      <c r="BM30" s="58"/>
+      <c r="BN30" s="49"/>
+      <c r="BO30" s="8"/>
+      <c r="BP30" s="1"/>
+      <c r="BQ30" s="49"/>
+      <c r="BR30" s="49"/>
+      <c r="BS30" s="49"/>
       <c r="BT30" s="1"/>
       <c r="BU30" s="1"/>
       <c r="BV30" s="1"/>
     </row>
-    <row r="31" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>48</v>
@@ -3666,14 +3669,14 @@
       <c r="U31" s="14"/>
       <c r="V31" s="14"/>
       <c r="W31" s="14"/>
-      <c r="X31" s="14"/>
+      <c r="X31" s="16"/>
       <c r="Y31" s="14"/>
       <c r="Z31" s="14"/>
-      <c r="AA31" s="16"/>
+      <c r="AA31" s="14"/>
       <c r="AB31" s="14"/>
-      <c r="AC31" s="20"/>
-      <c r="AD31" s="20"/>
-      <c r="AE31" s="20"/>
+      <c r="AC31" s="14"/>
+      <c r="AD31" s="14"/>
+      <c r="AE31" s="14"/>
       <c r="AF31" s="14"/>
       <c r="AG31" s="14"/>
       <c r="AH31" s="14"/>
@@ -3695,33 +3698,33 @@
       <c r="AX31" s="14"/>
       <c r="AY31" s="14"/>
       <c r="AZ31" s="14"/>
-      <c r="BA31" s="14"/>
+      <c r="BA31" s="39"/>
       <c r="BB31" s="14"/>
       <c r="BC31" s="14"/>
       <c r="BD31" s="14"/>
       <c r="BE31" s="14"/>
-      <c r="BF31" s="14"/>
+      <c r="BF31" s="42"/>
       <c r="BG31" s="14"/>
-      <c r="BH31" s="69"/>
-      <c r="BI31" s="69"/>
-      <c r="BJ31" s="73"/>
-      <c r="BK31" s="74"/>
-      <c r="BL31" s="29"/>
-      <c r="BM31" s="31"/>
-      <c r="BN31" s="30"/>
-      <c r="BO31" s="40"/>
+      <c r="BH31" s="26"/>
+      <c r="BI31" s="49"/>
+      <c r="BJ31" s="49"/>
+      <c r="BK31" s="49"/>
+      <c r="BL31" s="49"/>
+      <c r="BM31" s="60"/>
+      <c r="BN31" s="52"/>
+      <c r="BO31" s="8"/>
       <c r="BP31" s="1"/>
-      <c r="BQ31" s="8"/>
-      <c r="BR31" s="1"/>
-      <c r="BS31" s="1"/>
+      <c r="BQ31" s="49"/>
+      <c r="BR31" s="49"/>
+      <c r="BS31" s="49"/>
       <c r="BT31" s="1"/>
       <c r="BU31" s="1"/>
       <c r="BV31" s="1"/>
     </row>
-    <row r="32" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
-      <c r="B32" s="19" t="s">
-        <v>56</v>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>48</v>
@@ -3750,9 +3753,10 @@
       <c r="Y32" s="14"/>
       <c r="Z32" s="14"/>
       <c r="AA32" s="16"/>
-      <c r="AC32" s="14"/>
-      <c r="AD32" s="14"/>
-      <c r="AE32" s="14"/>
+      <c r="AB32" s="14"/>
+      <c r="AC32" s="20"/>
+      <c r="AD32" s="20"/>
+      <c r="AE32" s="20"/>
       <c r="AF32" s="14"/>
       <c r="AG32" s="14"/>
       <c r="AH32" s="14"/>
@@ -3781,26 +3785,26 @@
       <c r="BE32" s="14"/>
       <c r="BF32" s="14"/>
       <c r="BG32" s="14"/>
-      <c r="BH32" s="69"/>
-      <c r="BI32" s="69"/>
-      <c r="BJ32" s="69"/>
-      <c r="BK32" s="75"/>
-      <c r="BL32" s="76"/>
-      <c r="BM32" s="7"/>
-      <c r="BN32" s="77"/>
-      <c r="BO32" s="21"/>
-      <c r="BP32" s="1"/>
-      <c r="BQ32" s="8"/>
-      <c r="BR32" s="1"/>
+      <c r="BH32" s="14"/>
+      <c r="BI32" s="49"/>
+      <c r="BJ32" s="53"/>
+      <c r="BK32" s="49"/>
+      <c r="BL32" s="59"/>
+      <c r="BM32" s="27"/>
+      <c r="BN32" s="29"/>
+      <c r="BO32" s="28"/>
+      <c r="BP32" s="22"/>
+      <c r="BQ32" s="30"/>
+      <c r="BR32" s="22"/>
       <c r="BS32" s="1"/>
       <c r="BT32" s="1"/>
       <c r="BU32" s="1"/>
       <c r="BV32" s="1"/>
     </row>
-    <row r="33" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>48</v>
@@ -3860,15 +3864,15 @@
       <c r="BE33" s="14"/>
       <c r="BF33" s="14"/>
       <c r="BG33" s="14"/>
-      <c r="BH33" s="69"/>
-      <c r="BI33" s="69"/>
-      <c r="BJ33" s="69"/>
-      <c r="BK33" s="75"/>
-      <c r="BL33" s="78"/>
-      <c r="BM33" s="79"/>
-      <c r="BN33" s="25"/>
-      <c r="BO33" s="26"/>
-      <c r="BP33" s="22"/>
+      <c r="BH33" s="14"/>
+      <c r="BI33" s="49"/>
+      <c r="BJ33" s="49"/>
+      <c r="BK33" s="49"/>
+      <c r="BL33" s="59"/>
+      <c r="BM33" s="54"/>
+      <c r="BN33" s="7"/>
+      <c r="BO33" s="55"/>
+      <c r="BP33" s="1"/>
       <c r="BQ33" s="8"/>
       <c r="BR33" s="1"/>
       <c r="BS33" s="1"/>
@@ -3876,10 +3880,10 @@
       <c r="BU33" s="1"/>
       <c r="BV33" s="1"/>
     </row>
-    <row r="34" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>8</v>
+      <c r="B34" s="19" t="s">
+        <v>58</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>48</v>
@@ -3907,11 +3911,10 @@
       <c r="X34" s="14"/>
       <c r="Y34" s="14"/>
       <c r="Z34" s="14"/>
-      <c r="AA34" s="14"/>
-      <c r="AB34" s="16"/>
-      <c r="AC34" s="20"/>
-      <c r="AD34" s="20"/>
-      <c r="AE34" s="20"/>
+      <c r="AA34" s="16"/>
+      <c r="AC34" s="14"/>
+      <c r="AD34" s="14"/>
+      <c r="AE34" s="14"/>
       <c r="AF34" s="14"/>
       <c r="AG34" s="14"/>
       <c r="AH34" s="14"/>
@@ -3940,26 +3943,26 @@
       <c r="BE34" s="14"/>
       <c r="BF34" s="14"/>
       <c r="BG34" s="14"/>
-      <c r="BH34" s="69"/>
-      <c r="BI34" s="69"/>
-      <c r="BJ34" s="69"/>
-      <c r="BK34" s="80"/>
-      <c r="BL34" s="81"/>
-      <c r="BM34" s="73"/>
-      <c r="BN34" s="82"/>
-      <c r="BO34" s="29"/>
-      <c r="BP34" s="30"/>
-      <c r="BQ34" s="40"/>
-      <c r="BR34" s="41"/>
-      <c r="BS34" s="8"/>
+      <c r="BH34" s="14"/>
+      <c r="BI34" s="49"/>
+      <c r="BJ34" s="49"/>
+      <c r="BK34" s="49"/>
+      <c r="BL34" s="59"/>
+      <c r="BM34" s="56"/>
+      <c r="BN34" s="57"/>
+      <c r="BO34" s="24"/>
+      <c r="BP34" s="21"/>
+      <c r="BQ34" s="8"/>
+      <c r="BR34" s="1"/>
+      <c r="BS34" s="1"/>
       <c r="BT34" s="1"/>
       <c r="BU34" s="1"/>
       <c r="BV34" s="1"/>
     </row>
-    <row r="35" spans="1:74" ht="15" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
-      <c r="B35" s="19" t="s">
-        <v>57</v>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>48</v>
@@ -3988,10 +3991,10 @@
       <c r="Y35" s="14"/>
       <c r="Z35" s="14"/>
       <c r="AA35" s="14"/>
-      <c r="AB35" s="5"/>
-      <c r="AC35" s="14"/>
-      <c r="AD35" s="14"/>
-      <c r="AE35" s="14"/>
+      <c r="AB35" s="16"/>
+      <c r="AC35" s="20"/>
+      <c r="AD35" s="20"/>
+      <c r="AE35" s="20"/>
       <c r="AF35" s="14"/>
       <c r="AG35" s="14"/>
       <c r="AH35" s="14"/>
@@ -4020,26 +4023,26 @@
       <c r="BE35" s="14"/>
       <c r="BF35" s="14"/>
       <c r="BG35" s="14"/>
-      <c r="BH35" s="69"/>
-      <c r="BI35" s="69"/>
-      <c r="BJ35" s="69"/>
-      <c r="BK35" s="80"/>
-      <c r="BL35" s="80"/>
-      <c r="BM35" s="69"/>
-      <c r="BN35" s="83"/>
-      <c r="BO35" s="24"/>
-      <c r="BP35" s="25"/>
-      <c r="BQ35" s="21"/>
-      <c r="BR35" s="8"/>
+      <c r="BH35" s="14"/>
+      <c r="BI35" s="49"/>
+      <c r="BJ35" s="49"/>
+      <c r="BK35" s="49"/>
+      <c r="BL35" s="49"/>
+      <c r="BM35" s="53"/>
+      <c r="BN35" s="53"/>
+      <c r="BO35" s="84"/>
+      <c r="BP35" s="27"/>
+      <c r="BQ35" s="28"/>
+      <c r="BR35" s="30"/>
       <c r="BS35" s="8"/>
       <c r="BT35" s="1"/>
       <c r="BU35" s="1"/>
       <c r="BV35" s="1"/>
     </row>
-    <row r="36" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:74" ht="15" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
-        <v>6</v>
+      <c r="B36" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>48</v>
@@ -4068,10 +4071,10 @@
       <c r="Y36" s="14"/>
       <c r="Z36" s="14"/>
       <c r="AA36" s="14"/>
-      <c r="AB36" s="14"/>
-      <c r="AC36" s="16"/>
-      <c r="AD36" s="20"/>
-      <c r="AE36" s="20"/>
+      <c r="AB36" s="5"/>
+      <c r="AC36" s="14"/>
+      <c r="AD36" s="14"/>
+      <c r="AE36" s="14"/>
       <c r="AF36" s="14"/>
       <c r="AG36" s="14"/>
       <c r="AH36" s="14"/>
@@ -4098,30 +4101,30 @@
       <c r="BC36" s="14"/>
       <c r="BD36" s="14"/>
       <c r="BE36" s="14"/>
-      <c r="BF36" s="67"/>
+      <c r="BF36" s="14"/>
       <c r="BG36" s="14"/>
-      <c r="BH36" s="69"/>
-      <c r="BI36" s="69"/>
-      <c r="BJ36" s="69"/>
-      <c r="BK36" s="84"/>
-      <c r="BL36" s="84"/>
-      <c r="BM36" s="72"/>
-      <c r="BN36" s="72"/>
-      <c r="BO36" s="44"/>
-      <c r="BP36" s="44"/>
-      <c r="BQ36" s="45"/>
-      <c r="BR36" s="22"/>
-      <c r="BS36" s="22"/>
-      <c r="BT36" s="27"/>
-      <c r="BU36" s="27"/>
-      <c r="BV36" s="22"/>
+      <c r="BH36" s="14"/>
+      <c r="BI36" s="49"/>
+      <c r="BJ36" s="49"/>
+      <c r="BK36" s="49"/>
+      <c r="BL36" s="49"/>
+      <c r="BM36" s="49"/>
+      <c r="BN36" s="49"/>
+      <c r="BO36" s="83"/>
+      <c r="BP36" s="23"/>
+      <c r="BQ36" s="24"/>
+      <c r="BR36" s="8"/>
+      <c r="BS36" s="8"/>
+      <c r="BT36" s="1"/>
+      <c r="BU36" s="1"/>
+      <c r="BV36" s="1"/>
     </row>
     <row r="37" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="B37" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="47" t="s">
+      <c r="B37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="15"/>
@@ -4149,9 +4152,10 @@
       <c r="Z37" s="14"/>
       <c r="AA37" s="14"/>
       <c r="AB37" s="14"/>
-      <c r="AC37" s="14"/>
-      <c r="AD37" s="14"/>
-      <c r="AE37" s="16"/>
+      <c r="AC37" s="16"/>
+      <c r="AD37" s="20"/>
+      <c r="AE37" s="20"/>
+      <c r="AF37" s="14"/>
       <c r="AG37" s="14"/>
       <c r="AH37" s="14"/>
       <c r="AI37" s="14"/>
@@ -4177,30 +4181,29 @@
       <c r="BC37" s="14"/>
       <c r="BD37" s="14"/>
       <c r="BE37" s="14"/>
-      <c r="BF37" s="14"/>
+      <c r="BF37" s="47"/>
       <c r="BG37" s="14"/>
-      <c r="BH37" s="69"/>
-      <c r="BI37" s="69"/>
-      <c r="BJ37" s="69"/>
-      <c r="BK37" s="69"/>
-      <c r="BL37" s="69"/>
-      <c r="BM37" s="69"/>
-      <c r="BN37" s="53"/>
-      <c r="BO37" s="46"/>
-      <c r="BP37" s="46"/>
-      <c r="BQ37" s="46"/>
-      <c r="BR37" s="46"/>
-      <c r="BS37" s="4"/>
-      <c r="BT37" s="4"/>
-      <c r="BU37" s="4"/>
-      <c r="BV37" s="4"/>
-    </row>
-    <row r="38" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="BH37" s="14"/>
+      <c r="BI37" s="49"/>
+      <c r="BJ37" s="49"/>
+      <c r="BK37" s="60"/>
+      <c r="BL37" s="60"/>
+      <c r="BM37" s="49"/>
+      <c r="BN37" s="49"/>
+      <c r="BO37" s="1"/>
+      <c r="BP37" s="82"/>
+      <c r="BR37" s="33"/>
+      <c r="BS37" s="33"/>
+      <c r="BT37" s="25"/>
+      <c r="BU37" s="25"/>
+      <c r="BV37" s="21"/>
+    </row>
+    <row r="38" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="47" t="s">
+      <c r="B38" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="35" t="s">
         <v>48</v>
       </c>
       <c r="D38" s="15"/>
@@ -4231,7 +4234,6 @@
       <c r="AC38" s="14"/>
       <c r="AD38" s="14"/>
       <c r="AE38" s="16"/>
-      <c r="AF38" s="14"/>
       <c r="AG38" s="14"/>
       <c r="AH38" s="14"/>
       <c r="AI38" s="14"/>
@@ -4259,17 +4261,17 @@
       <c r="BE38" s="14"/>
       <c r="BF38" s="14"/>
       <c r="BG38" s="14"/>
-      <c r="BH38" s="69"/>
-      <c r="BI38" s="80"/>
-      <c r="BJ38" s="69"/>
-      <c r="BK38" s="69"/>
-      <c r="BL38" s="69"/>
-      <c r="BM38" s="69"/>
-      <c r="BN38" s="69"/>
-      <c r="BO38" s="4"/>
-      <c r="BP38" s="4"/>
-      <c r="BQ38" s="4"/>
-      <c r="BR38" s="4"/>
+      <c r="BH38" s="14"/>
+      <c r="BI38" s="49"/>
+      <c r="BJ38" s="49"/>
+      <c r="BK38" s="49"/>
+      <c r="BL38" s="49"/>
+      <c r="BM38" s="49"/>
+      <c r="BN38" s="40"/>
+      <c r="BO38" s="34"/>
+      <c r="BP38" s="34"/>
+      <c r="BQ38" s="34"/>
+      <c r="BR38" s="34"/>
       <c r="BS38" s="4"/>
       <c r="BT38" s="4"/>
       <c r="BU38" s="4"/>
@@ -4277,10 +4279,10 @@
     </row>
     <row r="39" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="47" t="s">
+      <c r="B39" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C39" s="35" t="s">
         <v>48</v>
       </c>
       <c r="D39" s="15"/>
@@ -4339,13 +4341,13 @@
       <c r="BE39" s="14"/>
       <c r="BF39" s="14"/>
       <c r="BG39" s="14"/>
-      <c r="BH39" s="69"/>
-      <c r="BI39" s="80"/>
-      <c r="BJ39" s="69"/>
-      <c r="BK39" s="69"/>
-      <c r="BL39" s="69"/>
-      <c r="BM39" s="69"/>
-      <c r="BN39" s="69"/>
+      <c r="BH39" s="14"/>
+      <c r="BI39" s="58"/>
+      <c r="BJ39" s="49"/>
+      <c r="BK39" s="49"/>
+      <c r="BL39" s="49"/>
+      <c r="BM39" s="49"/>
+      <c r="BN39" s="49"/>
       <c r="BO39" s="4"/>
       <c r="BP39" s="4"/>
       <c r="BQ39" s="4"/>
@@ -4355,12 +4357,12 @@
       <c r="BU39" s="4"/>
       <c r="BV39" s="4"/>
     </row>
-    <row r="40" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" s="47" t="s">
+      <c r="B40" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="35" t="s">
         <v>48</v>
       </c>
       <c r="D40" s="15"/>
@@ -4419,13 +4421,13 @@
       <c r="BE40" s="14"/>
       <c r="BF40" s="14"/>
       <c r="BG40" s="14"/>
-      <c r="BH40" s="69"/>
-      <c r="BI40" s="84"/>
-      <c r="BJ40" s="72"/>
-      <c r="BK40" s="69"/>
-      <c r="BL40" s="69"/>
-      <c r="BM40" s="69"/>
-      <c r="BN40" s="69"/>
+      <c r="BH40" s="14"/>
+      <c r="BI40" s="58"/>
+      <c r="BJ40" s="49"/>
+      <c r="BK40" s="49"/>
+      <c r="BL40" s="49"/>
+      <c r="BM40" s="49"/>
+      <c r="BN40" s="49"/>
       <c r="BO40" s="4"/>
       <c r="BP40" s="4"/>
       <c r="BQ40" s="4"/>
@@ -4435,12 +4437,12 @@
       <c r="BU40" s="4"/>
       <c r="BV40" s="4"/>
     </row>
-    <row r="41" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1"/>
-      <c r="B41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="35" t="s">
         <v>48</v>
       </c>
       <c r="D41" s="15"/>
@@ -4464,13 +4466,13 @@
       <c r="V41" s="14"/>
       <c r="W41" s="14"/>
       <c r="X41" s="14"/>
-      <c r="Y41" s="16"/>
+      <c r="Y41" s="14"/>
       <c r="Z41" s="14"/>
       <c r="AA41" s="14"/>
       <c r="AB41" s="14"/>
       <c r="AC41" s="14"/>
       <c r="AD41" s="14"/>
-      <c r="AE41" s="14"/>
+      <c r="AE41" s="16"/>
       <c r="AF41" s="14"/>
       <c r="AG41" s="14"/>
       <c r="AH41" s="14"/>
@@ -4499,26 +4501,26 @@
       <c r="BE41" s="14"/>
       <c r="BF41" s="14"/>
       <c r="BG41" s="14"/>
-      <c r="BH41" s="83"/>
-      <c r="BI41" s="29"/>
-      <c r="BJ41" s="31"/>
-      <c r="BK41" s="30"/>
-      <c r="BL41" s="73"/>
-      <c r="BM41" s="69"/>
-      <c r="BN41" s="69"/>
-      <c r="BO41" s="41"/>
-      <c r="BP41" s="23"/>
-      <c r="BQ41" s="23"/>
-      <c r="BR41" s="23"/>
-      <c r="BS41" s="23"/>
-      <c r="BT41" s="23"/>
-      <c r="BU41" s="23"/>
-      <c r="BV41" s="23"/>
-    </row>
-    <row r="42" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="BH41" s="14"/>
+      <c r="BI41" s="60"/>
+      <c r="BJ41" s="52"/>
+      <c r="BK41" s="52"/>
+      <c r="BL41" s="52"/>
+      <c r="BM41" s="49"/>
+      <c r="BN41" s="49"/>
+      <c r="BO41" s="4"/>
+      <c r="BP41" s="4"/>
+      <c r="BQ41" s="4"/>
+      <c r="BR41" s="4"/>
+      <c r="BS41" s="4"/>
+      <c r="BT41" s="4"/>
+      <c r="BU41" s="4"/>
+      <c r="BV41" s="4"/>
+    </row>
+    <row r="42" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
-      <c r="B42" s="19" t="s">
-        <v>52</v>
+      <c r="B42" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>48</v>
@@ -4579,26 +4581,26 @@
       <c r="BE42" s="14"/>
       <c r="BF42" s="14"/>
       <c r="BG42" s="14"/>
-      <c r="BH42" s="83"/>
-      <c r="BI42" s="85"/>
-      <c r="BJ42" s="69"/>
-      <c r="BK42" s="77"/>
-      <c r="BL42" s="69"/>
-      <c r="BM42" s="69"/>
-      <c r="BN42" s="69"/>
-      <c r="BO42" s="8"/>
-      <c r="BP42" s="1"/>
-      <c r="BQ42" s="1"/>
-      <c r="BR42" s="1"/>
-      <c r="BS42" s="1"/>
-      <c r="BT42" s="1"/>
-      <c r="BU42" s="1"/>
-      <c r="BV42" s="1"/>
+      <c r="BH42" s="39"/>
+      <c r="BI42" s="59"/>
+      <c r="BJ42" s="27"/>
+      <c r="BK42" s="29"/>
+      <c r="BL42" s="28"/>
+      <c r="BM42" s="58"/>
+      <c r="BN42" s="30"/>
+      <c r="BO42" s="49"/>
+      <c r="BP42" s="22"/>
+      <c r="BQ42" s="22"/>
+      <c r="BR42" s="22"/>
+      <c r="BS42" s="22"/>
+      <c r="BT42" s="22"/>
+      <c r="BU42" s="22"/>
+      <c r="BV42" s="22"/>
     </row>
     <row r="43" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>48</v>
@@ -4659,14 +4661,14 @@
       <c r="BE43" s="14"/>
       <c r="BF43" s="14"/>
       <c r="BG43" s="14"/>
-      <c r="BH43" s="83"/>
-      <c r="BI43" s="76"/>
-      <c r="BJ43" s="7"/>
-      <c r="BK43" s="77"/>
-      <c r="BL43" s="69"/>
-      <c r="BM43" s="69"/>
-      <c r="BN43" s="69"/>
-      <c r="BO43" s="8"/>
+      <c r="BH43" s="39"/>
+      <c r="BI43" s="59"/>
+      <c r="BJ43" s="61"/>
+      <c r="BK43" s="49"/>
+      <c r="BL43" s="55"/>
+      <c r="BM43" s="58"/>
+      <c r="BN43" s="8"/>
+      <c r="BO43" s="49"/>
       <c r="BP43" s="1"/>
       <c r="BQ43" s="1"/>
       <c r="BR43" s="1"/>
@@ -4678,7 +4680,7 @@
     <row r="44" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>48</v>
@@ -4739,14 +4741,14 @@
       <c r="BE44" s="14"/>
       <c r="BF44" s="14"/>
       <c r="BG44" s="14"/>
-      <c r="BH44" s="83"/>
-      <c r="BI44" s="76"/>
-      <c r="BJ44" s="69"/>
-      <c r="BK44" s="42"/>
-      <c r="BL44" s="69"/>
-      <c r="BM44" s="69"/>
-      <c r="BN44" s="69"/>
-      <c r="BO44" s="8"/>
+      <c r="BH44" s="39"/>
+      <c r="BI44" s="59"/>
+      <c r="BJ44" s="54"/>
+      <c r="BK44" s="7"/>
+      <c r="BL44" s="55"/>
+      <c r="BM44" s="58"/>
+      <c r="BN44" s="8"/>
+      <c r="BO44" s="49"/>
       <c r="BP44" s="1"/>
       <c r="BQ44" s="1"/>
       <c r="BR44" s="1"/>
@@ -4758,7 +4760,7 @@
     <row r="45" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>48</v>
@@ -4819,14 +4821,14 @@
       <c r="BE45" s="14"/>
       <c r="BF45" s="14"/>
       <c r="BG45" s="14"/>
-      <c r="BH45" s="83"/>
-      <c r="BI45" s="76"/>
-      <c r="BJ45" s="69"/>
-      <c r="BK45" s="42"/>
-      <c r="BL45" s="69"/>
-      <c r="BM45" s="69"/>
-      <c r="BN45" s="69"/>
-      <c r="BO45" s="8"/>
+      <c r="BH45" s="39"/>
+      <c r="BI45" s="59"/>
+      <c r="BJ45" s="54"/>
+      <c r="BK45" s="49"/>
+      <c r="BL45" s="31"/>
+      <c r="BM45" s="58"/>
+      <c r="BN45" s="8"/>
+      <c r="BO45" s="49"/>
       <c r="BP45" s="1"/>
       <c r="BQ45" s="1"/>
       <c r="BR45" s="1"/>
@@ -4838,7 +4840,7 @@
     <row r="46" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>48</v>
@@ -4899,14 +4901,14 @@
       <c r="BE46" s="14"/>
       <c r="BF46" s="14"/>
       <c r="BG46" s="14"/>
-      <c r="BH46" s="83"/>
-      <c r="BI46" s="76"/>
-      <c r="BJ46" s="7"/>
-      <c r="BK46" s="77"/>
-      <c r="BL46" s="69"/>
-      <c r="BM46" s="69"/>
-      <c r="BN46" s="69"/>
-      <c r="BO46" s="8"/>
+      <c r="BH46" s="39"/>
+      <c r="BI46" s="59"/>
+      <c r="BJ46" s="54"/>
+      <c r="BK46" s="49"/>
+      <c r="BL46" s="31"/>
+      <c r="BM46" s="58"/>
+      <c r="BN46" s="8"/>
+      <c r="BO46" s="49"/>
       <c r="BP46" s="1"/>
       <c r="BQ46" s="1"/>
       <c r="BR46" s="1"/>
@@ -4915,10 +4917,10 @@
       <c r="BU46" s="1"/>
       <c r="BV46" s="1"/>
     </row>
-    <row r="47" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="19" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>48</v>
@@ -4944,8 +4946,8 @@
       <c r="V47" s="14"/>
       <c r="W47" s="14"/>
       <c r="X47" s="14"/>
-      <c r="Y47" s="14"/>
-      <c r="Z47" s="16"/>
+      <c r="Y47" s="16"/>
+      <c r="Z47" s="14"/>
       <c r="AA47" s="14"/>
       <c r="AB47" s="14"/>
       <c r="AC47" s="14"/>
@@ -4979,14 +4981,14 @@
       <c r="BE47" s="14"/>
       <c r="BF47" s="14"/>
       <c r="BG47" s="14"/>
-      <c r="BH47" s="83"/>
-      <c r="BI47" s="43"/>
-      <c r="BJ47" s="79"/>
-      <c r="BK47" s="86"/>
-      <c r="BL47" s="69"/>
-      <c r="BM47" s="69"/>
-      <c r="BN47" s="69"/>
-      <c r="BO47" s="8"/>
+      <c r="BH47" s="39"/>
+      <c r="BI47" s="59"/>
+      <c r="BJ47" s="54"/>
+      <c r="BK47" s="7"/>
+      <c r="BL47" s="55"/>
+      <c r="BM47" s="58"/>
+      <c r="BN47" s="8"/>
+      <c r="BO47" s="49"/>
       <c r="BP47" s="1"/>
       <c r="BQ47" s="1"/>
       <c r="BR47" s="1"/>
@@ -4995,248 +4997,248 @@
       <c r="BU47" s="1"/>
       <c r="BV47" s="1"/>
     </row>
-    <row r="48" spans="1:74" s="33" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="36" t="s">
+    <row r="48" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="21"/>
+      <c r="B48" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="79"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="47"/>
+      <c r="P48" s="47"/>
+      <c r="Q48" s="47"/>
+      <c r="R48" s="47"/>
+      <c r="S48" s="47"/>
+      <c r="T48" s="47"/>
+      <c r="U48" s="47"/>
+      <c r="V48" s="47"/>
+      <c r="W48" s="47"/>
+      <c r="X48" s="47"/>
+      <c r="Y48" s="47"/>
+      <c r="Z48" s="80"/>
+      <c r="AA48" s="47"/>
+      <c r="AB48" s="47"/>
+      <c r="AC48" s="47"/>
+      <c r="AD48" s="47"/>
+      <c r="AE48" s="47"/>
+      <c r="AF48" s="47"/>
+      <c r="AG48" s="47"/>
+      <c r="AH48" s="47"/>
+      <c r="AI48" s="47"/>
+      <c r="AJ48" s="47"/>
+      <c r="AK48" s="47"/>
+      <c r="AL48" s="47"/>
+      <c r="AM48" s="47"/>
+      <c r="AN48" s="47"/>
+      <c r="AO48" s="47"/>
+      <c r="AP48" s="47"/>
+      <c r="AQ48" s="47"/>
+      <c r="AR48" s="47"/>
+      <c r="AS48" s="47"/>
+      <c r="AT48" s="47"/>
+      <c r="AU48" s="47"/>
+      <c r="AV48" s="47"/>
+      <c r="AW48" s="47"/>
+      <c r="AX48" s="47"/>
+      <c r="AY48" s="47"/>
+      <c r="AZ48" s="47"/>
+      <c r="BA48" s="47"/>
+      <c r="BB48" s="47"/>
+      <c r="BC48" s="47"/>
+      <c r="BD48" s="47"/>
+      <c r="BE48" s="47"/>
+      <c r="BF48" s="47"/>
+      <c r="BG48" s="47"/>
+      <c r="BH48" s="81"/>
+      <c r="BI48" s="59"/>
+      <c r="BJ48" s="32"/>
+      <c r="BK48" s="57"/>
+      <c r="BL48" s="62"/>
+      <c r="BM48" s="60"/>
+      <c r="BN48" s="25"/>
+      <c r="BO48" s="52"/>
+      <c r="BP48" s="21"/>
+      <c r="BQ48" s="21"/>
+      <c r="BR48" s="21"/>
+      <c r="BS48" s="21"/>
+      <c r="BT48" s="21"/>
+      <c r="BU48" s="21"/>
+      <c r="BV48" s="21"/>
+    </row>
+    <row r="49" spans="1:74" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="37"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="37"/>
-      <c r="K48" s="37"/>
-      <c r="L48" s="37"/>
-      <c r="M48" s="37"/>
-      <c r="N48" s="37"/>
-      <c r="O48" s="37"/>
-      <c r="P48" s="37"/>
-      <c r="Q48" s="37"/>
-      <c r="R48" s="37"/>
-      <c r="S48" s="37"/>
-      <c r="T48" s="37"/>
-      <c r="U48" s="37"/>
-      <c r="V48" s="37"/>
-      <c r="W48" s="37"/>
-      <c r="X48" s="37"/>
-      <c r="Y48" s="37"/>
-      <c r="Z48" s="37"/>
-      <c r="AA48" s="37"/>
-      <c r="AB48" s="37"/>
-      <c r="AC48" s="37"/>
-      <c r="AD48" s="37"/>
-      <c r="AE48" s="37"/>
-      <c r="AF48" s="37"/>
-      <c r="AG48" s="37"/>
-      <c r="AH48" s="37"/>
-      <c r="AI48" s="37"/>
-      <c r="AJ48" s="37"/>
-      <c r="AK48" s="37"/>
-      <c r="AL48" s="37"/>
-      <c r="AM48" s="37"/>
-      <c r="AN48" s="37"/>
-      <c r="AO48" s="37"/>
-      <c r="AP48" s="37"/>
-      <c r="AQ48" s="39"/>
-      <c r="AR48" s="39"/>
-      <c r="AS48" s="39"/>
-      <c r="AT48" s="39"/>
-      <c r="AU48" s="39"/>
-      <c r="AV48" s="39"/>
-      <c r="AW48" s="39"/>
-      <c r="AX48" s="39"/>
-      <c r="AY48" s="39"/>
-      <c r="AZ48" s="39"/>
-      <c r="BA48" s="39"/>
-      <c r="BB48" s="39"/>
-      <c r="BC48" s="39"/>
-      <c r="BD48" s="39"/>
-      <c r="BE48" s="39"/>
-      <c r="BF48" s="39"/>
-      <c r="BG48" s="39"/>
-      <c r="BH48" s="37"/>
-      <c r="BI48" s="37"/>
-      <c r="BJ48" s="37"/>
-      <c r="BK48" s="37"/>
-      <c r="BL48" s="37"/>
-      <c r="BM48" s="37"/>
-      <c r="BN48" s="37"/>
-      <c r="BO48" s="37"/>
-      <c r="BP48" s="37"/>
-      <c r="BQ48" s="37"/>
-      <c r="BR48" s="37"/>
-      <c r="BS48" s="37"/>
-      <c r="BT48" s="37"/>
-      <c r="BU48" s="37"/>
-      <c r="BV48" s="37"/>
-    </row>
-    <row r="49" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="70"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="70"/>
+      <c r="F49" s="70"/>
+      <c r="G49" s="70"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="70"/>
+      <c r="J49" s="70"/>
+      <c r="K49" s="70"/>
+      <c r="L49" s="70"/>
+      <c r="M49" s="70"/>
+      <c r="N49" s="70"/>
+      <c r="O49" s="70"/>
+      <c r="P49" s="70"/>
+      <c r="Q49" s="70"/>
+      <c r="R49" s="70"/>
+      <c r="S49" s="70"/>
+      <c r="T49" s="70"/>
+      <c r="U49" s="70"/>
+      <c r="V49" s="70"/>
+      <c r="W49" s="70"/>
+      <c r="X49" s="70"/>
+      <c r="Y49" s="70"/>
+      <c r="Z49" s="70"/>
+      <c r="AA49" s="70"/>
+      <c r="AB49" s="70"/>
+      <c r="AC49" s="70"/>
+      <c r="AD49" s="70"/>
+      <c r="AE49" s="70"/>
+      <c r="AF49" s="70"/>
+      <c r="AG49" s="70"/>
+      <c r="AH49" s="70"/>
+      <c r="AI49" s="70"/>
+      <c r="AJ49" s="70"/>
+      <c r="AK49" s="70"/>
+      <c r="AL49" s="70"/>
+      <c r="AM49" s="70"/>
+      <c r="AN49" s="70"/>
+      <c r="AO49" s="70"/>
+      <c r="AP49" s="70"/>
+      <c r="AQ49" s="70"/>
+      <c r="AR49" s="70"/>
+      <c r="AS49" s="70"/>
+      <c r="AT49" s="70"/>
+      <c r="AU49" s="70"/>
+      <c r="AV49" s="70"/>
+      <c r="AW49" s="70"/>
+      <c r="AX49" s="70"/>
+      <c r="AY49" s="70"/>
+      <c r="AZ49" s="70"/>
+      <c r="BA49" s="70"/>
+      <c r="BB49" s="70"/>
+      <c r="BC49" s="70"/>
+      <c r="BD49" s="70"/>
+      <c r="BE49" s="70"/>
+      <c r="BF49" s="70"/>
+      <c r="BG49" s="70"/>
+      <c r="BH49" s="70"/>
+      <c r="BI49" s="71"/>
+      <c r="BJ49" s="71"/>
+      <c r="BK49" s="71"/>
+      <c r="BL49" s="71"/>
+      <c r="BM49" s="70"/>
+      <c r="BN49" s="70"/>
+      <c r="BO49" s="70"/>
+      <c r="BP49" s="70"/>
+      <c r="BQ49" s="70"/>
+      <c r="BR49" s="70"/>
+      <c r="BS49" s="70"/>
+      <c r="BT49" s="70"/>
+      <c r="BU49" s="70"/>
+      <c r="BV49" s="70"/>
+    </row>
+    <row r="50" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="15"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
-      <c r="U49" s="14"/>
-      <c r="V49" s="14"/>
-      <c r="W49" s="14"/>
-      <c r="X49" s="14"/>
-      <c r="Y49" s="14"/>
-      <c r="Z49" s="14"/>
-      <c r="AA49" s="14"/>
-      <c r="AB49" s="14"/>
-      <c r="AC49" s="14"/>
-      <c r="AD49" s="14"/>
-      <c r="AE49" s="14"/>
-      <c r="AF49" s="14"/>
-      <c r="AG49" s="16"/>
-      <c r="AH49" s="14"/>
-      <c r="AI49" s="14"/>
-      <c r="AJ49" s="14"/>
-      <c r="AK49" s="14"/>
-      <c r="AL49" s="14"/>
-      <c r="AM49" s="14"/>
-      <c r="AN49" s="28"/>
-      <c r="AO49" s="28"/>
-      <c r="AP49" s="28"/>
-      <c r="AQ49" s="28"/>
-      <c r="AR49" s="14"/>
-      <c r="AS49" s="14"/>
-      <c r="AT49" s="14"/>
-      <c r="AU49" s="14"/>
-      <c r="AV49" s="14"/>
-      <c r="AW49" s="49"/>
-      <c r="AX49" s="49"/>
-      <c r="AY49" s="14"/>
-      <c r="AZ49" s="14"/>
-      <c r="BA49" s="14"/>
-      <c r="BB49" s="14"/>
-      <c r="BC49" s="14"/>
-      <c r="BD49" s="14"/>
-      <c r="BE49" s="14"/>
-      <c r="BF49" s="14"/>
-      <c r="BG49" s="14"/>
-      <c r="BH49" s="69"/>
-      <c r="BI49" s="8"/>
-      <c r="BJ49" s="69"/>
-      <c r="BK49" s="69"/>
-      <c r="BL49" s="69"/>
-      <c r="BM49" s="69"/>
-      <c r="BN49" s="69"/>
-      <c r="BO49" s="1"/>
-      <c r="BP49" s="1"/>
-      <c r="BQ49" s="1"/>
-      <c r="BR49" s="1"/>
-      <c r="BS49" s="1"/>
-      <c r="BT49" s="1"/>
-      <c r="BU49" s="1"/>
-      <c r="BV49" s="1"/>
-    </row>
-    <row r="50" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="15"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="14"/>
-      <c r="M50" s="14"/>
-      <c r="N50" s="14"/>
-      <c r="O50" s="14"/>
-      <c r="P50" s="14"/>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="14"/>
-      <c r="S50" s="14"/>
-      <c r="T50" s="14"/>
-      <c r="U50" s="14"/>
-      <c r="V50" s="14"/>
-      <c r="W50" s="14"/>
-      <c r="X50" s="14"/>
-      <c r="Y50" s="14"/>
-      <c r="Z50" s="14"/>
-      <c r="AA50" s="14"/>
-      <c r="AB50" s="14"/>
-      <c r="AC50" s="14"/>
-      <c r="AD50" s="14"/>
-      <c r="AE50" s="14"/>
-      <c r="AF50" s="14"/>
-      <c r="AG50" s="16"/>
-      <c r="AH50" s="14"/>
-      <c r="AI50" s="14"/>
-      <c r="AJ50" s="14"/>
-      <c r="AK50" s="14"/>
-      <c r="AL50" s="14"/>
-      <c r="AM50" s="14"/>
-      <c r="AN50" s="14"/>
-      <c r="AO50" s="14"/>
-      <c r="AP50" s="14"/>
-      <c r="AQ50" s="14"/>
-      <c r="AR50" s="28"/>
-      <c r="AS50" s="28"/>
-      <c r="AT50" s="28"/>
-      <c r="AU50" s="14"/>
-      <c r="AV50" s="14"/>
-      <c r="AW50" s="49"/>
-      <c r="AX50" s="49"/>
-      <c r="AY50" s="14"/>
-      <c r="AZ50" s="14"/>
-      <c r="BA50" s="14"/>
-      <c r="BB50" s="14"/>
-      <c r="BC50" s="14"/>
-      <c r="BD50" s="14"/>
-      <c r="BE50" s="14"/>
-      <c r="BF50" s="14"/>
-      <c r="BG50" s="14"/>
-      <c r="BH50" s="69"/>
-      <c r="BI50" s="8"/>
-      <c r="BJ50" s="69"/>
-      <c r="BK50" s="69"/>
-      <c r="BL50" s="69"/>
-      <c r="BM50" s="69"/>
-      <c r="BN50" s="69"/>
-      <c r="BO50" s="1"/>
-      <c r="BP50" s="1"/>
-      <c r="BQ50" s="1"/>
-      <c r="BR50" s="1"/>
-      <c r="BS50" s="1"/>
-      <c r="BT50" s="1"/>
-      <c r="BU50" s="1"/>
-      <c r="BV50" s="1"/>
+      <c r="D50" s="72"/>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="48"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
+      <c r="S50" s="48"/>
+      <c r="T50" s="48"/>
+      <c r="U50" s="48"/>
+      <c r="V50" s="48"/>
+      <c r="W50" s="48"/>
+      <c r="X50" s="48"/>
+      <c r="Y50" s="48"/>
+      <c r="Z50" s="48"/>
+      <c r="AA50" s="48"/>
+      <c r="AB50" s="48"/>
+      <c r="AC50" s="48"/>
+      <c r="AD50" s="48"/>
+      <c r="AE50" s="48"/>
+      <c r="AF50" s="48"/>
+      <c r="AG50" s="73"/>
+      <c r="AH50" s="48"/>
+      <c r="AI50" s="48"/>
+      <c r="AJ50" s="48"/>
+      <c r="AK50" s="48"/>
+      <c r="AL50" s="48"/>
+      <c r="AM50" s="48"/>
+      <c r="AN50" s="76"/>
+      <c r="AO50" s="76"/>
+      <c r="AP50" s="76"/>
+      <c r="AQ50" s="76"/>
+      <c r="AR50" s="48"/>
+      <c r="AS50" s="48"/>
+      <c r="AT50" s="48"/>
+      <c r="AU50" s="48"/>
+      <c r="AV50" s="48"/>
+      <c r="AW50" s="77"/>
+      <c r="AX50" s="77"/>
+      <c r="AY50" s="48"/>
+      <c r="AZ50" s="48"/>
+      <c r="BA50" s="48"/>
+      <c r="BB50" s="48"/>
+      <c r="BC50" s="48"/>
+      <c r="BD50" s="48"/>
+      <c r="BE50" s="48"/>
+      <c r="BF50" s="48"/>
+      <c r="BG50" s="48"/>
+      <c r="BH50" s="48"/>
+      <c r="BI50" s="1"/>
+      <c r="BJ50" s="1"/>
+      <c r="BK50" s="53"/>
+      <c r="BL50" s="30"/>
+      <c r="BM50" s="53"/>
+      <c r="BN50" s="53"/>
+      <c r="BO50" s="22"/>
+      <c r="BP50" s="22"/>
+      <c r="BQ50" s="22"/>
+      <c r="BR50" s="22"/>
+      <c r="BS50" s="22"/>
+      <c r="BT50" s="22"/>
+      <c r="BU50" s="22"/>
+      <c r="BV50" s="22"/>
     </row>
     <row r="51" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>48</v>
@@ -5281,13 +5283,13 @@
       <c r="AO51" s="14"/>
       <c r="AP51" s="14"/>
       <c r="AQ51" s="14"/>
-      <c r="AR51" s="14"/>
-      <c r="AS51" s="14"/>
-      <c r="AT51" s="28"/>
-      <c r="AU51" s="28"/>
-      <c r="AV51" s="28"/>
-      <c r="AW51" s="49"/>
-      <c r="AX51" s="49"/>
+      <c r="AR51" s="26"/>
+      <c r="AS51" s="26"/>
+      <c r="AT51" s="26"/>
+      <c r="AU51" s="14"/>
+      <c r="AV51" s="14"/>
+      <c r="AW51" s="37"/>
+      <c r="AX51" s="37"/>
       <c r="AY51" s="14"/>
       <c r="AZ51" s="14"/>
       <c r="BA51" s="14"/>
@@ -5297,12 +5299,13 @@
       <c r="BE51" s="14"/>
       <c r="BF51" s="14"/>
       <c r="BG51" s="14"/>
-      <c r="BH51" s="69"/>
-      <c r="BJ51" s="8"/>
-      <c r="BK51" s="69"/>
-      <c r="BL51" s="69"/>
-      <c r="BM51" s="69"/>
-      <c r="BN51" s="69"/>
+      <c r="BH51" s="14"/>
+      <c r="BI51" s="1"/>
+      <c r="BJ51" s="1"/>
+      <c r="BK51" s="49"/>
+      <c r="BL51" s="8"/>
+      <c r="BM51" s="49"/>
+      <c r="BN51" s="49"/>
       <c r="BO51" s="1"/>
       <c r="BP51" s="1"/>
       <c r="BQ51" s="1"/>
@@ -5315,7 +5318,7 @@
     <row r="52" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>48</v>
@@ -5349,7 +5352,8 @@
       <c r="AD52" s="14"/>
       <c r="AE52" s="14"/>
       <c r="AF52" s="14"/>
-      <c r="AH52" s="16"/>
+      <c r="AG52" s="16"/>
+      <c r="AH52" s="14"/>
       <c r="AI52" s="14"/>
       <c r="AJ52" s="14"/>
       <c r="AK52" s="14"/>
@@ -5361,27 +5365,26 @@
       <c r="AQ52" s="14"/>
       <c r="AR52" s="14"/>
       <c r="AS52" s="14"/>
-      <c r="AT52" s="14"/>
-      <c r="AU52" s="14"/>
-      <c r="AV52" s="14"/>
-      <c r="AW52" s="28"/>
-      <c r="AX52" s="50"/>
-      <c r="AY52" s="50"/>
-      <c r="AZ52" s="50"/>
-      <c r="BA52" s="28"/>
-      <c r="BB52" s="28"/>
+      <c r="AT52" s="26"/>
+      <c r="AU52" s="26"/>
+      <c r="AV52" s="26"/>
+      <c r="AW52" s="37"/>
+      <c r="AX52" s="37"/>
+      <c r="AY52" s="14"/>
+      <c r="AZ52" s="14"/>
+      <c r="BA52" s="14"/>
+      <c r="BB52" s="14"/>
       <c r="BC52" s="14"/>
       <c r="BD52" s="14"/>
       <c r="BE52" s="14"/>
       <c r="BF52" s="14"/>
       <c r="BG52" s="14"/>
-      <c r="BH52" s="69"/>
-      <c r="BI52" s="69"/>
-      <c r="BJ52" s="69"/>
-      <c r="BK52" s="8"/>
-      <c r="BL52" s="69"/>
-      <c r="BM52" s="69"/>
-      <c r="BN52" s="69"/>
+      <c r="BH52" s="14"/>
+      <c r="BI52" s="1"/>
+      <c r="BJ52" s="1"/>
+      <c r="BK52" s="1"/>
+      <c r="BL52" s="8"/>
+      <c r="BN52" s="49"/>
       <c r="BO52" s="1"/>
       <c r="BP52" s="1"/>
       <c r="BQ52" s="1"/>
@@ -5394,7 +5397,7 @@
     <row r="53" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>48</v>
@@ -5428,7 +5431,6 @@
       <c r="AD53" s="14"/>
       <c r="AE53" s="14"/>
       <c r="AF53" s="14"/>
-      <c r="AG53" s="14"/>
       <c r="AH53" s="16"/>
       <c r="AI53" s="14"/>
       <c r="AJ53" s="14"/>
@@ -5444,24 +5446,24 @@
       <c r="AT53" s="14"/>
       <c r="AU53" s="14"/>
       <c r="AV53" s="14"/>
-      <c r="AW53" s="14"/>
-      <c r="AX53" s="14"/>
-      <c r="AY53" s="14"/>
-      <c r="AZ53" s="14"/>
-      <c r="BA53" s="14"/>
-      <c r="BB53" s="14"/>
-      <c r="BC53" s="28"/>
-      <c r="BD53" s="28"/>
-      <c r="BE53" s="28"/>
-      <c r="BF53" s="28"/>
+      <c r="AW53" s="26"/>
+      <c r="AX53" s="38"/>
+      <c r="AY53" s="38"/>
+      <c r="AZ53" s="38"/>
+      <c r="BA53" s="26"/>
+      <c r="BB53" s="26"/>
+      <c r="BC53" s="14"/>
+      <c r="BD53" s="14"/>
+      <c r="BE53" s="14"/>
+      <c r="BF53" s="14"/>
       <c r="BG53" s="14"/>
-      <c r="BH53" s="69"/>
-      <c r="BI53" s="69"/>
-      <c r="BJ53" s="69"/>
-      <c r="BK53" s="69"/>
-      <c r="BL53" s="8"/>
-      <c r="BM53" s="69"/>
-      <c r="BN53" s="69"/>
+      <c r="BH53" s="14"/>
+      <c r="BI53" s="1"/>
+      <c r="BJ53" s="1"/>
+      <c r="BK53" s="1"/>
+      <c r="BL53" s="49"/>
+      <c r="BM53" s="8"/>
+      <c r="BN53" s="1"/>
       <c r="BO53" s="1"/>
       <c r="BP53" s="1"/>
       <c r="BQ53" s="1"/>
@@ -5471,44 +5473,127 @@
       <c r="BU53" s="1"/>
       <c r="BV53" s="1"/>
     </row>
-    <row r="56" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="1" t="s">
-        <v>38</v>
-      </c>
+    <row r="54" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="15"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="14"/>
+      <c r="W54" s="14"/>
+      <c r="X54" s="14"/>
+      <c r="Y54" s="14"/>
+      <c r="Z54" s="14"/>
+      <c r="AA54" s="14"/>
+      <c r="AB54" s="14"/>
+      <c r="AC54" s="14"/>
+      <c r="AD54" s="14"/>
+      <c r="AE54" s="14"/>
+      <c r="AF54" s="14"/>
+      <c r="AG54" s="14"/>
+      <c r="AH54" s="16"/>
+      <c r="AI54" s="14"/>
+      <c r="AJ54" s="14"/>
+      <c r="AK54" s="14"/>
+      <c r="AL54" s="14"/>
+      <c r="AM54" s="14"/>
+      <c r="AN54" s="14"/>
+      <c r="AO54" s="14"/>
+      <c r="AP54" s="14"/>
+      <c r="AQ54" s="14"/>
+      <c r="AR54" s="14"/>
+      <c r="AS54" s="14"/>
+      <c r="AT54" s="14"/>
+      <c r="AU54" s="14"/>
+      <c r="AV54" s="14"/>
+      <c r="AW54" s="14"/>
+      <c r="AX54" s="14"/>
+      <c r="AY54" s="14"/>
+      <c r="AZ54" s="14"/>
+      <c r="BA54" s="14"/>
+      <c r="BB54" s="14"/>
+      <c r="BC54" s="26"/>
+      <c r="BD54" s="26"/>
+      <c r="BE54" s="26"/>
+      <c r="BF54" s="26"/>
+      <c r="BG54" s="14"/>
+      <c r="BH54" s="14"/>
+      <c r="BI54" s="49"/>
+      <c r="BJ54" s="49"/>
+      <c r="BK54" s="49"/>
+      <c r="BL54" s="49"/>
+      <c r="BM54" s="8"/>
+      <c r="BN54" s="1"/>
+      <c r="BO54" s="1"/>
+      <c r="BP54" s="1"/>
+      <c r="BQ54" s="1"/>
+      <c r="BR54" s="1"/>
+      <c r="BS54" s="1"/>
+      <c r="BT54" s="1"/>
+      <c r="BU54" s="1"/>
+      <c r="BV54" s="1"/>
     </row>
     <row r="57" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B57" s="6"/>
+        <v>34</v>
+      </c>
+      <c r="B57" s="5"/>
       <c r="C57" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="1" t="s">
+      <c r="B59" s="9"/>
+      <c r="C59" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="59" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
+    <row r="60" spans="1:74" x14ac:dyDescent="0.35">
+      <c r="A60" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B59" s="10"/>
-      <c r="C59" s="4" t="s">
+      <c r="B60" s="10"/>
+      <c r="C60" s="4" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="A19:XFD19"/>
+    <mergeCell ref="A3:XFD3"/>
+    <mergeCell ref="A49:XFD49"/>
     <mergeCell ref="BH1:BN1"/>
     <mergeCell ref="BO1:BU1"/>
     <mergeCell ref="D1:J1"/>

</xml_diff>

<commit_message>
Version 1.1 (tous les contenus et les evenements sont dynamiques) => à livrer pour première recette
</commit_message>
<xml_diff>
--- a/ALM/Planning.xlsx
+++ b/ALM/Planning.xlsx
@@ -317,6 +317,11 @@
     </fill>
     <fill>
       <patternFill patternType="gray0625">
+        <bgColor theme="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray0625">
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
@@ -353,14 +358,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -595,6 +594,21 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -675,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -708,84 +722,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="18" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="19" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -793,9 +803,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -803,11 +813,30 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1090,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BV60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BO8" sqref="BO8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="BT11" sqref="BT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="2" x14ac:dyDescent="0.35"/>
@@ -1100,102 +1129,102 @@
     <col min="2" max="2" width="37.08984375" customWidth="1"/>
     <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.36328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="60" width="3.36328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="61" max="66" width="3.36328125" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="61" width="3.36328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="62" max="66" width="3.36328125" style="56" bestFit="1" customWidth="1"/>
     <col min="67" max="74" width="3.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="65" t="s">
+      <c r="D1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="63" t="s">
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63" t="s">
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63" t="s">
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="63" t="s">
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="63"/>
-      <c r="AJ1" s="63"/>
-      <c r="AK1" s="63"/>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="66" t="s">
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
-      <c r="AQ1" s="67"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="68"/>
-      <c r="AT1" s="63" t="s">
+      <c r="AN1" s="72"/>
+      <c r="AO1" s="72"/>
+      <c r="AP1" s="72"/>
+      <c r="AQ1" s="72"/>
+      <c r="AR1" s="72"/>
+      <c r="AS1" s="73"/>
+      <c r="AT1" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="AU1" s="63"/>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="66" t="s">
+      <c r="AU1" s="68"/>
+      <c r="AV1" s="68"/>
+      <c r="AW1" s="68"/>
+      <c r="AX1" s="68"/>
+      <c r="AY1" s="68"/>
+      <c r="AZ1" s="68"/>
+      <c r="BA1" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="BB1" s="67"/>
-      <c r="BC1" s="67"/>
-      <c r="BD1" s="67"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="67"/>
-      <c r="BG1" s="68"/>
-      <c r="BH1" s="66" t="s">
+      <c r="BB1" s="72"/>
+      <c r="BC1" s="72"/>
+      <c r="BD1" s="72"/>
+      <c r="BE1" s="72"/>
+      <c r="BF1" s="72"/>
+      <c r="BG1" s="73"/>
+      <c r="BH1" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="BI1" s="67"/>
-      <c r="BJ1" s="67"/>
-      <c r="BK1" s="67"/>
-      <c r="BL1" s="67"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="68"/>
-      <c r="BO1" s="64" t="s">
+      <c r="BI1" s="92"/>
+      <c r="BJ1" s="89"/>
+      <c r="BK1" s="89"/>
+      <c r="BL1" s="89"/>
+      <c r="BM1" s="89"/>
+      <c r="BN1" s="90"/>
+      <c r="BO1" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="BP1" s="64"/>
-      <c r="BQ1" s="64"/>
-      <c r="BR1" s="64"/>
-      <c r="BS1" s="64"/>
-      <c r="BT1" s="64"/>
-      <c r="BU1" s="64"/>
+      <c r="BP1" s="69"/>
+      <c r="BQ1" s="69"/>
+      <c r="BR1" s="69"/>
+      <c r="BS1" s="69"/>
+      <c r="BT1" s="69"/>
+      <c r="BU1" s="69"/>
     </row>
     <row r="2" spans="1:74" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="11">
@@ -1369,126 +1398,126 @@
       <c r="BH2" s="11">
         <v>43451</v>
       </c>
-      <c r="BI2" s="50">
+      <c r="BI2" s="11">
         <v>43452</v>
       </c>
-      <c r="BJ2" s="50">
+      <c r="BJ2" s="55">
         <v>43453</v>
       </c>
-      <c r="BK2" s="50">
+      <c r="BK2" s="55">
         <v>43454</v>
       </c>
-      <c r="BL2" s="41">
+      <c r="BL2" s="46">
         <v>43455</v>
       </c>
-      <c r="BM2" s="41">
+      <c r="BM2" s="46">
         <v>43456</v>
       </c>
-      <c r="BN2" s="41">
+      <c r="BN2" s="46">
         <v>43457</v>
       </c>
-      <c r="BO2" s="41">
+      <c r="BO2" s="104">
         <v>43458</v>
       </c>
-      <c r="BP2" s="41">
+      <c r="BP2" s="104">
         <v>43459</v>
       </c>
-      <c r="BQ2" s="41">
+      <c r="BQ2" s="46">
         <v>43460</v>
       </c>
-      <c r="BR2" s="41">
+      <c r="BR2" s="46">
         <v>43461</v>
       </c>
-      <c r="BS2" s="41">
+      <c r="BS2" s="46">
         <v>43462</v>
       </c>
-      <c r="BT2" s="41">
+      <c r="BT2" s="46">
         <v>43463</v>
       </c>
-      <c r="BU2" s="41">
+      <c r="BU2" s="46">
         <v>43464</v>
       </c>
-      <c r="BV2" s="41">
+      <c r="BV2" s="104">
         <v>43465</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="69" t="s">
+    <row r="3" spans="1:74" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="70"/>
-      <c r="X3" s="70"/>
-      <c r="Y3" s="70"/>
-      <c r="Z3" s="70"/>
-      <c r="AA3" s="70"/>
-      <c r="AB3" s="70"/>
-      <c r="AC3" s="70"/>
-      <c r="AD3" s="70"/>
-      <c r="AE3" s="70"/>
-      <c r="AF3" s="70"/>
-      <c r="AG3" s="70"/>
-      <c r="AH3" s="70"/>
-      <c r="AI3" s="70"/>
-      <c r="AJ3" s="70"/>
-      <c r="AK3" s="70"/>
-      <c r="AL3" s="70"/>
-      <c r="AM3" s="70"/>
-      <c r="AN3" s="70"/>
-      <c r="AO3" s="70"/>
-      <c r="AP3" s="70"/>
-      <c r="AQ3" s="70"/>
-      <c r="AR3" s="70"/>
-      <c r="AS3" s="70"/>
-      <c r="AT3" s="70"/>
-      <c r="AU3" s="70"/>
-      <c r="AV3" s="70"/>
-      <c r="AW3" s="70"/>
-      <c r="AX3" s="70"/>
-      <c r="AY3" s="70"/>
-      <c r="AZ3" s="70"/>
-      <c r="BA3" s="70"/>
-      <c r="BB3" s="70"/>
-      <c r="BC3" s="70"/>
-      <c r="BD3" s="70"/>
-      <c r="BE3" s="70"/>
-      <c r="BF3" s="70"/>
-      <c r="BG3" s="70"/>
-      <c r="BH3" s="70"/>
-      <c r="BI3" s="70"/>
-      <c r="BJ3" s="70"/>
-      <c r="BK3" s="70"/>
-      <c r="BL3" s="70"/>
-      <c r="BM3" s="70"/>
-      <c r="BN3" s="70"/>
-      <c r="BO3" s="70"/>
-      <c r="BP3" s="70"/>
-      <c r="BQ3" s="70"/>
-      <c r="BR3" s="70"/>
-      <c r="BS3" s="70"/>
-      <c r="BT3" s="70"/>
-      <c r="BU3" s="70"/>
-      <c r="BV3" s="70"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="33"/>
+      <c r="Z3" s="33"/>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="33"/>
+      <c r="AE3" s="33"/>
+      <c r="AF3" s="33"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="33"/>
+      <c r="AI3" s="33"/>
+      <c r="AJ3" s="33"/>
+      <c r="AK3" s="33"/>
+      <c r="AL3" s="33"/>
+      <c r="AM3" s="33"/>
+      <c r="AN3" s="33"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="33"/>
+      <c r="AQ3" s="33"/>
+      <c r="AR3" s="33"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="33"/>
+      <c r="AU3" s="33"/>
+      <c r="AV3" s="33"/>
+      <c r="AW3" s="33"/>
+      <c r="AX3" s="33"/>
+      <c r="AY3" s="33"/>
+      <c r="AZ3" s="33"/>
+      <c r="BA3" s="33"/>
+      <c r="BB3" s="33"/>
+      <c r="BC3" s="33"/>
+      <c r="BD3" s="33"/>
+      <c r="BE3" s="33"/>
+      <c r="BF3" s="33"/>
+      <c r="BG3" s="33"/>
+      <c r="BH3" s="33"/>
+      <c r="BI3" s="34"/>
+      <c r="BJ3" s="33"/>
+      <c r="BK3" s="33"/>
+      <c r="BL3" s="33"/>
+      <c r="BM3" s="33"/>
+      <c r="BN3" s="33"/>
+      <c r="BO3" s="33"/>
+      <c r="BP3" s="33"/>
+      <c r="BQ3" s="33"/>
+      <c r="BR3" s="33"/>
+      <c r="BS3" s="33"/>
+      <c r="BT3" s="33"/>
+      <c r="BU3" s="33"/>
+      <c r="BV3" s="33"/>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
@@ -1555,12 +1584,12 @@
       <c r="BF4" s="14"/>
       <c r="BG4" s="14"/>
       <c r="BH4" s="14"/>
-      <c r="BI4" s="49"/>
-      <c r="BJ4" s="49"/>
-      <c r="BK4" s="49"/>
-      <c r="BL4" s="49"/>
-      <c r="BM4" s="49"/>
-      <c r="BN4" s="49"/>
+      <c r="BI4" s="14"/>
+      <c r="BJ4" s="54"/>
+      <c r="BK4" s="54"/>
+      <c r="BL4" s="54"/>
+      <c r="BM4" s="54"/>
+      <c r="BN4" s="54"/>
       <c r="BO4" s="1"/>
       <c r="BP4" s="1"/>
       <c r="BQ4" s="1"/>
@@ -1635,12 +1664,12 @@
       <c r="BF5" s="14"/>
       <c r="BG5" s="14"/>
       <c r="BH5" s="14"/>
-      <c r="BI5" s="49"/>
-      <c r="BJ5" s="49"/>
-      <c r="BK5" s="49"/>
-      <c r="BL5" s="49"/>
-      <c r="BM5" s="49"/>
-      <c r="BN5" s="49"/>
+      <c r="BI5" s="14"/>
+      <c r="BJ5" s="54"/>
+      <c r="BK5" s="54"/>
+      <c r="BL5" s="54"/>
+      <c r="BM5" s="54"/>
+      <c r="BN5" s="54"/>
       <c r="BO5" s="1"/>
       <c r="BP5" s="1"/>
       <c r="BQ5" s="1"/>
@@ -1715,12 +1744,12 @@
       <c r="BF6" s="14"/>
       <c r="BG6" s="14"/>
       <c r="BH6" s="14"/>
-      <c r="BI6" s="49"/>
-      <c r="BJ6" s="49"/>
-      <c r="BK6" s="49"/>
-      <c r="BL6" s="49"/>
-      <c r="BM6" s="49"/>
-      <c r="BN6" s="49"/>
+      <c r="BI6" s="14"/>
+      <c r="BJ6" s="54"/>
+      <c r="BK6" s="54"/>
+      <c r="BL6" s="54"/>
+      <c r="BM6" s="54"/>
+      <c r="BN6" s="54"/>
       <c r="BO6" s="1"/>
       <c r="BP6" s="1"/>
       <c r="BQ6" s="1"/>
@@ -1795,12 +1824,12 @@
       <c r="BF7" s="13"/>
       <c r="BG7" s="13"/>
       <c r="BH7" s="13"/>
-      <c r="BI7" s="49"/>
-      <c r="BJ7" s="49"/>
-      <c r="BK7" s="49"/>
-      <c r="BL7" s="49"/>
-      <c r="BM7" s="49"/>
-      <c r="BN7" s="49"/>
+      <c r="BI7" s="13"/>
+      <c r="BJ7" s="54"/>
+      <c r="BK7" s="54"/>
+      <c r="BL7" s="54"/>
+      <c r="BM7" s="54"/>
+      <c r="BN7" s="54"/>
       <c r="BO7" s="1"/>
       <c r="BP7" s="1"/>
       <c r="BQ7" s="1"/>
@@ -1875,12 +1904,12 @@
       <c r="BF8" s="13"/>
       <c r="BG8" s="13"/>
       <c r="BH8" s="13"/>
-      <c r="BI8" s="49"/>
-      <c r="BJ8" s="49"/>
-      <c r="BK8" s="49"/>
-      <c r="BL8" s="49"/>
-      <c r="BM8" s="49"/>
-      <c r="BN8" s="49"/>
+      <c r="BI8" s="14"/>
+      <c r="BJ8" s="54"/>
+      <c r="BK8" s="54"/>
+      <c r="BL8" s="54"/>
+      <c r="BM8" s="54"/>
+      <c r="BN8" s="54"/>
       <c r="BO8" s="1"/>
       <c r="BP8" s="1"/>
       <c r="BQ8" s="1"/>
@@ -1955,12 +1984,12 @@
       <c r="BF9" s="14"/>
       <c r="BG9" s="14"/>
       <c r="BH9" s="14"/>
-      <c r="BI9" s="49"/>
-      <c r="BJ9" s="49"/>
-      <c r="BK9" s="49"/>
-      <c r="BL9" s="49"/>
-      <c r="BM9" s="49"/>
-      <c r="BN9" s="49"/>
+      <c r="BI9" s="14"/>
+      <c r="BJ9" s="54"/>
+      <c r="BK9" s="54"/>
+      <c r="BL9" s="54"/>
+      <c r="BM9" s="54"/>
+      <c r="BN9" s="54"/>
       <c r="BO9" s="1"/>
       <c r="BP9" s="1"/>
       <c r="BQ9" s="1"/>
@@ -2035,12 +2064,12 @@
       <c r="BF10" s="14"/>
       <c r="BG10" s="14"/>
       <c r="BH10" s="14"/>
-      <c r="BI10" s="49"/>
-      <c r="BJ10" s="49"/>
-      <c r="BK10" s="49"/>
-      <c r="BL10" s="49"/>
-      <c r="BM10" s="49"/>
-      <c r="BN10" s="49"/>
+      <c r="BI10" s="14"/>
+      <c r="BJ10" s="54"/>
+      <c r="BK10" s="54"/>
+      <c r="BL10" s="54"/>
+      <c r="BM10" s="54"/>
+      <c r="BN10" s="54"/>
       <c r="BO10" s="1"/>
       <c r="BP10" s="1"/>
       <c r="BQ10" s="1"/>
@@ -2115,12 +2144,12 @@
       <c r="BF11" s="14"/>
       <c r="BG11" s="14"/>
       <c r="BH11" s="14"/>
-      <c r="BI11" s="49"/>
-      <c r="BJ11" s="49"/>
-      <c r="BK11" s="49"/>
-      <c r="BL11" s="49"/>
-      <c r="BM11" s="49"/>
-      <c r="BN11" s="49"/>
+      <c r="BI11" s="14"/>
+      <c r="BJ11" s="54"/>
+      <c r="BK11" s="54"/>
+      <c r="BL11" s="54"/>
+      <c r="BM11" s="54"/>
+      <c r="BN11" s="54"/>
       <c r="BO11" s="1"/>
       <c r="BP11" s="1"/>
       <c r="BQ11" s="1"/>
@@ -2195,12 +2224,12 @@
       <c r="BF12" s="14"/>
       <c r="BG12" s="14"/>
       <c r="BH12" s="14"/>
-      <c r="BI12" s="49"/>
-      <c r="BJ12" s="49"/>
-      <c r="BK12" s="49"/>
-      <c r="BL12" s="49"/>
-      <c r="BM12" s="49"/>
-      <c r="BN12" s="49"/>
+      <c r="BI12" s="14"/>
+      <c r="BJ12" s="54"/>
+      <c r="BK12" s="54"/>
+      <c r="BL12" s="54"/>
+      <c r="BM12" s="54"/>
+      <c r="BN12" s="54"/>
       <c r="BO12" s="1"/>
       <c r="BP12" s="1"/>
       <c r="BQ12" s="1"/>
@@ -2275,12 +2304,12 @@
       <c r="BF13" s="14"/>
       <c r="BG13" s="14"/>
       <c r="BH13" s="14"/>
-      <c r="BI13" s="49"/>
-      <c r="BJ13" s="49"/>
-      <c r="BK13" s="49"/>
-      <c r="BL13" s="49"/>
-      <c r="BM13" s="49"/>
-      <c r="BN13" s="49"/>
+      <c r="BI13" s="14"/>
+      <c r="BJ13" s="54"/>
+      <c r="BK13" s="54"/>
+      <c r="BL13" s="54"/>
+      <c r="BM13" s="54"/>
+      <c r="BN13" s="54"/>
       <c r="BO13" s="1"/>
       <c r="BP13" s="1"/>
       <c r="BQ13" s="1"/>
@@ -2353,12 +2382,12 @@
       <c r="BF14" s="14"/>
       <c r="BG14" s="14"/>
       <c r="BH14" s="14"/>
-      <c r="BI14" s="49"/>
-      <c r="BJ14" s="49"/>
-      <c r="BK14" s="49"/>
-      <c r="BL14" s="49"/>
-      <c r="BM14" s="49"/>
-      <c r="BN14" s="49"/>
+      <c r="BI14" s="14"/>
+      <c r="BJ14" s="54"/>
+      <c r="BK14" s="54"/>
+      <c r="BL14" s="54"/>
+      <c r="BM14" s="54"/>
+      <c r="BN14" s="54"/>
       <c r="BO14" s="1"/>
       <c r="BP14" s="1"/>
       <c r="BQ14" s="1"/>
@@ -2433,12 +2462,12 @@
       <c r="BF15" s="14"/>
       <c r="BG15" s="14"/>
       <c r="BH15" s="14"/>
-      <c r="BI15" s="49"/>
-      <c r="BJ15" s="49"/>
-      <c r="BK15" s="49"/>
-      <c r="BL15" s="49"/>
-      <c r="BM15" s="49"/>
-      <c r="BN15" s="49"/>
+      <c r="BI15" s="14"/>
+      <c r="BJ15" s="54"/>
+      <c r="BK15" s="54"/>
+      <c r="BL15" s="54"/>
+      <c r="BM15" s="54"/>
+      <c r="BN15" s="54"/>
       <c r="BO15" s="1"/>
       <c r="BP15" s="1"/>
       <c r="BQ15" s="1"/>
@@ -2513,12 +2542,12 @@
       <c r="BF16" s="14"/>
       <c r="BG16" s="14"/>
       <c r="BH16" s="14"/>
-      <c r="BI16" s="49"/>
-      <c r="BJ16" s="49"/>
-      <c r="BK16" s="49"/>
-      <c r="BL16" s="49"/>
-      <c r="BM16" s="49"/>
-      <c r="BN16" s="49"/>
+      <c r="BI16" s="14"/>
+      <c r="BJ16" s="54"/>
+      <c r="BK16" s="54"/>
+      <c r="BL16" s="54"/>
+      <c r="BM16" s="54"/>
+      <c r="BN16" s="54"/>
       <c r="BO16" s="1"/>
       <c r="BP16" s="1"/>
       <c r="BQ16" s="1"/>
@@ -2593,12 +2622,12 @@
       <c r="BF17" s="14"/>
       <c r="BG17" s="14"/>
       <c r="BH17" s="14"/>
-      <c r="BI17" s="49"/>
-      <c r="BJ17" s="49"/>
-      <c r="BK17" s="49"/>
-      <c r="BL17" s="49"/>
-      <c r="BM17" s="49"/>
-      <c r="BN17" s="49"/>
+      <c r="BI17" s="14"/>
+      <c r="BJ17" s="54"/>
+      <c r="BK17" s="54"/>
+      <c r="BL17" s="54"/>
+      <c r="BM17" s="54"/>
+      <c r="BN17" s="54"/>
       <c r="BO17" s="1"/>
       <c r="BP17" s="1"/>
       <c r="BQ17" s="1"/>
@@ -2609,7 +2638,7 @@
       <c r="BV17" s="1"/>
     </row>
     <row r="18" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A18" s="83"/>
+      <c r="A18" s="86"/>
       <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
@@ -2673,12 +2702,12 @@
       <c r="BF18" s="14"/>
       <c r="BG18" s="14"/>
       <c r="BH18" s="14"/>
-      <c r="BI18" s="85"/>
-      <c r="BJ18" s="49"/>
-      <c r="BK18" s="49"/>
-      <c r="BL18" s="49"/>
-      <c r="BM18" s="49"/>
-      <c r="BN18" s="49"/>
+      <c r="BI18" s="13"/>
+      <c r="BJ18" s="54"/>
+      <c r="BK18" s="54"/>
+      <c r="BL18" s="54"/>
+      <c r="BM18" s="54"/>
+      <c r="BN18" s="54"/>
       <c r="BO18" s="1"/>
       <c r="BP18" s="1"/>
       <c r="BQ18" s="1"/>
@@ -2688,160 +2717,160 @@
       <c r="BU18" s="1"/>
       <c r="BV18" s="1"/>
     </row>
-    <row r="19" spans="1:74" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="69" t="s">
+    <row r="19" spans="1:74" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="70"/>
-      <c r="O19" s="70"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="70"/>
-      <c r="R19" s="70"/>
-      <c r="S19" s="70"/>
-      <c r="T19" s="70"/>
-      <c r="U19" s="70"/>
-      <c r="V19" s="70"/>
-      <c r="W19" s="70"/>
-      <c r="X19" s="70"/>
-      <c r="Y19" s="70"/>
-      <c r="Z19" s="70"/>
-      <c r="AA19" s="70"/>
-      <c r="AB19" s="70"/>
-      <c r="AC19" s="70"/>
-      <c r="AD19" s="70"/>
-      <c r="AE19" s="70"/>
-      <c r="AF19" s="70"/>
-      <c r="AG19" s="70"/>
-      <c r="AH19" s="70"/>
-      <c r="AI19" s="70"/>
-      <c r="AJ19" s="70"/>
-      <c r="AK19" s="70"/>
-      <c r="AL19" s="70"/>
-      <c r="AM19" s="70"/>
-      <c r="AN19" s="70"/>
-      <c r="AO19" s="70"/>
-      <c r="AP19" s="70"/>
-      <c r="AQ19" s="70"/>
-      <c r="AR19" s="70"/>
-      <c r="AS19" s="70"/>
-      <c r="AT19" s="70"/>
-      <c r="AU19" s="70"/>
-      <c r="AV19" s="70"/>
-      <c r="AW19" s="70"/>
-      <c r="AX19" s="70"/>
-      <c r="AY19" s="70"/>
-      <c r="AZ19" s="70"/>
-      <c r="BA19" s="70"/>
-      <c r="BB19" s="70"/>
-      <c r="BC19" s="70"/>
-      <c r="BD19" s="70"/>
-      <c r="BE19" s="70"/>
-      <c r="BF19" s="70"/>
-      <c r="BG19" s="70"/>
-      <c r="BH19" s="70"/>
-      <c r="BI19" s="70"/>
-      <c r="BJ19" s="70"/>
-      <c r="BK19" s="70"/>
-      <c r="BL19" s="70"/>
-      <c r="BM19" s="70"/>
-      <c r="BN19" s="70"/>
-      <c r="BO19" s="70"/>
-      <c r="BP19" s="70"/>
-      <c r="BQ19" s="70"/>
-      <c r="BR19" s="70"/>
-      <c r="BS19" s="70"/>
-      <c r="BT19" s="70"/>
-      <c r="BU19" s="70"/>
-      <c r="BV19" s="70"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
+      <c r="Z19" s="33"/>
+      <c r="AA19" s="33"/>
+      <c r="AB19" s="33"/>
+      <c r="AC19" s="33"/>
+      <c r="AD19" s="33"/>
+      <c r="AE19" s="33"/>
+      <c r="AF19" s="33"/>
+      <c r="AG19" s="33"/>
+      <c r="AH19" s="33"/>
+      <c r="AI19" s="33"/>
+      <c r="AJ19" s="33"/>
+      <c r="AK19" s="33"/>
+      <c r="AL19" s="33"/>
+      <c r="AM19" s="33"/>
+      <c r="AN19" s="33"/>
+      <c r="AO19" s="33"/>
+      <c r="AP19" s="33"/>
+      <c r="AQ19" s="33"/>
+      <c r="AR19" s="33"/>
+      <c r="AS19" s="33"/>
+      <c r="AT19" s="33"/>
+      <c r="AU19" s="33"/>
+      <c r="AV19" s="33"/>
+      <c r="AW19" s="33"/>
+      <c r="AX19" s="33"/>
+      <c r="AY19" s="33"/>
+      <c r="AZ19" s="33"/>
+      <c r="BA19" s="33"/>
+      <c r="BB19" s="33"/>
+      <c r="BC19" s="33"/>
+      <c r="BD19" s="33"/>
+      <c r="BE19" s="33"/>
+      <c r="BF19" s="33"/>
+      <c r="BG19" s="33"/>
+      <c r="BH19" s="33"/>
+      <c r="BI19" s="34"/>
+      <c r="BJ19" s="33"/>
+      <c r="BK19" s="33"/>
+      <c r="BL19" s="33"/>
+      <c r="BM19" s="33"/>
+      <c r="BN19" s="33"/>
+      <c r="BO19" s="33"/>
+      <c r="BP19" s="33"/>
+      <c r="BQ19" s="33"/>
+      <c r="BR19" s="33"/>
+      <c r="BS19" s="33"/>
+      <c r="BT19" s="33"/>
+      <c r="BU19" s="33"/>
+      <c r="BV19" s="33"/>
     </row>
     <row r="20" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="48"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="48"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="48"/>
-      <c r="S20" s="73"/>
-      <c r="T20" s="73"/>
-      <c r="U20" s="73"/>
-      <c r="V20" s="73"/>
-      <c r="W20" s="73"/>
-      <c r="X20" s="73"/>
-      <c r="Y20" s="48"/>
-      <c r="Z20" s="48"/>
-      <c r="AA20" s="48"/>
-      <c r="AB20" s="48"/>
-      <c r="AC20" s="48"/>
-      <c r="AD20" s="48"/>
-      <c r="AE20" s="48"/>
-      <c r="AF20" s="48"/>
-      <c r="AG20" s="48"/>
-      <c r="AH20" s="48"/>
-      <c r="AI20" s="48"/>
-      <c r="AJ20" s="48"/>
-      <c r="AK20" s="48"/>
-      <c r="AL20" s="48"/>
-      <c r="AM20" s="48"/>
-      <c r="AN20" s="48"/>
-      <c r="AO20" s="48"/>
-      <c r="AP20" s="48"/>
-      <c r="AQ20" s="48"/>
-      <c r="AR20" s="48"/>
-      <c r="AS20" s="48"/>
-      <c r="AT20" s="48"/>
-      <c r="AU20" s="48"/>
-      <c r="AV20" s="48"/>
-      <c r="AW20" s="48"/>
-      <c r="AX20" s="48"/>
-      <c r="AY20" s="48"/>
-      <c r="AZ20" s="48"/>
-      <c r="BA20" s="74"/>
-      <c r="BB20" s="48"/>
-      <c r="BC20" s="48"/>
-      <c r="BD20" s="48"/>
-      <c r="BE20" s="48"/>
-      <c r="BF20" s="74"/>
-      <c r="BG20" s="75"/>
+      <c r="D20" s="74"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="75"/>
+      <c r="T20" s="75"/>
+      <c r="U20" s="75"/>
+      <c r="V20" s="75"/>
+      <c r="W20" s="75"/>
+      <c r="X20" s="75"/>
+      <c r="Y20" s="53"/>
+      <c r="Z20" s="53"/>
+      <c r="AA20" s="53"/>
+      <c r="AB20" s="53"/>
+      <c r="AC20" s="53"/>
+      <c r="AD20" s="53"/>
+      <c r="AE20" s="53"/>
+      <c r="AF20" s="53"/>
+      <c r="AG20" s="53"/>
+      <c r="AH20" s="53"/>
+      <c r="AI20" s="53"/>
+      <c r="AJ20" s="53"/>
+      <c r="AK20" s="53"/>
+      <c r="AL20" s="53"/>
+      <c r="AM20" s="53"/>
+      <c r="AN20" s="53"/>
+      <c r="AO20" s="53"/>
+      <c r="AP20" s="53"/>
+      <c r="AQ20" s="53"/>
+      <c r="AR20" s="53"/>
+      <c r="AS20" s="53"/>
+      <c r="AT20" s="53"/>
+      <c r="AU20" s="53"/>
+      <c r="AV20" s="53"/>
+      <c r="AW20" s="53"/>
+      <c r="AX20" s="53"/>
+      <c r="AY20" s="53"/>
+      <c r="AZ20" s="53"/>
+      <c r="BA20" s="76"/>
+      <c r="BB20" s="53"/>
+      <c r="BC20" s="53"/>
+      <c r="BD20" s="53"/>
+      <c r="BE20" s="53"/>
+      <c r="BF20" s="76"/>
+      <c r="BG20" s="77"/>
       <c r="BI20" s="53"/>
-      <c r="BJ20" s="53"/>
-      <c r="BK20" s="53"/>
-      <c r="BM20" s="30"/>
-      <c r="BO20" s="22"/>
-      <c r="BP20" s="22"/>
-      <c r="BQ20" s="22"/>
-      <c r="BR20" s="22"/>
-      <c r="BS20" s="22"/>
-      <c r="BT20" s="22"/>
-      <c r="BU20" s="22"/>
-      <c r="BV20" s="22"/>
+      <c r="BJ20" s="58"/>
+      <c r="BK20" s="58"/>
+      <c r="BM20" s="36"/>
+      <c r="BO20" s="23"/>
+      <c r="BP20" s="23"/>
+      <c r="BQ20" s="23"/>
+      <c r="BR20" s="23"/>
+      <c r="BS20" s="23"/>
+      <c r="BT20" s="23"/>
+      <c r="BU20" s="23"/>
+      <c r="BV20" s="23"/>
     </row>
     <row r="21" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
@@ -2900,20 +2929,20 @@
       <c r="AX21" s="14"/>
       <c r="AY21" s="14"/>
       <c r="AZ21" s="14"/>
-      <c r="BA21" s="39"/>
+      <c r="BA21" s="44"/>
       <c r="BB21" s="14"/>
       <c r="BC21" s="14"/>
       <c r="BD21" s="14"/>
       <c r="BE21" s="14"/>
-      <c r="BF21" s="39"/>
-      <c r="BG21" s="43"/>
+      <c r="BF21" s="44"/>
+      <c r="BG21" s="48"/>
       <c r="BH21" s="14"/>
-      <c r="BI21" s="49"/>
-      <c r="BJ21" s="49"/>
-      <c r="BK21" s="49"/>
-      <c r="BL21" s="49"/>
-      <c r="BM21" s="49"/>
-      <c r="BN21" s="49"/>
+      <c r="BI21" s="14"/>
+      <c r="BJ21" s="54"/>
+      <c r="BK21" s="54"/>
+      <c r="BL21" s="54"/>
+      <c r="BM21" s="54"/>
+      <c r="BN21" s="54"/>
       <c r="BO21" s="1"/>
       <c r="BP21" s="1"/>
       <c r="BQ21" s="1"/>
@@ -2980,20 +3009,20 @@
       <c r="AX22" s="14"/>
       <c r="AY22" s="14"/>
       <c r="AZ22" s="14"/>
-      <c r="BA22" s="39"/>
+      <c r="BA22" s="44"/>
       <c r="BB22" s="14"/>
       <c r="BC22" s="14"/>
       <c r="BD22" s="14"/>
       <c r="BE22" s="14"/>
-      <c r="BF22" s="39"/>
-      <c r="BG22" s="43"/>
+      <c r="BF22" s="44"/>
+      <c r="BG22" s="48"/>
       <c r="BH22" s="14"/>
-      <c r="BI22" s="49"/>
-      <c r="BJ22" s="49"/>
-      <c r="BK22" s="49"/>
-      <c r="BL22" s="49"/>
-      <c r="BM22" s="49"/>
-      <c r="BN22" s="49"/>
+      <c r="BI22" s="14"/>
+      <c r="BJ22" s="54"/>
+      <c r="BK22" s="54"/>
+      <c r="BL22" s="54"/>
+      <c r="BM22" s="54"/>
+      <c r="BN22" s="54"/>
       <c r="BO22" s="1"/>
       <c r="BP22" s="1"/>
       <c r="BQ22" s="1"/>
@@ -3060,20 +3089,20 @@
       <c r="AX23" s="14"/>
       <c r="AY23" s="14"/>
       <c r="AZ23" s="14"/>
-      <c r="BA23" s="39"/>
+      <c r="BA23" s="44"/>
       <c r="BB23" s="14"/>
       <c r="BC23" s="14"/>
       <c r="BD23" s="14"/>
       <c r="BE23" s="14"/>
-      <c r="BF23" s="39"/>
-      <c r="BG23" s="44"/>
+      <c r="BF23" s="44"/>
+      <c r="BG23" s="49"/>
       <c r="BH23" s="14"/>
-      <c r="BI23" s="49"/>
-      <c r="BJ23" s="49"/>
-      <c r="BK23" s="49"/>
-      <c r="BL23" s="49"/>
-      <c r="BM23" s="49"/>
-      <c r="BN23" s="49"/>
+      <c r="BI23" s="14"/>
+      <c r="BJ23" s="54"/>
+      <c r="BK23" s="54"/>
+      <c r="BL23" s="54"/>
+      <c r="BM23" s="54"/>
+      <c r="BN23" s="54"/>
       <c r="BO23" s="1"/>
       <c r="BP23" s="1"/>
       <c r="BQ23" s="1"/>
@@ -3140,20 +3169,20 @@
       <c r="AX24" s="14"/>
       <c r="AY24" s="14"/>
       <c r="AZ24" s="14"/>
-      <c r="BA24" s="39"/>
+      <c r="BA24" s="44"/>
       <c r="BB24" s="14"/>
       <c r="BC24" s="14"/>
       <c r="BD24" s="14"/>
       <c r="BE24" s="14"/>
-      <c r="BF24" s="39"/>
-      <c r="BG24" s="44"/>
+      <c r="BF24" s="44"/>
+      <c r="BG24" s="49"/>
       <c r="BH24" s="14"/>
-      <c r="BI24" s="49"/>
-      <c r="BJ24" s="49"/>
-      <c r="BK24" s="49"/>
-      <c r="BL24" s="49"/>
-      <c r="BM24" s="49"/>
-      <c r="BN24" s="49"/>
+      <c r="BI24" s="14"/>
+      <c r="BJ24" s="54"/>
+      <c r="BK24" s="54"/>
+      <c r="BL24" s="54"/>
+      <c r="BM24" s="54"/>
+      <c r="BN24" s="54"/>
       <c r="BO24" s="1"/>
       <c r="BP24" s="1"/>
       <c r="BQ24" s="1"/>
@@ -3220,25 +3249,25 @@
       <c r="AX25" s="14"/>
       <c r="AY25" s="14"/>
       <c r="AZ25" s="14"/>
-      <c r="BA25" s="39"/>
+      <c r="BA25" s="44"/>
       <c r="BB25" s="14"/>
       <c r="BC25" s="14"/>
       <c r="BD25" s="14"/>
       <c r="BE25" s="14"/>
-      <c r="BF25" s="39"/>
-      <c r="BG25" s="43"/>
+      <c r="BF25" s="44"/>
+      <c r="BG25" s="48"/>
       <c r="BH25" s="14"/>
-      <c r="BI25" s="49"/>
-      <c r="BJ25" s="49"/>
-      <c r="BK25" s="49"/>
-      <c r="BL25" s="49"/>
-      <c r="BM25" s="49"/>
-      <c r="BN25" s="49"/>
-      <c r="BO25" s="49"/>
-      <c r="BP25" s="49"/>
-      <c r="BQ25" s="49"/>
-      <c r="BR25" s="49"/>
-      <c r="BS25" s="49"/>
+      <c r="BI25" s="14"/>
+      <c r="BJ25" s="54"/>
+      <c r="BK25" s="54"/>
+      <c r="BL25" s="54"/>
+      <c r="BM25" s="54"/>
+      <c r="BN25" s="54"/>
+      <c r="BO25" s="54"/>
+      <c r="BP25" s="54"/>
+      <c r="BQ25" s="54"/>
+      <c r="BR25" s="54"/>
+      <c r="BS25" s="54"/>
       <c r="BT25" s="1"/>
       <c r="BU25" s="1"/>
       <c r="BV25" s="1"/>
@@ -3300,25 +3329,25 @@
       <c r="AX26" s="14"/>
       <c r="AY26" s="14"/>
       <c r="AZ26" s="14"/>
-      <c r="BA26" s="39"/>
+      <c r="BA26" s="44"/>
       <c r="BB26" s="14"/>
       <c r="BC26" s="14"/>
       <c r="BD26" s="14"/>
       <c r="BE26" s="14"/>
-      <c r="BF26" s="39"/>
-      <c r="BG26" s="45"/>
+      <c r="BF26" s="44"/>
+      <c r="BG26" s="50"/>
       <c r="BH26" s="14"/>
-      <c r="BI26" s="49"/>
-      <c r="BJ26" s="49"/>
-      <c r="BK26" s="49"/>
-      <c r="BL26" s="49"/>
-      <c r="BM26" s="49"/>
-      <c r="BN26" s="49"/>
-      <c r="BO26" s="49"/>
-      <c r="BP26" s="49"/>
-      <c r="BQ26" s="49"/>
-      <c r="BR26" s="49"/>
-      <c r="BS26" s="49"/>
+      <c r="BI26" s="14"/>
+      <c r="BJ26" s="54"/>
+      <c r="BK26" s="54"/>
+      <c r="BL26" s="54"/>
+      <c r="BM26" s="54"/>
+      <c r="BN26" s="54"/>
+      <c r="BO26" s="54"/>
+      <c r="BP26" s="54"/>
+      <c r="BQ26" s="54"/>
+      <c r="BR26" s="54"/>
+      <c r="BS26" s="54"/>
       <c r="BT26" s="1"/>
       <c r="BU26" s="1"/>
       <c r="BV26" s="1"/>
@@ -3380,25 +3409,25 @@
       <c r="AX27" s="14"/>
       <c r="AY27" s="14"/>
       <c r="AZ27" s="14"/>
-      <c r="BA27" s="39"/>
+      <c r="BA27" s="44"/>
       <c r="BB27" s="14"/>
       <c r="BC27" s="14"/>
       <c r="BD27" s="14"/>
-      <c r="BE27" s="48"/>
-      <c r="BF27" s="46"/>
+      <c r="BE27" s="53"/>
+      <c r="BF27" s="51"/>
       <c r="BG27" s="14"/>
-      <c r="BH27" s="26"/>
-      <c r="BI27" s="49"/>
-      <c r="BJ27" s="49"/>
-      <c r="BK27" s="49"/>
-      <c r="BL27" s="49"/>
-      <c r="BM27" s="49"/>
-      <c r="BN27" s="49"/>
-      <c r="BO27" s="8"/>
-      <c r="BP27" s="49"/>
-      <c r="BQ27" s="49"/>
-      <c r="BR27" s="49"/>
-      <c r="BS27" s="49"/>
+      <c r="BH27" s="28"/>
+      <c r="BI27" s="14"/>
+      <c r="BJ27" s="54"/>
+      <c r="BK27" s="54"/>
+      <c r="BL27" s="54"/>
+      <c r="BM27" s="54"/>
+      <c r="BN27" s="8"/>
+      <c r="BO27" s="1"/>
+      <c r="BP27" s="54"/>
+      <c r="BQ27" s="54"/>
+      <c r="BR27" s="54"/>
+      <c r="BS27" s="54"/>
       <c r="BT27" s="1"/>
       <c r="BU27" s="1"/>
       <c r="BV27" s="1"/>
@@ -3459,25 +3488,25 @@
       <c r="AX28" s="14"/>
       <c r="AY28" s="14"/>
       <c r="AZ28" s="14"/>
-      <c r="BA28" s="39"/>
+      <c r="BA28" s="44"/>
       <c r="BB28" s="14"/>
       <c r="BC28" s="14"/>
       <c r="BD28" s="14"/>
       <c r="BE28" s="14"/>
-      <c r="BF28" s="42"/>
+      <c r="BF28" s="47"/>
       <c r="BG28" s="14"/>
-      <c r="BH28" s="26"/>
-      <c r="BI28" s="49"/>
-      <c r="BJ28" s="49"/>
-      <c r="BK28" s="49"/>
-      <c r="BL28" s="49"/>
-      <c r="BM28" s="58"/>
-      <c r="BN28" s="49"/>
-      <c r="BO28" s="8"/>
-      <c r="BP28" s="49"/>
-      <c r="BQ28" s="49"/>
-      <c r="BR28" s="49"/>
-      <c r="BS28" s="49"/>
+      <c r="BH28" s="28"/>
+      <c r="BI28" s="14"/>
+      <c r="BJ28" s="54"/>
+      <c r="BK28" s="54"/>
+      <c r="BL28" s="54"/>
+      <c r="BM28" s="54"/>
+      <c r="BN28" s="8"/>
+      <c r="BO28" s="1"/>
+      <c r="BP28" s="54"/>
+      <c r="BQ28" s="54"/>
+      <c r="BR28" s="54"/>
+      <c r="BS28" s="54"/>
       <c r="BT28" s="1"/>
       <c r="BU28" s="1"/>
       <c r="BV28" s="1"/>
@@ -3538,25 +3567,25 @@
       <c r="AX29" s="14"/>
       <c r="AY29" s="14"/>
       <c r="AZ29" s="14"/>
-      <c r="BA29" s="39"/>
+      <c r="BA29" s="44"/>
       <c r="BB29" s="14"/>
       <c r="BC29" s="14"/>
       <c r="BD29" s="14"/>
       <c r="BE29" s="14"/>
-      <c r="BF29" s="42"/>
+      <c r="BF29" s="47"/>
       <c r="BG29" s="14"/>
-      <c r="BH29" s="26"/>
-      <c r="BI29" s="49"/>
-      <c r="BJ29" s="49"/>
-      <c r="BK29" s="49"/>
-      <c r="BL29" s="49"/>
-      <c r="BM29" s="58"/>
-      <c r="BN29" s="49"/>
-      <c r="BO29" s="8"/>
-      <c r="BP29" s="49"/>
-      <c r="BQ29" s="49"/>
-      <c r="BR29" s="49"/>
-      <c r="BS29" s="49"/>
+      <c r="BH29" s="28"/>
+      <c r="BI29" s="14"/>
+      <c r="BJ29" s="54"/>
+      <c r="BK29" s="54"/>
+      <c r="BL29" s="54"/>
+      <c r="BM29" s="54"/>
+      <c r="BN29" s="8"/>
+      <c r="BO29" s="1"/>
+      <c r="BP29" s="54"/>
+      <c r="BQ29" s="54"/>
+      <c r="BR29" s="54"/>
+      <c r="BS29" s="54"/>
       <c r="BT29" s="1"/>
       <c r="BU29" s="1"/>
       <c r="BV29" s="1"/>
@@ -3618,25 +3647,25 @@
       <c r="AX30" s="14"/>
       <c r="AY30" s="14"/>
       <c r="AZ30" s="14"/>
-      <c r="BA30" s="39"/>
+      <c r="BA30" s="44"/>
       <c r="BB30" s="14"/>
       <c r="BC30" s="14"/>
       <c r="BD30" s="14"/>
       <c r="BE30" s="14"/>
-      <c r="BF30" s="42"/>
+      <c r="BF30" s="47"/>
       <c r="BG30" s="14"/>
-      <c r="BH30" s="26"/>
-      <c r="BI30" s="49"/>
-      <c r="BJ30" s="49"/>
-      <c r="BK30" s="49"/>
-      <c r="BL30" s="49"/>
-      <c r="BM30" s="58"/>
-      <c r="BN30" s="49"/>
-      <c r="BO30" s="8"/>
+      <c r="BH30" s="28"/>
+      <c r="BI30" s="14"/>
+      <c r="BJ30" s="54"/>
+      <c r="BK30" s="54"/>
+      <c r="BL30" s="54"/>
+      <c r="BM30" s="54"/>
+      <c r="BN30" s="8"/>
+      <c r="BO30" s="1"/>
       <c r="BP30" s="1"/>
-      <c r="BQ30" s="49"/>
-      <c r="BR30" s="49"/>
-      <c r="BS30" s="49"/>
+      <c r="BQ30" s="54"/>
+      <c r="BR30" s="54"/>
+      <c r="BS30" s="54"/>
       <c r="BT30" s="1"/>
       <c r="BU30" s="1"/>
       <c r="BV30" s="1"/>
@@ -3698,25 +3727,25 @@
       <c r="AX31" s="14"/>
       <c r="AY31" s="14"/>
       <c r="AZ31" s="14"/>
-      <c r="BA31" s="39"/>
+      <c r="BA31" s="44"/>
       <c r="BB31" s="14"/>
       <c r="BC31" s="14"/>
       <c r="BD31" s="14"/>
       <c r="BE31" s="14"/>
-      <c r="BF31" s="42"/>
+      <c r="BF31" s="47"/>
       <c r="BG31" s="14"/>
-      <c r="BH31" s="26"/>
-      <c r="BI31" s="49"/>
-      <c r="BJ31" s="49"/>
-      <c r="BK31" s="49"/>
-      <c r="BL31" s="49"/>
-      <c r="BM31" s="60"/>
-      <c r="BN31" s="52"/>
-      <c r="BO31" s="8"/>
+      <c r="BH31" s="28"/>
+      <c r="BI31" s="14"/>
+      <c r="BJ31" s="54"/>
+      <c r="BK31" s="54"/>
+      <c r="BL31" s="54"/>
+      <c r="BM31" s="57"/>
+      <c r="BN31" s="27"/>
+      <c r="BO31" s="22"/>
       <c r="BP31" s="1"/>
-      <c r="BQ31" s="49"/>
-      <c r="BR31" s="49"/>
-      <c r="BS31" s="49"/>
+      <c r="BQ31" s="54"/>
+      <c r="BR31" s="57"/>
+      <c r="BS31" s="57"/>
       <c r="BT31" s="1"/>
       <c r="BU31" s="1"/>
       <c r="BV31" s="1"/>
@@ -3786,18 +3815,18 @@
       <c r="BF32" s="14"/>
       <c r="BG32" s="14"/>
       <c r="BH32" s="14"/>
-      <c r="BI32" s="49"/>
-      <c r="BJ32" s="53"/>
-      <c r="BK32" s="49"/>
-      <c r="BL32" s="59"/>
-      <c r="BM32" s="27"/>
-      <c r="BN32" s="29"/>
-      <c r="BO32" s="28"/>
-      <c r="BP32" s="22"/>
-      <c r="BQ32" s="30"/>
-      <c r="BR32" s="22"/>
-      <c r="BS32" s="1"/>
-      <c r="BT32" s="1"/>
+      <c r="BI32" s="14"/>
+      <c r="BJ32" s="58"/>
+      <c r="BK32" s="54"/>
+      <c r="BL32" s="64"/>
+      <c r="BM32" s="29"/>
+      <c r="BN32" s="31"/>
+      <c r="BO32" s="30"/>
+      <c r="BP32" s="54"/>
+      <c r="BQ32" s="86"/>
+      <c r="BR32" s="95"/>
+      <c r="BS32" s="96"/>
+      <c r="BT32" s="21"/>
       <c r="BU32" s="1"/>
       <c r="BV32" s="1"/>
     </row>
@@ -3865,18 +3894,18 @@
       <c r="BF33" s="14"/>
       <c r="BG33" s="14"/>
       <c r="BH33" s="14"/>
-      <c r="BI33" s="49"/>
-      <c r="BJ33" s="49"/>
-      <c r="BK33" s="49"/>
-      <c r="BL33" s="59"/>
-      <c r="BM33" s="54"/>
+      <c r="BI33" s="14"/>
+      <c r="BJ33" s="54"/>
+      <c r="BK33" s="54"/>
+      <c r="BL33" s="64"/>
+      <c r="BM33" s="59"/>
       <c r="BN33" s="7"/>
-      <c r="BO33" s="55"/>
+      <c r="BO33" s="60"/>
       <c r="BP33" s="1"/>
-      <c r="BQ33" s="8"/>
-      <c r="BR33" s="1"/>
-      <c r="BS33" s="1"/>
-      <c r="BT33" s="1"/>
+      <c r="BQ33" s="86"/>
+      <c r="BR33" s="97"/>
+      <c r="BS33" s="98"/>
+      <c r="BT33" s="21"/>
       <c r="BU33" s="1"/>
       <c r="BV33" s="1"/>
     </row>
@@ -3944,18 +3973,18 @@
       <c r="BF34" s="14"/>
       <c r="BG34" s="14"/>
       <c r="BH34" s="14"/>
-      <c r="BI34" s="49"/>
-      <c r="BJ34" s="49"/>
-      <c r="BK34" s="49"/>
-      <c r="BL34" s="59"/>
-      <c r="BM34" s="56"/>
-      <c r="BN34" s="57"/>
-      <c r="BO34" s="24"/>
-      <c r="BP34" s="21"/>
-      <c r="BQ34" s="8"/>
-      <c r="BR34" s="1"/>
-      <c r="BS34" s="1"/>
-      <c r="BT34" s="1"/>
+      <c r="BI34" s="14"/>
+      <c r="BJ34" s="54"/>
+      <c r="BK34" s="54"/>
+      <c r="BL34" s="64"/>
+      <c r="BM34" s="61"/>
+      <c r="BN34" s="62"/>
+      <c r="BO34" s="25"/>
+      <c r="BP34" s="22"/>
+      <c r="BQ34" s="100"/>
+      <c r="BR34" s="24"/>
+      <c r="BS34" s="99"/>
+      <c r="BT34" s="26"/>
       <c r="BU34" s="1"/>
       <c r="BV34" s="1"/>
     </row>
@@ -4024,19 +4053,19 @@
       <c r="BF35" s="14"/>
       <c r="BG35" s="14"/>
       <c r="BH35" s="14"/>
-      <c r="BI35" s="49"/>
-      <c r="BJ35" s="49"/>
-      <c r="BK35" s="49"/>
-      <c r="BL35" s="49"/>
-      <c r="BM35" s="53"/>
-      <c r="BN35" s="53"/>
-      <c r="BO35" s="84"/>
-      <c r="BP35" s="27"/>
-      <c r="BQ35" s="28"/>
-      <c r="BR35" s="30"/>
-      <c r="BS35" s="8"/>
-      <c r="BT35" s="1"/>
-      <c r="BU35" s="1"/>
+      <c r="BI35" s="14"/>
+      <c r="BJ35" s="54"/>
+      <c r="BK35" s="54"/>
+      <c r="BL35" s="54"/>
+      <c r="BM35" s="58"/>
+      <c r="BN35" s="58"/>
+      <c r="BO35" s="87"/>
+      <c r="BP35" s="29"/>
+      <c r="BQ35" s="30"/>
+      <c r="BR35" s="35"/>
+      <c r="BS35" s="87"/>
+      <c r="BT35" s="102"/>
+      <c r="BU35" s="21"/>
       <c r="BV35" s="1"/>
     </row>
     <row r="36" spans="1:74" ht="15" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.4">
@@ -4104,19 +4133,19 @@
       <c r="BF36" s="14"/>
       <c r="BG36" s="14"/>
       <c r="BH36" s="14"/>
-      <c r="BI36" s="49"/>
-      <c r="BJ36" s="49"/>
-      <c r="BK36" s="49"/>
-      <c r="BL36" s="49"/>
-      <c r="BM36" s="49"/>
-      <c r="BN36" s="49"/>
-      <c r="BO36" s="83"/>
-      <c r="BP36" s="23"/>
-      <c r="BQ36" s="24"/>
-      <c r="BR36" s="8"/>
-      <c r="BS36" s="8"/>
-      <c r="BT36" s="1"/>
-      <c r="BU36" s="1"/>
+      <c r="BI36" s="14"/>
+      <c r="BJ36" s="54"/>
+      <c r="BK36" s="54"/>
+      <c r="BL36" s="54"/>
+      <c r="BM36" s="54"/>
+      <c r="BN36" s="54"/>
+      <c r="BO36" s="86"/>
+      <c r="BP36" s="24"/>
+      <c r="BQ36" s="25"/>
+      <c r="BR36" s="21"/>
+      <c r="BS36" s="86"/>
+      <c r="BT36" s="103"/>
+      <c r="BU36" s="21"/>
       <c r="BV36" s="1"/>
     </row>
     <row r="37" spans="1:74" x14ac:dyDescent="0.35">
@@ -4181,29 +4210,30 @@
       <c r="BC37" s="14"/>
       <c r="BD37" s="14"/>
       <c r="BE37" s="14"/>
-      <c r="BF37" s="47"/>
+      <c r="BF37" s="52"/>
       <c r="BG37" s="14"/>
       <c r="BH37" s="14"/>
-      <c r="BI37" s="49"/>
-      <c r="BJ37" s="49"/>
-      <c r="BK37" s="60"/>
-      <c r="BL37" s="60"/>
-      <c r="BM37" s="49"/>
-      <c r="BN37" s="49"/>
+      <c r="BI37" s="14"/>
+      <c r="BJ37" s="54"/>
+      <c r="BK37" s="65"/>
+      <c r="BL37" s="65"/>
+      <c r="BM37" s="54"/>
+      <c r="BN37" s="54"/>
       <c r="BO37" s="1"/>
-      <c r="BP37" s="82"/>
-      <c r="BR37" s="33"/>
-      <c r="BS37" s="33"/>
-      <c r="BT37" s="25"/>
-      <c r="BU37" s="25"/>
-      <c r="BV37" s="21"/>
+      <c r="BP37" s="85"/>
+      <c r="BQ37" s="23"/>
+      <c r="BR37" s="84"/>
+      <c r="BS37" s="84"/>
+      <c r="BT37" s="101"/>
+      <c r="BU37" s="8"/>
+      <c r="BV37" s="22"/>
     </row>
     <row r="38" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="40" t="s">
         <v>48</v>
       </c>
       <c r="D38" s="15"/>
@@ -4262,16 +4292,16 @@
       <c r="BF38" s="14"/>
       <c r="BG38" s="14"/>
       <c r="BH38" s="14"/>
-      <c r="BI38" s="49"/>
-      <c r="BJ38" s="49"/>
-      <c r="BK38" s="49"/>
-      <c r="BL38" s="49"/>
-      <c r="BM38" s="49"/>
-      <c r="BN38" s="40"/>
-      <c r="BO38" s="34"/>
-      <c r="BP38" s="34"/>
-      <c r="BQ38" s="34"/>
-      <c r="BR38" s="34"/>
+      <c r="BI38" s="14"/>
+      <c r="BJ38" s="54"/>
+      <c r="BK38" s="54"/>
+      <c r="BL38" s="54"/>
+      <c r="BM38" s="54"/>
+      <c r="BN38" s="45"/>
+      <c r="BO38" s="39"/>
+      <c r="BP38" s="39"/>
+      <c r="BQ38" s="39"/>
+      <c r="BR38" s="39"/>
       <c r="BS38" s="4"/>
       <c r="BT38" s="4"/>
       <c r="BU38" s="4"/>
@@ -4279,10 +4309,10 @@
     </row>
     <row r="39" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="40" t="s">
         <v>48</v>
       </c>
       <c r="D39" s="15"/>
@@ -4342,12 +4372,12 @@
       <c r="BF39" s="14"/>
       <c r="BG39" s="14"/>
       <c r="BH39" s="14"/>
-      <c r="BI39" s="58"/>
-      <c r="BJ39" s="49"/>
-      <c r="BK39" s="49"/>
-      <c r="BL39" s="49"/>
-      <c r="BM39" s="49"/>
-      <c r="BN39" s="49"/>
+      <c r="BI39" s="47"/>
+      <c r="BJ39" s="54"/>
+      <c r="BK39" s="54"/>
+      <c r="BL39" s="54"/>
+      <c r="BM39" s="54"/>
+      <c r="BN39" s="54"/>
       <c r="BO39" s="4"/>
       <c r="BP39" s="4"/>
       <c r="BQ39" s="4"/>
@@ -4359,10 +4389,10 @@
     </row>
     <row r="40" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="40" t="s">
         <v>48</v>
       </c>
       <c r="D40" s="15"/>
@@ -4422,12 +4452,12 @@
       <c r="BF40" s="14"/>
       <c r="BG40" s="14"/>
       <c r="BH40" s="14"/>
-      <c r="BI40" s="58"/>
-      <c r="BJ40" s="49"/>
-      <c r="BK40" s="49"/>
-      <c r="BL40" s="49"/>
-      <c r="BM40" s="49"/>
-      <c r="BN40" s="49"/>
+      <c r="BI40" s="47"/>
+      <c r="BJ40" s="54"/>
+      <c r="BK40" s="54"/>
+      <c r="BL40" s="54"/>
+      <c r="BM40" s="54"/>
+      <c r="BN40" s="54"/>
       <c r="BO40" s="4"/>
       <c r="BP40" s="4"/>
       <c r="BQ40" s="4"/>
@@ -4439,10 +4469,10 @@
     </row>
     <row r="41" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1"/>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="40" t="s">
         <v>48</v>
       </c>
       <c r="D41" s="15"/>
@@ -4502,12 +4532,12 @@
       <c r="BF41" s="14"/>
       <c r="BG41" s="14"/>
       <c r="BH41" s="14"/>
-      <c r="BI41" s="60"/>
-      <c r="BJ41" s="52"/>
-      <c r="BK41" s="52"/>
-      <c r="BL41" s="52"/>
-      <c r="BM41" s="49"/>
-      <c r="BN41" s="49"/>
+      <c r="BI41" s="93"/>
+      <c r="BJ41" s="57"/>
+      <c r="BK41" s="57"/>
+      <c r="BL41" s="57"/>
+      <c r="BM41" s="54"/>
+      <c r="BN41" s="54"/>
       <c r="BO41" s="4"/>
       <c r="BP41" s="4"/>
       <c r="BQ41" s="4"/>
@@ -4581,21 +4611,21 @@
       <c r="BE42" s="14"/>
       <c r="BF42" s="14"/>
       <c r="BG42" s="14"/>
-      <c r="BH42" s="39"/>
-      <c r="BI42" s="59"/>
-      <c r="BJ42" s="27"/>
-      <c r="BK42" s="29"/>
-      <c r="BL42" s="28"/>
-      <c r="BM42" s="58"/>
-      <c r="BN42" s="30"/>
-      <c r="BO42" s="49"/>
-      <c r="BP42" s="22"/>
-      <c r="BQ42" s="22"/>
-      <c r="BR42" s="22"/>
-      <c r="BS42" s="22"/>
-      <c r="BT42" s="22"/>
-      <c r="BU42" s="22"/>
-      <c r="BV42" s="22"/>
+      <c r="BH42" s="44"/>
+      <c r="BI42" s="44"/>
+      <c r="BJ42" s="29"/>
+      <c r="BK42" s="31"/>
+      <c r="BL42" s="30"/>
+      <c r="BM42" s="63"/>
+      <c r="BN42" s="54"/>
+      <c r="BO42" s="1"/>
+      <c r="BP42" s="1"/>
+      <c r="BQ42" s="8"/>
+      <c r="BR42" s="23"/>
+      <c r="BS42" s="23"/>
+      <c r="BT42" s="23"/>
+      <c r="BU42" s="23"/>
+      <c r="BV42" s="23"/>
     </row>
     <row r="43" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
@@ -4661,16 +4691,16 @@
       <c r="BE43" s="14"/>
       <c r="BF43" s="14"/>
       <c r="BG43" s="14"/>
-      <c r="BH43" s="39"/>
-      <c r="BI43" s="59"/>
-      <c r="BJ43" s="61"/>
-      <c r="BK43" s="49"/>
-      <c r="BL43" s="55"/>
-      <c r="BM43" s="58"/>
-      <c r="BN43" s="8"/>
-      <c r="BO43" s="49"/>
+      <c r="BH43" s="44"/>
+      <c r="BI43" s="44"/>
+      <c r="BJ43" s="66"/>
+      <c r="BK43" s="54"/>
+      <c r="BL43" s="60"/>
+      <c r="BM43" s="63"/>
+      <c r="BN43" s="54"/>
+      <c r="BO43" s="1"/>
       <c r="BP43" s="1"/>
-      <c r="BQ43" s="1"/>
+      <c r="BQ43" s="8"/>
       <c r="BR43" s="1"/>
       <c r="BS43" s="1"/>
       <c r="BT43" s="1"/>
@@ -4741,16 +4771,16 @@
       <c r="BE44" s="14"/>
       <c r="BF44" s="14"/>
       <c r="BG44" s="14"/>
-      <c r="BH44" s="39"/>
-      <c r="BI44" s="59"/>
-      <c r="BJ44" s="54"/>
+      <c r="BH44" s="44"/>
+      <c r="BI44" s="44"/>
+      <c r="BJ44" s="59"/>
       <c r="BK44" s="7"/>
-      <c r="BL44" s="55"/>
-      <c r="BM44" s="58"/>
-      <c r="BN44" s="8"/>
-      <c r="BO44" s="49"/>
+      <c r="BL44" s="60"/>
+      <c r="BM44" s="63"/>
+      <c r="BN44" s="54"/>
+      <c r="BO44" s="1"/>
       <c r="BP44" s="1"/>
-      <c r="BQ44" s="1"/>
+      <c r="BQ44" s="8"/>
       <c r="BR44" s="1"/>
       <c r="BS44" s="1"/>
       <c r="BT44" s="1"/>
@@ -4821,16 +4851,16 @@
       <c r="BE45" s="14"/>
       <c r="BF45" s="14"/>
       <c r="BG45" s="14"/>
-      <c r="BH45" s="39"/>
-      <c r="BI45" s="59"/>
-      <c r="BJ45" s="54"/>
-      <c r="BK45" s="49"/>
-      <c r="BL45" s="31"/>
-      <c r="BM45" s="58"/>
-      <c r="BN45" s="8"/>
-      <c r="BO45" s="49"/>
+      <c r="BH45" s="44"/>
+      <c r="BI45" s="44"/>
+      <c r="BJ45" s="59"/>
+      <c r="BK45" s="54"/>
+      <c r="BL45" s="37"/>
+      <c r="BM45" s="63"/>
+      <c r="BN45" s="54"/>
+      <c r="BO45" s="1"/>
       <c r="BP45" s="1"/>
-      <c r="BQ45" s="1"/>
+      <c r="BQ45" s="8"/>
       <c r="BR45" s="1"/>
       <c r="BS45" s="1"/>
       <c r="BT45" s="1"/>
@@ -4901,16 +4931,16 @@
       <c r="BE46" s="14"/>
       <c r="BF46" s="14"/>
       <c r="BG46" s="14"/>
-      <c r="BH46" s="39"/>
-      <c r="BI46" s="59"/>
-      <c r="BJ46" s="54"/>
-      <c r="BK46" s="49"/>
-      <c r="BL46" s="31"/>
-      <c r="BM46" s="58"/>
-      <c r="BN46" s="8"/>
-      <c r="BO46" s="49"/>
+      <c r="BH46" s="44"/>
+      <c r="BI46" s="44"/>
+      <c r="BJ46" s="59"/>
+      <c r="BK46" s="54"/>
+      <c r="BL46" s="37"/>
+      <c r="BM46" s="63"/>
+      <c r="BN46" s="54"/>
+      <c r="BO46" s="1"/>
       <c r="BP46" s="1"/>
-      <c r="BQ46" s="1"/>
+      <c r="BQ46" s="8"/>
       <c r="BR46" s="1"/>
       <c r="BS46" s="1"/>
       <c r="BT46" s="1"/>
@@ -4981,16 +5011,16 @@
       <c r="BE47" s="14"/>
       <c r="BF47" s="14"/>
       <c r="BG47" s="14"/>
-      <c r="BH47" s="39"/>
-      <c r="BI47" s="59"/>
-      <c r="BJ47" s="54"/>
+      <c r="BH47" s="44"/>
+      <c r="BI47" s="44"/>
+      <c r="BJ47" s="59"/>
       <c r="BK47" s="7"/>
-      <c r="BL47" s="55"/>
-      <c r="BM47" s="58"/>
-      <c r="BN47" s="8"/>
-      <c r="BO47" s="49"/>
+      <c r="BL47" s="60"/>
+      <c r="BM47" s="63"/>
+      <c r="BN47" s="54"/>
+      <c r="BO47" s="1"/>
       <c r="BP47" s="1"/>
-      <c r="BQ47" s="1"/>
+      <c r="BQ47" s="8"/>
       <c r="BR47" s="1"/>
       <c r="BS47" s="1"/>
       <c r="BT47" s="1"/>
@@ -4998,242 +5028,242 @@
       <c r="BV47" s="1"/>
     </row>
     <row r="48" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="21"/>
-      <c r="B48" s="78" t="s">
+      <c r="A48" s="22"/>
+      <c r="B48" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="79"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
-      <c r="I48" s="47"/>
-      <c r="J48" s="47"/>
-      <c r="K48" s="47"/>
-      <c r="L48" s="47"/>
-      <c r="M48" s="47"/>
-      <c r="N48" s="47"/>
-      <c r="O48" s="47"/>
-      <c r="P48" s="47"/>
-      <c r="Q48" s="47"/>
-      <c r="R48" s="47"/>
-      <c r="S48" s="47"/>
-      <c r="T48" s="47"/>
-      <c r="U48" s="47"/>
-      <c r="V48" s="47"/>
-      <c r="W48" s="47"/>
-      <c r="X48" s="47"/>
-      <c r="Y48" s="47"/>
-      <c r="Z48" s="80"/>
-      <c r="AA48" s="47"/>
-      <c r="AB48" s="47"/>
-      <c r="AC48" s="47"/>
-      <c r="AD48" s="47"/>
-      <c r="AE48" s="47"/>
-      <c r="AF48" s="47"/>
-      <c r="AG48" s="47"/>
-      <c r="AH48" s="47"/>
-      <c r="AI48" s="47"/>
-      <c r="AJ48" s="47"/>
-      <c r="AK48" s="47"/>
-      <c r="AL48" s="47"/>
-      <c r="AM48" s="47"/>
-      <c r="AN48" s="47"/>
-      <c r="AO48" s="47"/>
-      <c r="AP48" s="47"/>
-      <c r="AQ48" s="47"/>
-      <c r="AR48" s="47"/>
-      <c r="AS48" s="47"/>
-      <c r="AT48" s="47"/>
-      <c r="AU48" s="47"/>
-      <c r="AV48" s="47"/>
-      <c r="AW48" s="47"/>
-      <c r="AX48" s="47"/>
-      <c r="AY48" s="47"/>
-      <c r="AZ48" s="47"/>
-      <c r="BA48" s="47"/>
-      <c r="BB48" s="47"/>
-      <c r="BC48" s="47"/>
-      <c r="BD48" s="47"/>
-      <c r="BE48" s="47"/>
-      <c r="BF48" s="47"/>
-      <c r="BG48" s="47"/>
-      <c r="BH48" s="81"/>
-      <c r="BI48" s="59"/>
-      <c r="BJ48" s="32"/>
-      <c r="BK48" s="57"/>
-      <c r="BL48" s="62"/>
-      <c r="BM48" s="60"/>
-      <c r="BN48" s="25"/>
-      <c r="BO48" s="52"/>
-      <c r="BP48" s="21"/>
-      <c r="BQ48" s="21"/>
-      <c r="BR48" s="21"/>
-      <c r="BS48" s="21"/>
-      <c r="BT48" s="21"/>
-      <c r="BU48" s="21"/>
-      <c r="BV48" s="21"/>
-    </row>
-    <row r="49" spans="1:74" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="69" t="s">
+      <c r="D48" s="81"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="52"/>
+      <c r="P48" s="52"/>
+      <c r="Q48" s="52"/>
+      <c r="R48" s="52"/>
+      <c r="S48" s="52"/>
+      <c r="T48" s="52"/>
+      <c r="U48" s="52"/>
+      <c r="V48" s="52"/>
+      <c r="W48" s="52"/>
+      <c r="X48" s="52"/>
+      <c r="Y48" s="52"/>
+      <c r="Z48" s="82"/>
+      <c r="AA48" s="52"/>
+      <c r="AB48" s="52"/>
+      <c r="AC48" s="52"/>
+      <c r="AD48" s="52"/>
+      <c r="AE48" s="52"/>
+      <c r="AF48" s="52"/>
+      <c r="AG48" s="52"/>
+      <c r="AH48" s="52"/>
+      <c r="AI48" s="52"/>
+      <c r="AJ48" s="52"/>
+      <c r="AK48" s="52"/>
+      <c r="AL48" s="52"/>
+      <c r="AM48" s="52"/>
+      <c r="AN48" s="52"/>
+      <c r="AO48" s="52"/>
+      <c r="AP48" s="52"/>
+      <c r="AQ48" s="52"/>
+      <c r="AR48" s="52"/>
+      <c r="AS48" s="52"/>
+      <c r="AT48" s="52"/>
+      <c r="AU48" s="52"/>
+      <c r="AV48" s="52"/>
+      <c r="AW48" s="52"/>
+      <c r="AX48" s="52"/>
+      <c r="AY48" s="52"/>
+      <c r="AZ48" s="52"/>
+      <c r="BA48" s="52"/>
+      <c r="BB48" s="52"/>
+      <c r="BC48" s="52"/>
+      <c r="BD48" s="52"/>
+      <c r="BE48" s="52"/>
+      <c r="BF48" s="52"/>
+      <c r="BG48" s="52"/>
+      <c r="BH48" s="83"/>
+      <c r="BI48" s="44"/>
+      <c r="BJ48" s="38"/>
+      <c r="BK48" s="62"/>
+      <c r="BL48" s="67"/>
+      <c r="BM48" s="63"/>
+      <c r="BN48" s="54"/>
+      <c r="BO48" s="1"/>
+      <c r="BP48" s="1"/>
+      <c r="BQ48" s="8"/>
+      <c r="BR48" s="22"/>
+      <c r="BS48" s="22"/>
+      <c r="BT48" s="22"/>
+      <c r="BU48" s="22"/>
+      <c r="BV48" s="22"/>
+    </row>
+    <row r="49" spans="1:74" s="32" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="70"/>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
-      <c r="F49" s="70"/>
-      <c r="G49" s="70"/>
-      <c r="H49" s="70"/>
-      <c r="I49" s="70"/>
-      <c r="J49" s="70"/>
-      <c r="K49" s="70"/>
-      <c r="L49" s="70"/>
-      <c r="M49" s="70"/>
-      <c r="N49" s="70"/>
-      <c r="O49" s="70"/>
-      <c r="P49" s="70"/>
-      <c r="Q49" s="70"/>
-      <c r="R49" s="70"/>
-      <c r="S49" s="70"/>
-      <c r="T49" s="70"/>
-      <c r="U49" s="70"/>
-      <c r="V49" s="70"/>
-      <c r="W49" s="70"/>
-      <c r="X49" s="70"/>
-      <c r="Y49" s="70"/>
-      <c r="Z49" s="70"/>
-      <c r="AA49" s="70"/>
-      <c r="AB49" s="70"/>
-      <c r="AC49" s="70"/>
-      <c r="AD49" s="70"/>
-      <c r="AE49" s="70"/>
-      <c r="AF49" s="70"/>
-      <c r="AG49" s="70"/>
-      <c r="AH49" s="70"/>
-      <c r="AI49" s="70"/>
-      <c r="AJ49" s="70"/>
-      <c r="AK49" s="70"/>
-      <c r="AL49" s="70"/>
-      <c r="AM49" s="70"/>
-      <c r="AN49" s="70"/>
-      <c r="AO49" s="70"/>
-      <c r="AP49" s="70"/>
-      <c r="AQ49" s="70"/>
-      <c r="AR49" s="70"/>
-      <c r="AS49" s="70"/>
-      <c r="AT49" s="70"/>
-      <c r="AU49" s="70"/>
-      <c r="AV49" s="70"/>
-      <c r="AW49" s="70"/>
-      <c r="AX49" s="70"/>
-      <c r="AY49" s="70"/>
-      <c r="AZ49" s="70"/>
-      <c r="BA49" s="70"/>
-      <c r="BB49" s="70"/>
-      <c r="BC49" s="70"/>
-      <c r="BD49" s="70"/>
-      <c r="BE49" s="70"/>
-      <c r="BF49" s="70"/>
-      <c r="BG49" s="70"/>
-      <c r="BH49" s="70"/>
-      <c r="BI49" s="71"/>
-      <c r="BJ49" s="71"/>
-      <c r="BK49" s="71"/>
-      <c r="BL49" s="71"/>
-      <c r="BM49" s="70"/>
-      <c r="BN49" s="70"/>
-      <c r="BO49" s="70"/>
-      <c r="BP49" s="70"/>
-      <c r="BQ49" s="70"/>
-      <c r="BR49" s="70"/>
-      <c r="BS49" s="70"/>
-      <c r="BT49" s="70"/>
-      <c r="BU49" s="70"/>
-      <c r="BV49" s="70"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="33"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+      <c r="N49" s="33"/>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="33"/>
+      <c r="S49" s="33"/>
+      <c r="T49" s="33"/>
+      <c r="U49" s="33"/>
+      <c r="V49" s="33"/>
+      <c r="W49" s="33"/>
+      <c r="X49" s="33"/>
+      <c r="Y49" s="33"/>
+      <c r="Z49" s="33"/>
+      <c r="AA49" s="33"/>
+      <c r="AB49" s="33"/>
+      <c r="AC49" s="33"/>
+      <c r="AD49" s="33"/>
+      <c r="AE49" s="33"/>
+      <c r="AF49" s="33"/>
+      <c r="AG49" s="33"/>
+      <c r="AH49" s="33"/>
+      <c r="AI49" s="33"/>
+      <c r="AJ49" s="33"/>
+      <c r="AK49" s="33"/>
+      <c r="AL49" s="33"/>
+      <c r="AM49" s="33"/>
+      <c r="AN49" s="33"/>
+      <c r="AO49" s="33"/>
+      <c r="AP49" s="33"/>
+      <c r="AQ49" s="33"/>
+      <c r="AR49" s="33"/>
+      <c r="AS49" s="33"/>
+      <c r="AT49" s="33"/>
+      <c r="AU49" s="33"/>
+      <c r="AV49" s="33"/>
+      <c r="AW49" s="33"/>
+      <c r="AX49" s="33"/>
+      <c r="AY49" s="33"/>
+      <c r="AZ49" s="33"/>
+      <c r="BA49" s="33"/>
+      <c r="BB49" s="33"/>
+      <c r="BC49" s="33"/>
+      <c r="BD49" s="33"/>
+      <c r="BE49" s="33"/>
+      <c r="BF49" s="33"/>
+      <c r="BG49" s="33"/>
+      <c r="BH49" s="33"/>
+      <c r="BI49" s="94"/>
+      <c r="BJ49" s="91"/>
+      <c r="BK49" s="91"/>
+      <c r="BL49" s="91"/>
+      <c r="BM49" s="33"/>
+      <c r="BN49" s="33"/>
+      <c r="BO49" s="33"/>
+      <c r="BP49" s="33"/>
+      <c r="BQ49" s="33"/>
+      <c r="BR49" s="33"/>
+      <c r="BS49" s="33"/>
+      <c r="BT49" s="33"/>
+      <c r="BU49" s="33"/>
+      <c r="BV49" s="33"/>
     </row>
     <row r="50" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A50" s="22"/>
-      <c r="B50" s="22" t="s">
+      <c r="A50" s="23"/>
+      <c r="B50" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="22" t="s">
+      <c r="C50" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="72"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="48"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="48"/>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-      <c r="O50" s="48"/>
-      <c r="P50" s="48"/>
-      <c r="Q50" s="48"/>
-      <c r="R50" s="48"/>
-      <c r="S50" s="48"/>
-      <c r="T50" s="48"/>
-      <c r="U50" s="48"/>
-      <c r="V50" s="48"/>
-      <c r="W50" s="48"/>
-      <c r="X50" s="48"/>
-      <c r="Y50" s="48"/>
-      <c r="Z50" s="48"/>
-      <c r="AA50" s="48"/>
-      <c r="AB50" s="48"/>
-      <c r="AC50" s="48"/>
-      <c r="AD50" s="48"/>
-      <c r="AE50" s="48"/>
-      <c r="AF50" s="48"/>
-      <c r="AG50" s="73"/>
-      <c r="AH50" s="48"/>
-      <c r="AI50" s="48"/>
-      <c r="AJ50" s="48"/>
-      <c r="AK50" s="48"/>
-      <c r="AL50" s="48"/>
-      <c r="AM50" s="48"/>
-      <c r="AN50" s="76"/>
-      <c r="AO50" s="76"/>
-      <c r="AP50" s="76"/>
-      <c r="AQ50" s="76"/>
-      <c r="AR50" s="48"/>
-      <c r="AS50" s="48"/>
-      <c r="AT50" s="48"/>
-      <c r="AU50" s="48"/>
-      <c r="AV50" s="48"/>
-      <c r="AW50" s="77"/>
-      <c r="AX50" s="77"/>
-      <c r="AY50" s="48"/>
-      <c r="AZ50" s="48"/>
-      <c r="BA50" s="48"/>
-      <c r="BB50" s="48"/>
-      <c r="BC50" s="48"/>
-      <c r="BD50" s="48"/>
-      <c r="BE50" s="48"/>
-      <c r="BF50" s="48"/>
-      <c r="BG50" s="48"/>
-      <c r="BH50" s="48"/>
-      <c r="BI50" s="1"/>
+      <c r="D50" s="74"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="53"/>
+      <c r="N50" s="53"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="53"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="53"/>
+      <c r="S50" s="53"/>
+      <c r="T50" s="53"/>
+      <c r="U50" s="53"/>
+      <c r="V50" s="53"/>
+      <c r="W50" s="53"/>
+      <c r="X50" s="53"/>
+      <c r="Y50" s="53"/>
+      <c r="Z50" s="53"/>
+      <c r="AA50" s="53"/>
+      <c r="AB50" s="53"/>
+      <c r="AC50" s="53"/>
+      <c r="AD50" s="53"/>
+      <c r="AE50" s="53"/>
+      <c r="AF50" s="53"/>
+      <c r="AG50" s="75"/>
+      <c r="AH50" s="53"/>
+      <c r="AI50" s="53"/>
+      <c r="AJ50" s="53"/>
+      <c r="AK50" s="53"/>
+      <c r="AL50" s="53"/>
+      <c r="AM50" s="53"/>
+      <c r="AN50" s="78"/>
+      <c r="AO50" s="78"/>
+      <c r="AP50" s="78"/>
+      <c r="AQ50" s="78"/>
+      <c r="AR50" s="53"/>
+      <c r="AS50" s="53"/>
+      <c r="AT50" s="53"/>
+      <c r="AU50" s="53"/>
+      <c r="AV50" s="53"/>
+      <c r="AW50" s="79"/>
+      <c r="AX50" s="79"/>
+      <c r="AY50" s="53"/>
+      <c r="AZ50" s="53"/>
+      <c r="BA50" s="53"/>
+      <c r="BB50" s="53"/>
+      <c r="BC50" s="53"/>
+      <c r="BD50" s="53"/>
+      <c r="BE50" s="53"/>
+      <c r="BF50" s="53"/>
+      <c r="BG50" s="53"/>
+      <c r="BH50" s="53"/>
+      <c r="BI50" s="14"/>
       <c r="BJ50" s="1"/>
-      <c r="BK50" s="53"/>
-      <c r="BL50" s="30"/>
-      <c r="BM50" s="53"/>
-      <c r="BN50" s="53"/>
-      <c r="BO50" s="22"/>
-      <c r="BP50" s="22"/>
-      <c r="BQ50" s="22"/>
-      <c r="BR50" s="22"/>
-      <c r="BS50" s="22"/>
-      <c r="BT50" s="22"/>
-      <c r="BU50" s="22"/>
-      <c r="BV50" s="22"/>
+      <c r="BK50" s="58"/>
+      <c r="BL50" s="36"/>
+      <c r="BM50" s="58"/>
+      <c r="BN50" s="58"/>
+      <c r="BO50" s="23"/>
+      <c r="BP50" s="23"/>
+      <c r="BQ50" s="23"/>
+      <c r="BR50" s="23"/>
+      <c r="BS50" s="23"/>
+      <c r="BT50" s="23"/>
+      <c r="BU50" s="23"/>
+      <c r="BV50" s="23"/>
     </row>
     <row r="51" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
@@ -5283,13 +5313,13 @@
       <c r="AO51" s="14"/>
       <c r="AP51" s="14"/>
       <c r="AQ51" s="14"/>
-      <c r="AR51" s="26"/>
-      <c r="AS51" s="26"/>
-      <c r="AT51" s="26"/>
+      <c r="AR51" s="28"/>
+      <c r="AS51" s="28"/>
+      <c r="AT51" s="28"/>
       <c r="AU51" s="14"/>
       <c r="AV51" s="14"/>
-      <c r="AW51" s="37"/>
-      <c r="AX51" s="37"/>
+      <c r="AW51" s="42"/>
+      <c r="AX51" s="42"/>
       <c r="AY51" s="14"/>
       <c r="AZ51" s="14"/>
       <c r="BA51" s="14"/>
@@ -5300,12 +5330,12 @@
       <c r="BF51" s="14"/>
       <c r="BG51" s="14"/>
       <c r="BH51" s="14"/>
-      <c r="BI51" s="1"/>
+      <c r="BI51" s="14"/>
       <c r="BJ51" s="1"/>
-      <c r="BK51" s="49"/>
+      <c r="BK51" s="54"/>
       <c r="BL51" s="8"/>
-      <c r="BM51" s="49"/>
-      <c r="BN51" s="49"/>
+      <c r="BM51" s="54"/>
+      <c r="BN51" s="54"/>
       <c r="BO51" s="1"/>
       <c r="BP51" s="1"/>
       <c r="BQ51" s="1"/>
@@ -5365,11 +5395,11 @@
       <c r="AQ52" s="14"/>
       <c r="AR52" s="14"/>
       <c r="AS52" s="14"/>
-      <c r="AT52" s="26"/>
-      <c r="AU52" s="26"/>
-      <c r="AV52" s="26"/>
-      <c r="AW52" s="37"/>
-      <c r="AX52" s="37"/>
+      <c r="AT52" s="28"/>
+      <c r="AU52" s="28"/>
+      <c r="AV52" s="28"/>
+      <c r="AW52" s="42"/>
+      <c r="AX52" s="42"/>
       <c r="AY52" s="14"/>
       <c r="AZ52" s="14"/>
       <c r="BA52" s="14"/>
@@ -5380,11 +5410,11 @@
       <c r="BF52" s="14"/>
       <c r="BG52" s="14"/>
       <c r="BH52" s="14"/>
-      <c r="BI52" s="1"/>
+      <c r="BI52" s="14"/>
       <c r="BJ52" s="1"/>
       <c r="BK52" s="1"/>
       <c r="BL52" s="8"/>
-      <c r="BN52" s="49"/>
+      <c r="BN52" s="54"/>
       <c r="BO52" s="1"/>
       <c r="BP52" s="1"/>
       <c r="BQ52" s="1"/>
@@ -5446,22 +5476,22 @@
       <c r="AT53" s="14"/>
       <c r="AU53" s="14"/>
       <c r="AV53" s="14"/>
-      <c r="AW53" s="26"/>
-      <c r="AX53" s="38"/>
-      <c r="AY53" s="38"/>
-      <c r="AZ53" s="38"/>
-      <c r="BA53" s="26"/>
-      <c r="BB53" s="26"/>
+      <c r="AW53" s="28"/>
+      <c r="AX53" s="43"/>
+      <c r="AY53" s="43"/>
+      <c r="AZ53" s="43"/>
+      <c r="BA53" s="28"/>
+      <c r="BB53" s="28"/>
       <c r="BC53" s="14"/>
       <c r="BD53" s="14"/>
       <c r="BE53" s="14"/>
       <c r="BF53" s="14"/>
       <c r="BG53" s="14"/>
       <c r="BH53" s="14"/>
-      <c r="BI53" s="1"/>
+      <c r="BI53" s="14"/>
       <c r="BJ53" s="1"/>
       <c r="BK53" s="1"/>
-      <c r="BL53" s="49"/>
+      <c r="BL53" s="54"/>
       <c r="BM53" s="8"/>
       <c r="BN53" s="1"/>
       <c r="BO53" s="1"/>
@@ -5532,16 +5562,16 @@
       <c r="AZ54" s="14"/>
       <c r="BA54" s="14"/>
       <c r="BB54" s="14"/>
-      <c r="BC54" s="26"/>
-      <c r="BD54" s="26"/>
-      <c r="BE54" s="26"/>
-      <c r="BF54" s="26"/>
+      <c r="BC54" s="28"/>
+      <c r="BD54" s="28"/>
+      <c r="BE54" s="28"/>
+      <c r="BF54" s="28"/>
       <c r="BG54" s="14"/>
       <c r="BH54" s="14"/>
-      <c r="BI54" s="49"/>
-      <c r="BJ54" s="49"/>
-      <c r="BK54" s="49"/>
-      <c r="BL54" s="49"/>
+      <c r="BI54" s="14"/>
+      <c r="BJ54" s="54"/>
+      <c r="BK54" s="54"/>
+      <c r="BL54" s="54"/>
       <c r="BM54" s="8"/>
       <c r="BN54" s="1"/>
       <c r="BO54" s="1"/>
@@ -5590,11 +5620,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A19:XFD19"/>
-    <mergeCell ref="A3:XFD3"/>
-    <mergeCell ref="A49:XFD49"/>
-    <mergeCell ref="BH1:BN1"/>
+  <mergeCells count="9">
     <mergeCell ref="BO1:BU1"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="K1:Q1"/>

</xml_diff>

<commit_message>
Page Mon Compte + Connexion
</commit_message>
<xml_diff>
--- a/ALM/Planning.xlsx
+++ b/ALM/Planning.xlsx
@@ -692,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -781,24 +781,6 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
@@ -815,7 +797,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -839,6 +820,27 @@
       <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1119,10 +1121,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:BV61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="BI36" sqref="BI36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BM51" sqref="BM51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="2" x14ac:dyDescent="0.35"/>
@@ -1131,102 +1137,102 @@
     <col min="2" max="2" width="37.08984375" customWidth="1"/>
     <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.36328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="61" width="3.36328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="62" max="66" width="3.36328125" style="54" bestFit="1" customWidth="1"/>
+    <col min="5" max="62" width="3.36328125" style="17" bestFit="1" customWidth="1"/>
+    <col min="63" max="66" width="3.36328125" style="54" bestFit="1" customWidth="1"/>
     <col min="67" max="74" width="3.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="66" t="s">
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
+      <c r="K1" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="66" t="s">
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+      <c r="Q1" s="102"/>
+      <c r="R1" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66" t="s">
+      <c r="S1" s="102"/>
+      <c r="T1" s="102"/>
+      <c r="U1" s="102"/>
+      <c r="V1" s="102"/>
+      <c r="W1" s="102"/>
+      <c r="X1" s="102"/>
+      <c r="Y1" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66" t="s">
+      <c r="Z1" s="102"/>
+      <c r="AA1" s="102"/>
+      <c r="AB1" s="102"/>
+      <c r="AC1" s="102"/>
+      <c r="AD1" s="102"/>
+      <c r="AE1" s="102"/>
+      <c r="AF1" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="66"/>
-      <c r="AJ1" s="66"/>
-      <c r="AK1" s="66"/>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="69" t="s">
+      <c r="AG1" s="102"/>
+      <c r="AH1" s="102"/>
+      <c r="AI1" s="102"/>
+      <c r="AJ1" s="102"/>
+      <c r="AK1" s="102"/>
+      <c r="AL1" s="102"/>
+      <c r="AM1" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="70"/>
-      <c r="AO1" s="70"/>
-      <c r="AP1" s="70"/>
-      <c r="AQ1" s="70"/>
-      <c r="AR1" s="70"/>
-      <c r="AS1" s="71"/>
-      <c r="AT1" s="66" t="s">
+      <c r="AN1" s="104"/>
+      <c r="AO1" s="104"/>
+      <c r="AP1" s="104"/>
+      <c r="AQ1" s="104"/>
+      <c r="AR1" s="104"/>
+      <c r="AS1" s="105"/>
+      <c r="AT1" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="AU1" s="66"/>
-      <c r="AV1" s="66"/>
-      <c r="AW1" s="66"/>
-      <c r="AX1" s="66"/>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="66"/>
-      <c r="BA1" s="69" t="s">
+      <c r="AU1" s="102"/>
+      <c r="AV1" s="102"/>
+      <c r="AW1" s="102"/>
+      <c r="AX1" s="102"/>
+      <c r="AY1" s="102"/>
+      <c r="AZ1" s="102"/>
+      <c r="BA1" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="BB1" s="70"/>
-      <c r="BC1" s="70"/>
-      <c r="BD1" s="70"/>
-      <c r="BE1" s="70"/>
-      <c r="BF1" s="70"/>
-      <c r="BG1" s="71"/>
-      <c r="BH1" s="86" t="s">
+      <c r="BB1" s="104"/>
+      <c r="BC1" s="104"/>
+      <c r="BD1" s="104"/>
+      <c r="BE1" s="104"/>
+      <c r="BF1" s="104"/>
+      <c r="BG1" s="105"/>
+      <c r="BH1" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="BI1" s="90"/>
-      <c r="BJ1" s="87"/>
-      <c r="BK1" s="87"/>
-      <c r="BL1" s="87"/>
-      <c r="BM1" s="87"/>
-      <c r="BN1" s="88"/>
-      <c r="BO1" s="67" t="s">
+      <c r="BI1" s="83"/>
+      <c r="BJ1" s="83"/>
+      <c r="BK1" s="80"/>
+      <c r="BL1" s="80"/>
+      <c r="BM1" s="80"/>
+      <c r="BN1" s="81"/>
+      <c r="BO1" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="BP1" s="67"/>
-      <c r="BQ1" s="67"/>
-      <c r="BR1" s="67"/>
-      <c r="BS1" s="67"/>
-      <c r="BT1" s="67"/>
-      <c r="BU1" s="67"/>
+      <c r="BP1" s="100"/>
+      <c r="BQ1" s="100"/>
+      <c r="BR1" s="100"/>
+      <c r="BS1" s="100"/>
+      <c r="BT1" s="100"/>
+      <c r="BU1" s="100"/>
     </row>
     <row r="2" spans="1:74" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="11">
@@ -1403,13 +1409,13 @@
       <c r="BI2" s="11">
         <v>43452</v>
       </c>
-      <c r="BJ2" s="53">
+      <c r="BJ2" s="11">
         <v>43453</v>
       </c>
       <c r="BK2" s="53">
         <v>43454</v>
       </c>
-      <c r="BL2" s="44">
+      <c r="BL2" s="95">
         <v>43455</v>
       </c>
       <c r="BM2" s="44">
@@ -1418,10 +1424,10 @@
       <c r="BN2" s="44">
         <v>43457</v>
       </c>
-      <c r="BO2" s="102">
+      <c r="BO2" s="95">
         <v>43458</v>
       </c>
-      <c r="BP2" s="102">
+      <c r="BP2" s="95">
         <v>43459</v>
       </c>
       <c r="BQ2" s="44">
@@ -1439,7 +1445,7 @@
       <c r="BU2" s="44">
         <v>43464</v>
       </c>
-      <c r="BV2" s="102">
+      <c r="BV2" s="95">
         <v>43465</v>
       </c>
     </row>
@@ -1507,7 +1513,7 @@
       <c r="BG3" s="32"/>
       <c r="BH3" s="32"/>
       <c r="BI3" s="33"/>
-      <c r="BJ3" s="32"/>
+      <c r="BJ3" s="33"/>
       <c r="BK3" s="32"/>
       <c r="BL3" s="32"/>
       <c r="BM3" s="32"/>
@@ -1587,7 +1593,7 @@
       <c r="BG4" s="14"/>
       <c r="BH4" s="14"/>
       <c r="BI4" s="14"/>
-      <c r="BJ4" s="52"/>
+      <c r="BJ4" s="14"/>
       <c r="BK4" s="52"/>
       <c r="BL4" s="52"/>
       <c r="BM4" s="52"/>
@@ -1667,7 +1673,7 @@
       <c r="BG5" s="14"/>
       <c r="BH5" s="14"/>
       <c r="BI5" s="14"/>
-      <c r="BJ5" s="52"/>
+      <c r="BJ5" s="14"/>
       <c r="BK5" s="52"/>
       <c r="BL5" s="52"/>
       <c r="BM5" s="52"/>
@@ -1747,7 +1753,7 @@
       <c r="BG6" s="14"/>
       <c r="BH6" s="14"/>
       <c r="BI6" s="14"/>
-      <c r="BJ6" s="52"/>
+      <c r="BJ6" s="14"/>
       <c r="BK6" s="52"/>
       <c r="BL6" s="52"/>
       <c r="BM6" s="52"/>
@@ -1827,7 +1833,7 @@
       <c r="BG7" s="13"/>
       <c r="BH7" s="13"/>
       <c r="BI7" s="13"/>
-      <c r="BJ7" s="52"/>
+      <c r="BJ7" s="14"/>
       <c r="BK7" s="52"/>
       <c r="BL7" s="52"/>
       <c r="BM7" s="52"/>
@@ -1907,7 +1913,7 @@
       <c r="BG8" s="13"/>
       <c r="BH8" s="13"/>
       <c r="BI8" s="14"/>
-      <c r="BJ8" s="52"/>
+      <c r="BJ8" s="14"/>
       <c r="BK8" s="52"/>
       <c r="BL8" s="52"/>
       <c r="BM8" s="52"/>
@@ -1987,7 +1993,7 @@
       <c r="BG9" s="14"/>
       <c r="BH9" s="14"/>
       <c r="BI9" s="14"/>
-      <c r="BJ9" s="52"/>
+      <c r="BJ9" s="14"/>
       <c r="BK9" s="52"/>
       <c r="BL9" s="52"/>
       <c r="BM9" s="52"/>
@@ -2067,7 +2073,7 @@
       <c r="BG10" s="14"/>
       <c r="BH10" s="14"/>
       <c r="BI10" s="14"/>
-      <c r="BJ10" s="52"/>
+      <c r="BJ10" s="14"/>
       <c r="BK10" s="52"/>
       <c r="BL10" s="52"/>
       <c r="BM10" s="52"/>
@@ -2147,7 +2153,7 @@
       <c r="BG11" s="14"/>
       <c r="BH11" s="14"/>
       <c r="BI11" s="14"/>
-      <c r="BJ11" s="52"/>
+      <c r="BJ11" s="14"/>
       <c r="BK11" s="52"/>
       <c r="BL11" s="52"/>
       <c r="BM11" s="52"/>
@@ -2227,7 +2233,7 @@
       <c r="BG12" s="14"/>
       <c r="BH12" s="14"/>
       <c r="BI12" s="14"/>
-      <c r="BJ12" s="52"/>
+      <c r="BJ12" s="14"/>
       <c r="BK12" s="52"/>
       <c r="BL12" s="52"/>
       <c r="BM12" s="52"/>
@@ -2307,7 +2313,7 @@
       <c r="BG13" s="14"/>
       <c r="BH13" s="14"/>
       <c r="BI13" s="14"/>
-      <c r="BJ13" s="52"/>
+      <c r="BJ13" s="14"/>
       <c r="BK13" s="52"/>
       <c r="BL13" s="52"/>
       <c r="BM13" s="52"/>
@@ -2385,7 +2391,7 @@
       <c r="BG14" s="14"/>
       <c r="BH14" s="14"/>
       <c r="BI14" s="14"/>
-      <c r="BJ14" s="52"/>
+      <c r="BJ14" s="14"/>
       <c r="BK14" s="52"/>
       <c r="BL14" s="52"/>
       <c r="BM14" s="52"/>
@@ -2465,7 +2471,7 @@
       <c r="BG15" s="14"/>
       <c r="BH15" s="14"/>
       <c r="BI15" s="14"/>
-      <c r="BJ15" s="52"/>
+      <c r="BJ15" s="14"/>
       <c r="BK15" s="52"/>
       <c r="BL15" s="52"/>
       <c r="BM15" s="52"/>
@@ -2545,7 +2551,7 @@
       <c r="BG16" s="14"/>
       <c r="BH16" s="14"/>
       <c r="BI16" s="14"/>
-      <c r="BJ16" s="52"/>
+      <c r="BJ16" s="14"/>
       <c r="BK16" s="52"/>
       <c r="BL16" s="52"/>
       <c r="BM16" s="52"/>
@@ -2625,7 +2631,7 @@
       <c r="BG17" s="14"/>
       <c r="BH17" s="14"/>
       <c r="BI17" s="14"/>
-      <c r="BJ17" s="52"/>
+      <c r="BJ17" s="14"/>
       <c r="BK17" s="52"/>
       <c r="BL17" s="52"/>
       <c r="BM17" s="52"/>
@@ -2640,7 +2646,7 @@
       <c r="BV17" s="1"/>
     </row>
     <row r="18" spans="1:74" x14ac:dyDescent="0.35">
-      <c r="A18" s="84"/>
+      <c r="A18" s="77"/>
       <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
@@ -2705,7 +2711,7 @@
       <c r="BG18" s="14"/>
       <c r="BH18" s="14"/>
       <c r="BI18" s="13"/>
-      <c r="BJ18" s="52"/>
+      <c r="BJ18" s="14"/>
       <c r="BK18" s="52"/>
       <c r="BL18" s="52"/>
       <c r="BM18" s="52"/>
@@ -2783,7 +2789,7 @@
       <c r="BG19" s="32"/>
       <c r="BH19" s="32"/>
       <c r="BI19" s="33"/>
-      <c r="BJ19" s="32"/>
+      <c r="BJ19" s="33"/>
       <c r="BK19" s="32"/>
       <c r="BL19" s="32"/>
       <c r="BM19" s="32"/>
@@ -2805,7 +2811,7 @@
       <c r="C20" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="72"/>
+      <c r="D20" s="66"/>
       <c r="E20" s="51"/>
       <c r="F20" s="51"/>
       <c r="G20" s="51"/>
@@ -2820,12 +2826,12 @@
       <c r="P20" s="51"/>
       <c r="Q20" s="51"/>
       <c r="R20" s="51"/>
-      <c r="S20" s="73"/>
-      <c r="T20" s="73"/>
-      <c r="U20" s="73"/>
-      <c r="V20" s="73"/>
-      <c r="W20" s="73"/>
-      <c r="X20" s="73"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="67"/>
+      <c r="U20" s="67"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="67"/>
+      <c r="X20" s="67"/>
       <c r="Y20" s="51"/>
       <c r="Z20" s="51"/>
       <c r="AA20" s="51"/>
@@ -2854,15 +2860,15 @@
       <c r="AX20" s="51"/>
       <c r="AY20" s="51"/>
       <c r="AZ20" s="51"/>
-      <c r="BA20" s="74"/>
+      <c r="BA20" s="68"/>
       <c r="BB20" s="51"/>
       <c r="BC20" s="51"/>
       <c r="BD20" s="51"/>
       <c r="BE20" s="51"/>
-      <c r="BF20" s="74"/>
-      <c r="BG20" s="75"/>
+      <c r="BF20" s="68"/>
+      <c r="BG20" s="69"/>
       <c r="BI20" s="51"/>
-      <c r="BJ20" s="56"/>
+      <c r="BJ20" s="51"/>
       <c r="BK20" s="56"/>
       <c r="BM20" s="34"/>
       <c r="BO20" s="23"/>
@@ -2940,7 +2946,7 @@
       <c r="BG21" s="46"/>
       <c r="BH21" s="14"/>
       <c r="BI21" s="14"/>
-      <c r="BJ21" s="52"/>
+      <c r="BJ21" s="14"/>
       <c r="BK21" s="52"/>
       <c r="BL21" s="52"/>
       <c r="BM21" s="52"/>
@@ -3020,7 +3026,7 @@
       <c r="BG22" s="46"/>
       <c r="BH22" s="14"/>
       <c r="BI22" s="14"/>
-      <c r="BJ22" s="52"/>
+      <c r="BJ22" s="14"/>
       <c r="BK22" s="52"/>
       <c r="BL22" s="52"/>
       <c r="BM22" s="52"/>
@@ -3100,7 +3106,7 @@
       <c r="BG23" s="47"/>
       <c r="BH23" s="14"/>
       <c r="BI23" s="14"/>
-      <c r="BJ23" s="52"/>
+      <c r="BJ23" s="14"/>
       <c r="BK23" s="52"/>
       <c r="BL23" s="52"/>
       <c r="BM23" s="52"/>
@@ -3180,7 +3186,7 @@
       <c r="BG24" s="47"/>
       <c r="BH24" s="14"/>
       <c r="BI24" s="14"/>
-      <c r="BJ24" s="52"/>
+      <c r="BJ24" s="14"/>
       <c r="BK24" s="52"/>
       <c r="BL24" s="52"/>
       <c r="BM24" s="52"/>
@@ -3260,7 +3266,7 @@
       <c r="BG25" s="46"/>
       <c r="BH25" s="14"/>
       <c r="BI25" s="14"/>
-      <c r="BJ25" s="52"/>
+      <c r="BJ25" s="14"/>
       <c r="BK25" s="52"/>
       <c r="BL25" s="52"/>
       <c r="BM25" s="52"/>
@@ -3340,7 +3346,7 @@
       <c r="BG26" s="48"/>
       <c r="BH26" s="14"/>
       <c r="BI26" s="14"/>
-      <c r="BJ26" s="52"/>
+      <c r="BJ26" s="14"/>
       <c r="BK26" s="52"/>
       <c r="BL26" s="52"/>
       <c r="BM26" s="52"/>
@@ -3420,15 +3426,15 @@
       <c r="BG27" s="14"/>
       <c r="BH27" s="27"/>
       <c r="BI27" s="14"/>
-      <c r="BJ27" s="52"/>
+      <c r="BJ27" s="14"/>
       <c r="BK27" s="52"/>
       <c r="BL27" s="52"/>
       <c r="BM27" s="52"/>
-      <c r="BN27" s="8"/>
+      <c r="BN27" s="52"/>
       <c r="BO27" s="1"/>
       <c r="BP27" s="52"/>
-      <c r="BQ27" s="52"/>
-      <c r="BR27" s="52"/>
+      <c r="BQ27" s="97"/>
+      <c r="BR27" s="1"/>
       <c r="BS27" s="52"/>
       <c r="BT27" s="1"/>
       <c r="BU27" s="1"/>
@@ -3499,15 +3505,15 @@
       <c r="BG28" s="14"/>
       <c r="BH28" s="27"/>
       <c r="BI28" s="14"/>
-      <c r="BJ28" s="52"/>
+      <c r="BJ28" s="14"/>
       <c r="BK28" s="52"/>
       <c r="BL28" s="52"/>
       <c r="BM28" s="52"/>
-      <c r="BN28" s="8"/>
+      <c r="BN28" s="52"/>
       <c r="BO28" s="1"/>
       <c r="BP28" s="52"/>
-      <c r="BQ28" s="52"/>
-      <c r="BR28" s="52"/>
+      <c r="BQ28" s="97"/>
+      <c r="BR28" s="1"/>
       <c r="BS28" s="52"/>
       <c r="BT28" s="1"/>
       <c r="BU28" s="1"/>
@@ -3578,15 +3584,15 @@
       <c r="BG29" s="14"/>
       <c r="BH29" s="27"/>
       <c r="BI29" s="14"/>
-      <c r="BJ29" s="52"/>
+      <c r="BJ29" s="14"/>
       <c r="BK29" s="52"/>
       <c r="BL29" s="52"/>
       <c r="BM29" s="52"/>
-      <c r="BN29" s="8"/>
+      <c r="BN29" s="52"/>
       <c r="BO29" s="1"/>
       <c r="BP29" s="52"/>
-      <c r="BQ29" s="52"/>
-      <c r="BR29" s="52"/>
+      <c r="BQ29" s="97"/>
+      <c r="BR29" s="1"/>
       <c r="BS29" s="52"/>
       <c r="BT29" s="1"/>
       <c r="BU29" s="1"/>
@@ -3658,15 +3664,15 @@
       <c r="BG30" s="14"/>
       <c r="BH30" s="27"/>
       <c r="BI30" s="14"/>
-      <c r="BJ30" s="52"/>
+      <c r="BJ30" s="14"/>
       <c r="BK30" s="52"/>
       <c r="BL30" s="52"/>
       <c r="BM30" s="52"/>
-      <c r="BN30" s="8"/>
+      <c r="BN30" s="52"/>
       <c r="BO30" s="1"/>
       <c r="BP30" s="1"/>
-      <c r="BQ30" s="52"/>
-      <c r="BR30" s="52"/>
+      <c r="BQ30" s="97"/>
+      <c r="BR30" s="1"/>
       <c r="BS30" s="52"/>
       <c r="BT30" s="1"/>
       <c r="BU30" s="1"/>
@@ -3738,17 +3744,17 @@
       <c r="BG31" s="14"/>
       <c r="BH31" s="27"/>
       <c r="BI31" s="14"/>
-      <c r="BJ31" s="52"/>
+      <c r="BJ31" s="14"/>
       <c r="BK31" s="52"/>
       <c r="BL31" s="52"/>
       <c r="BM31" s="52"/>
-      <c r="BN31" s="103"/>
+      <c r="BN31" s="55"/>
       <c r="BO31" s="22"/>
-      <c r="BP31" s="1"/>
-      <c r="BQ31" s="52"/>
-      <c r="BR31" s="55"/>
+      <c r="BP31" s="22"/>
+      <c r="BQ31" s="96"/>
+      <c r="BR31" s="1"/>
       <c r="BS31" s="55"/>
-      <c r="BT31" s="1"/>
+      <c r="BT31" s="22"/>
       <c r="BU31" s="1"/>
       <c r="BV31" s="1"/>
     </row>
@@ -3818,17 +3824,17 @@
       <c r="BG32" s="14"/>
       <c r="BH32" s="14"/>
       <c r="BI32" s="14"/>
-      <c r="BJ32" s="56"/>
+      <c r="BJ32" s="51"/>
       <c r="BK32" s="52"/>
       <c r="BL32" s="52"/>
       <c r="BM32" s="62"/>
       <c r="BN32" s="28"/>
       <c r="BO32" s="30"/>
       <c r="BP32" s="29"/>
-      <c r="BQ32" s="84"/>
-      <c r="BR32" s="93"/>
-      <c r="BS32" s="94"/>
-      <c r="BT32" s="21"/>
+      <c r="BQ32" s="77"/>
+      <c r="BR32" s="78"/>
+      <c r="BS32" s="86"/>
+      <c r="BT32" s="87"/>
       <c r="BU32" s="1"/>
       <c r="BV32" s="1"/>
     </row>
@@ -3897,17 +3903,17 @@
       <c r="BG33" s="14"/>
       <c r="BH33" s="14"/>
       <c r="BI33" s="14"/>
-      <c r="BJ33" s="52"/>
+      <c r="BJ33" s="14"/>
       <c r="BK33" s="52"/>
       <c r="BL33" s="52"/>
       <c r="BM33" s="62"/>
       <c r="BN33" s="57"/>
       <c r="BO33" s="7"/>
       <c r="BP33" s="58"/>
-      <c r="BQ33" s="84"/>
-      <c r="BR33" s="95"/>
-      <c r="BS33" s="96"/>
-      <c r="BT33" s="21"/>
+      <c r="BQ33" s="77"/>
+      <c r="BR33" s="77"/>
+      <c r="BS33" s="88"/>
+      <c r="BT33" s="89"/>
       <c r="BU33" s="1"/>
       <c r="BV33" s="1"/>
     </row>
@@ -3976,18 +3982,18 @@
       <c r="BG34" s="14"/>
       <c r="BH34" s="14"/>
       <c r="BI34" s="14"/>
-      <c r="BJ34" s="52"/>
+      <c r="BJ34" s="14"/>
       <c r="BK34" s="52"/>
       <c r="BL34" s="52"/>
       <c r="BM34" s="62"/>
       <c r="BN34" s="59"/>
       <c r="BO34" s="60"/>
       <c r="BP34" s="25"/>
-      <c r="BQ34" s="98"/>
-      <c r="BR34" s="24"/>
-      <c r="BS34" s="97"/>
-      <c r="BT34" s="26"/>
-      <c r="BU34" s="1"/>
+      <c r="BQ34" s="91"/>
+      <c r="BR34" s="91"/>
+      <c r="BS34" s="24"/>
+      <c r="BT34" s="90"/>
+      <c r="BU34" s="22"/>
       <c r="BV34" s="1"/>
     </row>
     <row r="35" spans="1:74" x14ac:dyDescent="0.35">
@@ -4056,19 +4062,19 @@
       <c r="BG35" s="14"/>
       <c r="BH35" s="14"/>
       <c r="BI35" s="14"/>
-      <c r="BJ35" s="52"/>
+      <c r="BJ35" s="14"/>
       <c r="BK35" s="52"/>
       <c r="BL35" s="52"/>
       <c r="BM35" s="52"/>
       <c r="BN35" s="61"/>
       <c r="BO35" s="23"/>
-      <c r="BP35" s="85"/>
+      <c r="BP35" s="78"/>
       <c r="BQ35" s="28"/>
       <c r="BR35" s="29"/>
-      <c r="BS35" s="85"/>
-      <c r="BT35" s="100"/>
-      <c r="BU35" s="21"/>
-      <c r="BV35" s="1"/>
+      <c r="BS35" s="78"/>
+      <c r="BT35" s="78"/>
+      <c r="BU35" s="93"/>
+      <c r="BV35" s="21"/>
     </row>
     <row r="36" spans="1:74" ht="15" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1"/>
@@ -4136,19 +4142,19 @@
       <c r="BG36" s="14"/>
       <c r="BH36" s="14"/>
       <c r="BI36" s="14"/>
-      <c r="BJ36" s="52"/>
+      <c r="BJ36" s="14"/>
       <c r="BK36" s="52"/>
       <c r="BL36" s="52"/>
       <c r="BM36" s="52"/>
       <c r="BN36" s="52"/>
       <c r="BO36" s="1"/>
-      <c r="BP36" s="84"/>
+      <c r="BP36" s="77"/>
       <c r="BQ36" s="24"/>
       <c r="BR36" s="25"/>
-      <c r="BS36" s="84"/>
-      <c r="BT36" s="101"/>
-      <c r="BU36" s="21"/>
-      <c r="BV36" s="1"/>
+      <c r="BS36" s="77"/>
+      <c r="BT36" s="77"/>
+      <c r="BU36" s="94"/>
+      <c r="BV36" s="21"/>
     </row>
     <row r="37" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
@@ -4216,19 +4222,19 @@
       <c r="BG37" s="14"/>
       <c r="BH37" s="14"/>
       <c r="BI37" s="14"/>
-      <c r="BJ37" s="52"/>
+      <c r="BJ37" s="14"/>
       <c r="BK37" s="63"/>
       <c r="BL37" s="63"/>
       <c r="BM37" s="52"/>
       <c r="BN37" s="52"/>
       <c r="BO37" s="23"/>
-      <c r="BP37" s="83"/>
+      <c r="BP37" s="76"/>
       <c r="BQ37" s="23"/>
       <c r="BR37" s="37"/>
-      <c r="BS37" s="82"/>
+      <c r="BS37" s="98"/>
       <c r="BT37" s="99"/>
-      <c r="BU37" s="8"/>
-      <c r="BV37" s="22"/>
+      <c r="BU37" s="34"/>
+      <c r="BV37" s="26"/>
     </row>
     <row r="38" spans="1:74" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
@@ -4295,7 +4301,7 @@
       <c r="BG38" s="14"/>
       <c r="BH38" s="14"/>
       <c r="BI38" s="14"/>
-      <c r="BJ38" s="52"/>
+      <c r="BJ38" s="14"/>
       <c r="BK38" s="52"/>
       <c r="BL38" s="52"/>
       <c r="BM38" s="52"/>
@@ -4306,7 +4312,7 @@
       <c r="BR38" s="37"/>
       <c r="BS38" s="4"/>
       <c r="BT38" s="4"/>
-      <c r="BU38" s="4"/>
+      <c r="BU38" s="92"/>
       <c r="BV38" s="4"/>
     </row>
     <row r="39" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
@@ -4375,7 +4381,7 @@
       <c r="BG39" s="14"/>
       <c r="BH39" s="14"/>
       <c r="BI39" s="45"/>
-      <c r="BJ39" s="52"/>
+      <c r="BJ39" s="14"/>
       <c r="BK39" s="52"/>
       <c r="BL39" s="52"/>
       <c r="BM39" s="52"/>
@@ -4455,7 +4461,7 @@
       <c r="BG40" s="14"/>
       <c r="BH40" s="14"/>
       <c r="BI40" s="45"/>
-      <c r="BJ40" s="52"/>
+      <c r="BJ40" s="14"/>
       <c r="BK40" s="52"/>
       <c r="BL40" s="52"/>
       <c r="BM40" s="52"/>
@@ -4534,8 +4540,8 @@
       <c r="BF41" s="14"/>
       <c r="BG41" s="14"/>
       <c r="BH41" s="14"/>
-      <c r="BI41" s="91"/>
-      <c r="BJ41" s="55"/>
+      <c r="BI41" s="84"/>
+      <c r="BJ41" s="50"/>
       <c r="BK41" s="55"/>
       <c r="BL41" s="55"/>
       <c r="BM41" s="52"/>
@@ -4615,17 +4621,17 @@
       <c r="BG42" s="14"/>
       <c r="BH42" s="42"/>
       <c r="BI42" s="14"/>
-      <c r="BJ42" s="62"/>
+      <c r="BJ42" s="42"/>
       <c r="BK42" s="28"/>
       <c r="BL42" s="30"/>
       <c r="BM42" s="29"/>
       <c r="BN42" s="52"/>
       <c r="BO42" s="1"/>
       <c r="BP42" s="1"/>
-      <c r="BQ42" s="8"/>
-      <c r="BR42" s="23"/>
-      <c r="BS42" s="23"/>
-      <c r="BT42" s="23"/>
+      <c r="BQ42" s="1"/>
+      <c r="BR42" s="8"/>
+      <c r="BS42" s="1"/>
+      <c r="BT42" s="1"/>
       <c r="BU42" s="23"/>
       <c r="BV42" s="23"/>
     </row>
@@ -4695,15 +4701,15 @@
       <c r="BG43" s="14"/>
       <c r="BH43" s="42"/>
       <c r="BI43" s="14"/>
-      <c r="BJ43" s="62"/>
+      <c r="BJ43" s="42"/>
       <c r="BK43" s="64"/>
       <c r="BL43" s="52"/>
       <c r="BM43" s="58"/>
       <c r="BN43" s="52"/>
       <c r="BO43" s="1"/>
       <c r="BP43" s="1"/>
-      <c r="BQ43" s="8"/>
-      <c r="BR43" s="1"/>
+      <c r="BQ43" s="1"/>
+      <c r="BR43" s="8"/>
       <c r="BS43" s="1"/>
       <c r="BT43" s="1"/>
       <c r="BU43" s="1"/>
@@ -4775,15 +4781,15 @@
       <c r="BG44" s="14"/>
       <c r="BH44" s="42"/>
       <c r="BI44" s="14"/>
-      <c r="BJ44" s="62"/>
+      <c r="BJ44" s="42"/>
       <c r="BK44" s="57"/>
       <c r="BL44" s="7"/>
       <c r="BM44" s="58"/>
       <c r="BN44" s="52"/>
       <c r="BO44" s="1"/>
       <c r="BP44" s="1"/>
-      <c r="BQ44" s="8"/>
-      <c r="BR44" s="1"/>
+      <c r="BQ44" s="1"/>
+      <c r="BR44" s="8"/>
       <c r="BS44" s="1"/>
       <c r="BT44" s="1"/>
       <c r="BU44" s="1"/>
@@ -4855,15 +4861,15 @@
       <c r="BG45" s="14"/>
       <c r="BH45" s="42"/>
       <c r="BI45" s="14"/>
-      <c r="BJ45" s="62"/>
+      <c r="BJ45" s="42"/>
       <c r="BK45" s="57"/>
       <c r="BL45" s="7"/>
       <c r="BM45" s="58"/>
       <c r="BN45" s="52"/>
       <c r="BO45" s="1"/>
       <c r="BP45" s="1"/>
-      <c r="BQ45" s="8"/>
-      <c r="BR45" s="1"/>
+      <c r="BQ45" s="1"/>
+      <c r="BR45" s="8"/>
       <c r="BS45" s="1"/>
       <c r="BT45" s="1"/>
       <c r="BU45" s="1"/>
@@ -4935,15 +4941,15 @@
       <c r="BG46" s="14"/>
       <c r="BH46" s="42"/>
       <c r="BI46" s="14"/>
-      <c r="BJ46" s="62"/>
+      <c r="BJ46" s="42"/>
       <c r="BK46" s="57"/>
       <c r="BL46" s="7"/>
       <c r="BM46" s="58"/>
       <c r="BN46" s="52"/>
       <c r="BO46" s="1"/>
       <c r="BP46" s="1"/>
-      <c r="BQ46" s="8"/>
-      <c r="BR46" s="1"/>
+      <c r="BQ46" s="1"/>
+      <c r="BR46" s="8"/>
       <c r="BS46" s="1"/>
       <c r="BT46" s="1"/>
       <c r="BU46" s="1"/>
@@ -5015,15 +5021,15 @@
       <c r="BG47" s="14"/>
       <c r="BH47" s="42"/>
       <c r="BI47" s="14"/>
-      <c r="BJ47" s="62"/>
+      <c r="BJ47" s="42"/>
       <c r="BK47" s="57"/>
       <c r="BL47" s="7"/>
       <c r="BM47" s="58"/>
       <c r="BN47" s="52"/>
       <c r="BO47" s="1"/>
       <c r="BP47" s="1"/>
-      <c r="BQ47" s="8"/>
-      <c r="BR47" s="1"/>
+      <c r="BQ47" s="1"/>
+      <c r="BR47" s="8"/>
       <c r="BS47" s="1"/>
       <c r="BT47" s="1"/>
       <c r="BU47" s="1"/>
@@ -5095,15 +5101,15 @@
       <c r="BG48" s="14"/>
       <c r="BH48" s="42"/>
       <c r="BI48" s="14"/>
-      <c r="BJ48" s="62"/>
+      <c r="BJ48" s="42"/>
       <c r="BK48" s="57"/>
       <c r="BL48" s="52"/>
       <c r="BM48" s="35"/>
       <c r="BN48" s="52"/>
       <c r="BO48" s="1"/>
       <c r="BP48" s="1"/>
-      <c r="BQ48" s="8"/>
-      <c r="BR48" s="1"/>
+      <c r="BQ48" s="1"/>
+      <c r="BR48" s="8"/>
       <c r="BS48" s="1"/>
       <c r="BT48" s="1"/>
       <c r="BU48" s="1"/>
@@ -5111,13 +5117,13 @@
     </row>
     <row r="49" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="22"/>
-      <c r="B49" s="78" t="s">
+      <c r="B49" s="72" t="s">
         <v>50</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D49" s="79"/>
+      <c r="D49" s="73"/>
       <c r="E49" s="50"/>
       <c r="F49" s="50"/>
       <c r="G49" s="50"/>
@@ -5139,7 +5145,7 @@
       <c r="W49" s="50"/>
       <c r="X49" s="50"/>
       <c r="Y49" s="50"/>
-      <c r="Z49" s="80"/>
+      <c r="Z49" s="74"/>
       <c r="AA49" s="50"/>
       <c r="AB49" s="50"/>
       <c r="AC49" s="50"/>
@@ -5173,19 +5179,19 @@
       <c r="BE49" s="50"/>
       <c r="BF49" s="50"/>
       <c r="BG49" s="50"/>
-      <c r="BH49" s="81"/>
+      <c r="BH49" s="75"/>
       <c r="BI49" s="14"/>
-      <c r="BJ49" s="62"/>
+      <c r="BJ49" s="42"/>
       <c r="BK49" s="36"/>
       <c r="BL49" s="60"/>
       <c r="BM49" s="65"/>
       <c r="BN49" s="52"/>
       <c r="BO49" s="1"/>
       <c r="BP49" s="1"/>
-      <c r="BQ49" s="8"/>
-      <c r="BR49" s="22"/>
-      <c r="BS49" s="22"/>
-      <c r="BT49" s="22"/>
+      <c r="BQ49" s="1"/>
+      <c r="BR49" s="8"/>
+      <c r="BS49" s="1"/>
+      <c r="BT49" s="1"/>
       <c r="BU49" s="22"/>
       <c r="BV49" s="22"/>
     </row>
@@ -5252,10 +5258,10 @@
       <c r="BF50" s="32"/>
       <c r="BG50" s="32"/>
       <c r="BH50" s="32"/>
-      <c r="BI50" s="92"/>
-      <c r="BJ50" s="89"/>
-      <c r="BK50" s="89"/>
-      <c r="BL50" s="89"/>
+      <c r="BI50" s="85"/>
+      <c r="BJ50" s="85"/>
+      <c r="BK50" s="82"/>
+      <c r="BL50" s="82"/>
       <c r="BM50" s="32"/>
       <c r="BN50" s="32"/>
       <c r="BO50" s="32"/>
@@ -5275,7 +5281,7 @@
       <c r="C51" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="72"/>
+      <c r="D51" s="66"/>
       <c r="E51" s="51"/>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
@@ -5304,24 +5310,24 @@
       <c r="AD51" s="51"/>
       <c r="AE51" s="51"/>
       <c r="AF51" s="51"/>
-      <c r="AG51" s="73"/>
+      <c r="AG51" s="67"/>
       <c r="AH51" s="51"/>
       <c r="AI51" s="51"/>
       <c r="AJ51" s="51"/>
       <c r="AK51" s="51"/>
       <c r="AL51" s="51"/>
       <c r="AM51" s="51"/>
-      <c r="AN51" s="76"/>
-      <c r="AO51" s="76"/>
-      <c r="AP51" s="76"/>
-      <c r="AQ51" s="76"/>
+      <c r="AN51" s="70"/>
+      <c r="AO51" s="70"/>
+      <c r="AP51" s="70"/>
+      <c r="AQ51" s="70"/>
       <c r="AR51" s="51"/>
       <c r="AS51" s="51"/>
       <c r="AT51" s="51"/>
       <c r="AU51" s="51"/>
       <c r="AV51" s="51"/>
-      <c r="AW51" s="77"/>
-      <c r="AX51" s="77"/>
+      <c r="AW51" s="71"/>
+      <c r="AX51" s="71"/>
       <c r="AY51" s="51"/>
       <c r="AZ51" s="51"/>
       <c r="BA51" s="51"/>
@@ -5333,11 +5339,11 @@
       <c r="BG51" s="51"/>
       <c r="BH51" s="51"/>
       <c r="BI51" s="14"/>
-      <c r="BJ51" s="1"/>
+      <c r="BJ51" s="14"/>
       <c r="BK51" s="56"/>
-      <c r="BL51" s="34"/>
-      <c r="BM51" s="56"/>
-      <c r="BN51" s="56"/>
+      <c r="BL51" s="52"/>
+      <c r="BM51" s="8"/>
+      <c r="BN51" s="23"/>
       <c r="BO51" s="23"/>
       <c r="BP51" s="23"/>
       <c r="BQ51" s="23"/>
@@ -5413,10 +5419,10 @@
       <c r="BG52" s="14"/>
       <c r="BH52" s="14"/>
       <c r="BI52" s="14"/>
-      <c r="BJ52" s="1"/>
+      <c r="BJ52" s="14"/>
       <c r="BK52" s="52"/>
-      <c r="BL52" s="8"/>
-      <c r="BM52" s="52"/>
+      <c r="BL52" s="52"/>
+      <c r="BM52" s="8"/>
       <c r="BN52" s="52"/>
       <c r="BO52" s="1"/>
       <c r="BP52" s="1"/>
@@ -5493,9 +5499,10 @@
       <c r="BG53" s="14"/>
       <c r="BH53" s="14"/>
       <c r="BI53" s="14"/>
-      <c r="BJ53" s="1"/>
+      <c r="BJ53" s="14"/>
       <c r="BK53" s="1"/>
-      <c r="BL53" s="8"/>
+      <c r="BL53" s="52"/>
+      <c r="BM53" s="8"/>
       <c r="BN53" s="52"/>
       <c r="BO53" s="1"/>
       <c r="BP53" s="1"/>
@@ -5571,11 +5578,11 @@
       <c r="BG54" s="14"/>
       <c r="BH54" s="14"/>
       <c r="BI54" s="14"/>
-      <c r="BJ54" s="1"/>
+      <c r="BJ54" s="14"/>
       <c r="BK54" s="1"/>
       <c r="BL54" s="52"/>
-      <c r="BM54" s="8"/>
-      <c r="BN54" s="1"/>
+      <c r="BM54" s="52"/>
+      <c r="BN54" s="8"/>
       <c r="BO54" s="1"/>
       <c r="BP54" s="1"/>
       <c r="BQ54" s="1"/>
@@ -5651,11 +5658,11 @@
       <c r="BG55" s="14"/>
       <c r="BH55" s="14"/>
       <c r="BI55" s="14"/>
-      <c r="BJ55" s="52"/>
+      <c r="BJ55" s="14"/>
       <c r="BK55" s="52"/>
       <c r="BL55" s="52"/>
-      <c r="BM55" s="8"/>
-      <c r="BN55" s="1"/>
+      <c r="BM55" s="52"/>
+      <c r="BN55" s="8"/>
       <c r="BO55" s="1"/>
       <c r="BP55" s="1"/>
       <c r="BQ55" s="1"/>
@@ -5713,7 +5720,7 @@
     <mergeCell ref="AT1:AZ1"/>
     <mergeCell ref="BA1:BG1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version 1.3 (toutes les réservations sont ok mais pas de paypal)
</commit_message>
<xml_diff>
--- a/ALM/Planning.xlsx
+++ b/ALM/Planning.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1126,23 +1126,23 @@
   </sheetPr>
   <dimension ref="A1:BV61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BM51" sqref="BM51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AM1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BT2" sqref="BT2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelRow="2" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.1796875" customWidth="1"/>
-    <col min="2" max="2" width="37.08984375" customWidth="1"/>
-    <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.36328125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="62" width="3.36328125" style="17" bestFit="1" customWidth="1"/>
-    <col min="63" max="66" width="3.36328125" style="54" bestFit="1" customWidth="1"/>
-    <col min="67" max="74" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="62" width="3.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="63" max="66" width="3.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="67" max="74" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:74" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D1" s="101" t="s">
         <v>21</v>
       </c>
@@ -1234,7 +1234,7 @@
       <c r="BT1" s="100"/>
       <c r="BU1" s="100"/>
     </row>
-    <row r="2" spans="1:74" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:74" s="3" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="11">
         <v>43395</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>43465</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="31" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:74" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>41</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="BU3" s="32"/>
       <c r="BV3" s="32"/>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>46</v>
@@ -1607,7 +1607,7 @@
       <c r="BU4" s="1"/>
       <c r="BV4" s="1"/>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -1687,7 +1687,7 @@
       <c r="BU5" s="1"/>
       <c r="BV5" s="1"/>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>31</v>
@@ -1767,7 +1767,7 @@
       <c r="BU6" s="1"/>
       <c r="BV6" s="1"/>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>47</v>
@@ -1847,7 +1847,7 @@
       <c r="BU7" s="1"/>
       <c r="BV7" s="1"/>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>64</v>
@@ -1927,7 +1927,7 @@
       <c r="BU8" s="1"/>
       <c r="BV8" s="1"/>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>63</v>
@@ -2007,7 +2007,7 @@
       <c r="BU9" s="1"/>
       <c r="BV9" s="1"/>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>66</v>
@@ -2087,7 +2087,7 @@
       <c r="BU10" s="1"/>
       <c r="BV10" s="1"/>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>65</v>
@@ -2167,7 +2167,7 @@
       <c r="BU11" s="1"/>
       <c r="BV11" s="1"/>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>33</v>
@@ -2247,7 +2247,7 @@
       <c r="BU12" s="1"/>
       <c r="BV12" s="1"/>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>45</v>
@@ -2327,7 +2327,7 @@
       <c r="BU13" s="1"/>
       <c r="BV13" s="1"/>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>67</v>
@@ -2405,7 +2405,7 @@
       <c r="BU14" s="1"/>
       <c r="BV14" s="1"/>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>62</v>
@@ -2485,7 +2485,7 @@
       <c r="BU15" s="1"/>
       <c r="BV15" s="1"/>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>42</v>
@@ -2565,7 +2565,7 @@
       <c r="BU16" s="1"/>
       <c r="BV16" s="1"/>
     </row>
-    <row r="17" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>44</v>
@@ -2645,7 +2645,7 @@
       <c r="BU17" s="1"/>
       <c r="BV17" s="1"/>
     </row>
-    <row r="18" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A18" s="77"/>
       <c r="B18" s="1" t="s">
         <v>68</v>
@@ -2725,7 +2725,7 @@
       <c r="BU18" s="1"/>
       <c r="BV18" s="1"/>
     </row>
-    <row r="19" spans="1:74" s="31" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:74" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>14</v>
       </c>
@@ -2803,7 +2803,7 @@
       <c r="BU19" s="32"/>
       <c r="BV19" s="32"/>
     </row>
-    <row r="20" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="23" t="s">
         <v>13</v>
@@ -2880,7 +2880,7 @@
       <c r="BU20" s="23"/>
       <c r="BV20" s="23"/>
     </row>
-    <row r="21" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="19" t="s">
         <v>0</v>
@@ -2960,7 +2960,7 @@
       <c r="BU21" s="1"/>
       <c r="BV21" s="1"/>
     </row>
-    <row r="22" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="19" t="s">
         <v>1</v>
@@ -3040,7 +3040,7 @@
       <c r="BU22" s="1"/>
       <c r="BV22" s="1"/>
     </row>
-    <row r="23" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="19" t="s">
         <v>37</v>
@@ -3120,7 +3120,7 @@
       <c r="BU23" s="1"/>
       <c r="BV23" s="1"/>
     </row>
-    <row r="24" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="19" t="s">
         <v>2</v>
@@ -3200,7 +3200,7 @@
       <c r="BU24" s="1"/>
       <c r="BV24" s="1"/>
     </row>
-    <row r="25" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="19" t="s">
         <v>3</v>
@@ -3280,7 +3280,7 @@
       <c r="BU25" s="1"/>
       <c r="BV25" s="1"/>
     </row>
-    <row r="26" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:74" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="19" t="s">
         <v>49</v>
@@ -3360,7 +3360,7 @@
       <c r="BU26" s="1"/>
       <c r="BV26" s="1"/>
     </row>
-    <row r="27" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>12</v>
@@ -3440,7 +3440,7 @@
       <c r="BU27" s="1"/>
       <c r="BV27" s="1"/>
     </row>
-    <row r="28" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>11</v>
@@ -3519,7 +3519,7 @@
       <c r="BU28" s="1"/>
       <c r="BV28" s="1"/>
     </row>
-    <row r="29" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>9</v>
@@ -3598,7 +3598,7 @@
       <c r="BU29" s="1"/>
       <c r="BV29" s="1"/>
     </row>
-    <row r="30" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>10</v>
@@ -3678,7 +3678,7 @@
       <c r="BU30" s="1"/>
       <c r="BV30" s="1"/>
     </row>
-    <row r="31" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>36</v>
@@ -3758,7 +3758,7 @@
       <c r="BU31" s="1"/>
       <c r="BV31" s="1"/>
     </row>
-    <row r="32" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>7</v>
@@ -3838,7 +3838,7 @@
       <c r="BU32" s="1"/>
       <c r="BV32" s="1"/>
     </row>
-    <row r="33" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="19" t="s">
         <v>56</v>
@@ -3917,7 +3917,7 @@
       <c r="BU33" s="1"/>
       <c r="BV33" s="1"/>
     </row>
-    <row r="34" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:74" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="19" t="s">
         <v>58</v>
@@ -3996,7 +3996,7 @@
       <c r="BU34" s="22"/>
       <c r="BV34" s="1"/>
     </row>
-    <row r="35" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>8</v>
@@ -4076,7 +4076,7 @@
       <c r="BU35" s="93"/>
       <c r="BV35" s="21"/>
     </row>
-    <row r="36" spans="1:74" ht="15" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:74" ht="15.75" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="19" t="s">
         <v>57</v>
@@ -4156,7 +4156,7 @@
       <c r="BU36" s="94"/>
       <c r="BV36" s="21"/>
     </row>
-    <row r="37" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>6</v>
@@ -4236,7 +4236,7 @@
       <c r="BU37" s="34"/>
       <c r="BV37" s="26"/>
     </row>
-    <row r="38" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="38" t="s">
         <v>5</v>
@@ -4315,7 +4315,7 @@
       <c r="BU38" s="92"/>
       <c r="BV38" s="4"/>
     </row>
-    <row r="39" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="39" t="s">
         <v>61</v>
@@ -4395,7 +4395,7 @@
       <c r="BU39" s="4"/>
       <c r="BV39" s="4"/>
     </row>
-    <row r="40" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="39" t="s">
         <v>59</v>
@@ -4475,7 +4475,7 @@
       <c r="BU40" s="4"/>
       <c r="BV40" s="4"/>
     </row>
-    <row r="41" spans="1:74" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:74" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="39" t="s">
         <v>60</v>
@@ -4555,7 +4555,7 @@
       <c r="BU41" s="4"/>
       <c r="BV41" s="4"/>
     </row>
-    <row r="42" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>4</v>
@@ -4635,7 +4635,7 @@
       <c r="BU42" s="23"/>
       <c r="BV42" s="23"/>
     </row>
-    <row r="43" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="19" t="s">
         <v>52</v>
@@ -4715,7 +4715,7 @@
       <c r="BU43" s="1"/>
       <c r="BV43" s="1"/>
     </row>
-    <row r="44" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="19" t="s">
         <v>51</v>
@@ -4795,7 +4795,7 @@
       <c r="BU44" s="1"/>
       <c r="BV44" s="1"/>
     </row>
-    <row r="45" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="19" t="s">
         <v>53</v>
@@ -4875,7 +4875,7 @@
       <c r="BU45" s="1"/>
       <c r="BV45" s="1"/>
     </row>
-    <row r="46" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="19" t="s">
         <v>54</v>
@@ -4955,7 +4955,7 @@
       <c r="BU46" s="1"/>
       <c r="BV46" s="1"/>
     </row>
-    <row r="47" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="19" t="s">
         <v>55</v>
@@ -5035,7 +5035,7 @@
       <c r="BU47" s="1"/>
       <c r="BV47" s="1"/>
     </row>
-    <row r="48" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:74" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="19" t="s">
         <v>69</v>
@@ -5115,7 +5115,7 @@
       <c r="BU48" s="1"/>
       <c r="BV48" s="1"/>
     </row>
-    <row r="49" spans="1:74" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="22"/>
       <c r="B49" s="72" t="s">
         <v>50</v>
@@ -5195,7 +5195,7 @@
       <c r="BU49" s="22"/>
       <c r="BV49" s="22"/>
     </row>
-    <row r="50" spans="1:74" s="31" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:74" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>15</v>
       </c>
@@ -5273,7 +5273,7 @@
       <c r="BU50" s="32"/>
       <c r="BV50" s="32"/>
     </row>
-    <row r="51" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="23" t="s">
         <v>19</v>
@@ -5353,7 +5353,7 @@
       <c r="BU51" s="23"/>
       <c r="BV51" s="23"/>
     </row>
-    <row r="52" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
         <v>20</v>
@@ -5433,7 +5433,7 @@
       <c r="BU52" s="1"/>
       <c r="BV52" s="1"/>
     </row>
-    <row r="53" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
         <v>18</v>
@@ -5513,7 +5513,7 @@
       <c r="BU53" s="1"/>
       <c r="BV53" s="1"/>
     </row>
-    <row r="54" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
         <v>17</v>
@@ -5592,7 +5592,7 @@
       <c r="BU54" s="1"/>
       <c r="BV54" s="1"/>
     </row>
-    <row r="55" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
         <v>16</v>
@@ -5672,7 +5672,7 @@
       <c r="BU55" s="1"/>
       <c r="BV55" s="1"/>
     </row>
-    <row r="58" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>34</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>40</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>35</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:74" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>43</v>
       </c>
@@ -5721,6 +5721,6 @@
     <mergeCell ref="BA1:BG1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>